<commit_message>
Add 3.5mm terminal blocks
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12177" uniqueCount="4506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12189" uniqueCount="4512">
   <si>
     <t>Part Number</t>
   </si>
@@ -13549,6 +13549,24 @@
   </si>
   <si>
     <t>SW-SPDT</t>
+  </si>
+  <si>
+    <t>CONN-00022</t>
+  </si>
+  <si>
+    <t>CONN-00023</t>
+  </si>
+  <si>
+    <t>Term Blk, 3 Pos, 16A, 3.5mm Pitch</t>
+  </si>
+  <si>
+    <t>Term Blk, 2 Pos, 16A, 3.5mm Pitch</t>
+  </si>
+  <si>
+    <t>TERM_3.50MM_2x1_0</t>
+  </si>
+  <si>
+    <t>TERM_3.50MM_3x1_0</t>
   </si>
 </sst>
 </file>
@@ -34303,10 +34321,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34939,6 +34957,70 @@
       </c>
       <c r="J23" t="s">
         <v>2386</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>4506</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4508</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2385</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
+        <v>2383</v>
+      </c>
+      <c r="H24">
+        <v>1861946</v>
+      </c>
+      <c r="I24" t="s">
+        <v>4511</v>
+      </c>
+      <c r="J24" t="s">
+        <v>2386</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>4507</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4509</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2385</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>16</v>
+      </c>
+      <c r="G25" t="s">
+        <v>2383</v>
+      </c>
+      <c r="H25">
+        <v>1861933</v>
+      </c>
+      <c r="I25" t="s">
+        <v>4510</v>
+      </c>
+      <c r="J25" t="s">
+        <v>2393</v>
       </c>
     </row>
   </sheetData>
@@ -57160,8 +57242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add new components etc
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12189" uniqueCount="4512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12215" uniqueCount="4523">
   <si>
     <t>Part Number</t>
   </si>
@@ -13567,6 +13567,39 @@
   </si>
   <si>
     <t>TERM_3.50MM_3x1_0</t>
+  </si>
+  <si>
+    <t>ANLG-00017</t>
+  </si>
+  <si>
+    <t>TLV272CDGKR</t>
+  </si>
+  <si>
+    <t>VSSOP-8_0</t>
+  </si>
+  <si>
+    <t>Op Amp, Dual, Rail-Rail, 3MHZ, 8-VSSOP</t>
+  </si>
+  <si>
+    <t>TLV272DGK</t>
+  </si>
+  <si>
+    <t>CAP-00534</t>
+  </si>
+  <si>
+    <t>GRJ188R72A104KE11D</t>
+  </si>
+  <si>
+    <t>XSTR-00018</t>
+  </si>
+  <si>
+    <t>61A</t>
+  </si>
+  <si>
+    <t>118W</t>
+  </si>
+  <si>
+    <t>NVD5117PLT4G-VF01</t>
   </si>
 </sst>
 </file>
@@ -32199,10 +32232,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32873,6 +32906,41 @@
       </c>
       <c r="K19" t="s">
         <v>2261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>4519</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2419</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2123</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4520</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4521</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2270</v>
+      </c>
+      <c r="G20" t="s">
+        <v>2178</v>
+      </c>
+      <c r="H20" t="s">
+        <v>2094</v>
+      </c>
+      <c r="I20" t="s">
+        <v>4522</v>
+      </c>
+      <c r="J20" t="s">
+        <v>2416</v>
+      </c>
+      <c r="K20" t="s">
+        <v>2276</v>
       </c>
     </row>
   </sheetData>
@@ -34323,8 +34391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35031,10 +35099,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J535"/>
+  <dimension ref="A1:J536"/>
   <sheetViews>
-    <sheetView topLeftCell="A512" workbookViewId="0">
-      <selection activeCell="K524" sqref="K524"/>
+    <sheetView topLeftCell="A518" workbookViewId="0">
+      <selection activeCell="B537" sqref="B537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51621,7 +51689,7 @@
         <v>4459</v>
       </c>
       <c r="B503" t="str">
-        <f t="shared" ref="B503:B535" si="9">CONCATENATE("CAP",", ",C503,", ",D503,", ",E503,", ",F503,", 0603")</f>
+        <f t="shared" ref="B503:B536" si="9">CONCATENATE("CAP",", ",C503,", ",D503,", ",E503,", ",F503,", 0603")</f>
         <v>CAP, 470pF, ±10%, 100V, X7R, 0603</v>
       </c>
       <c r="C503" t="s">
@@ -52702,6 +52770,39 @@
         <v>35</v>
       </c>
       <c r="J535" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="536" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A536" t="s">
+        <v>4517</v>
+      </c>
+      <c r="B536" t="str">
+        <f t="shared" si="9"/>
+        <v>CAP, 0.1µF, ±10%, 100V, X7R, 0603</v>
+      </c>
+      <c r="C536" t="s">
+        <v>4362</v>
+      </c>
+      <c r="D536" t="s">
+        <v>4359</v>
+      </c>
+      <c r="E536" t="s">
+        <v>947</v>
+      </c>
+      <c r="F536" t="s">
+        <v>20</v>
+      </c>
+      <c r="G536" t="s">
+        <v>21</v>
+      </c>
+      <c r="H536" t="s">
+        <v>4518</v>
+      </c>
+      <c r="I536" t="s">
+        <v>35</v>
+      </c>
+      <c r="J536" t="s">
         <v>23</v>
       </c>
     </row>
@@ -56857,10 +56958,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57233,8 +57334,29 @@
         <v>4263</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>4512</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4515</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2290</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4513</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4514</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4516</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add TS3A5017 mux/demux and LM317 linear regulator and 4-pin D2PAK
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12244" uniqueCount="4531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12265" uniqueCount="4548">
   <si>
     <t>Part Number</t>
   </si>
@@ -13624,6 +13624,57 @@
   </si>
   <si>
     <t>54mW</t>
+  </si>
+  <si>
+    <t>UCTRL-00006</t>
+  </si>
+  <si>
+    <t>Teensy 3.6, 32-bit ARM</t>
+  </si>
+  <si>
+    <t>TEENSY_3_6</t>
+  </si>
+  <si>
+    <t>Teensy3-6</t>
+  </si>
+  <si>
+    <t>LOGIC-00011</t>
+  </si>
+  <si>
+    <t>Mux/Demux, 2x4:1, TSSOP-16, TS3A5017PWR</t>
+  </si>
+  <si>
+    <t>TS3A5017PWR</t>
+  </si>
+  <si>
+    <t>TSSOP-16_0</t>
+  </si>
+  <si>
+    <t>TS3A5017</t>
+  </si>
+  <si>
+    <t>PWREG-00014</t>
+  </si>
+  <si>
+    <t>REG, Linear, Adj, 1.5A</t>
+  </si>
+  <si>
+    <t>1.25 - 37V</t>
+  </si>
+  <si>
+    <t>Adf</t>
+  </si>
+  <si>
+    <t>LM317KTTR</t>
+  </si>
+  <si>
+    <t>D2PAK-4_0</t>
+  </si>
+  <si>
+    <t>LM317</t>
+  </si>
+  <si>
+    <t>4.25 - 40V</t>
   </si>
 </sst>
 </file>
@@ -32005,10 +32056,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32276,6 +32327,38 @@
         <v>4349</v>
       </c>
       <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4535</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4536</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2290</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4537</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4538</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4539</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G16" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -33032,7 +33115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -56167,10 +56250,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -56321,6 +56404,20 @@
       </c>
       <c r="F7" t="s">
         <v>4493</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4531</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4532</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4533</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4534</v>
       </c>
     </row>
   </sheetData>
@@ -56552,10 +56649,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57062,6 +57159,44 @@
       </c>
       <c r="M15" s="10">
         <v>11.15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>4540</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4541</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4547</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4542</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2335</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2564</v>
+      </c>
+      <c r="H16" t="s">
+        <v>4543</v>
+      </c>
+      <c r="I16" t="s">
+        <v>2290</v>
+      </c>
+      <c r="J16" t="s">
+        <v>4544</v>
+      </c>
+      <c r="K16" t="s">
+        <v>4545</v>
+      </c>
+      <c r="L16" t="s">
+        <v>4546</v>
+      </c>
+      <c r="M16" s="10">
+        <v>0.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 4 position terminal block, add 3D models for our 3.5mm pitch terminal blocks
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12265" uniqueCount="4548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12279" uniqueCount="4555">
   <si>
     <t>Part Number</t>
   </si>
@@ -13675,6 +13675,27 @@
   </si>
   <si>
     <t>4.25 - 40V</t>
+  </si>
+  <si>
+    <t>ANLG-00018</t>
+  </si>
+  <si>
+    <t>DAC, 16-bit, Voltage output, SPI, 8-VSSOP</t>
+  </si>
+  <si>
+    <t>DAC8551</t>
+  </si>
+  <si>
+    <t>DAC8551IDGKR</t>
+  </si>
+  <si>
+    <t>CONN-00024</t>
+  </si>
+  <si>
+    <t>Term Blk, 4 Pos, 16A, 3.5mm Pitch</t>
+  </si>
+  <si>
+    <t>TERM_3.50MM_4x1_0</t>
   </si>
 </sst>
 </file>
@@ -13748,12 +13769,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -14037,8 +14058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J839"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="A285" workbookViewId="0">
+      <selection activeCell="J309" sqref="J309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14052,6 +14073,7 @@
     <col min="7" max="7" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -14061,7 +14083,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>924</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -14081,6 +14103,9 @@
       </c>
       <c r="I1" t="s">
         <v>7</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>4523</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -14111,7 +14136,7 @@
       <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="7"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -22871,7 +22896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>586</v>
       </c>
@@ -22900,7 +22925,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>587</v>
       </c>
@@ -22929,7 +22954,7 @@
         <v>2346</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>588</v>
       </c>
@@ -22958,7 +22983,7 @@
         <v>2346</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>589</v>
       </c>
@@ -22986,8 +23011,11 @@
       <c r="I308" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J308" s="9">
+        <v>0.14399999999999999</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>590</v>
       </c>
@@ -23016,7 +23044,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>591</v>
       </c>
@@ -23045,7 +23073,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>592</v>
       </c>
@@ -23074,7 +23102,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>593</v>
       </c>
@@ -23103,7 +23131,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>594</v>
       </c>
@@ -23132,7 +23160,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>595</v>
       </c>
@@ -23161,7 +23189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>596</v>
       </c>
@@ -23190,7 +23218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>597</v>
       </c>
@@ -23219,7 +23247,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>598</v>
       </c>
@@ -23248,7 +23276,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>599</v>
       </c>
@@ -23277,7 +23305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>600</v>
       </c>
@@ -23306,7 +23334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>601</v>
       </c>
@@ -32114,7 +32142,7 @@
       <c r="F2" t="s">
         <v>2567</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -32135,7 +32163,7 @@
       <c r="F3" t="s">
         <v>2570</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -32156,7 +32184,7 @@
       <c r="F4" t="s">
         <v>2573</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -32177,7 +32205,7 @@
       <c r="F5" t="s">
         <v>2582</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -32198,7 +32226,7 @@
       <c r="F6" t="s">
         <v>4329</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -32219,7 +32247,7 @@
       <c r="F7" t="s">
         <v>4316</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -32240,7 +32268,7 @@
       <c r="F8" t="s">
         <v>4316</v>
       </c>
-      <c r="G8" s="10"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -32261,7 +32289,7 @@
       <c r="F9" t="s">
         <v>4315</v>
       </c>
-      <c r="G9" s="10"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -32282,7 +32310,7 @@
       <c r="F10" t="s">
         <v>4315</v>
       </c>
-      <c r="G10" s="10"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -32303,7 +32331,7 @@
       <c r="F11" t="s">
         <v>4349</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>0.45</v>
       </c>
     </row>
@@ -32326,7 +32354,7 @@
       <c r="F12" t="s">
         <v>4349</v>
       </c>
-      <c r="G12" s="10"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -32347,18 +32375,18 @@
       <c r="F13" t="s">
         <v>4539</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="9">
         <v>0.84</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G14" s="10"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G15" s="10"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G16" s="10"/>
+      <c r="G16" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32371,7 +32399,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32460,7 +32488,7 @@
       <c r="K2" t="s">
         <v>2238</v>
       </c>
-      <c r="L2" s="10"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -32496,7 +32524,7 @@
       <c r="K3" t="s">
         <v>2238</v>
       </c>
-      <c r="L3" s="10"/>
+      <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -32532,7 +32560,7 @@
       <c r="K4" t="s">
         <v>2246</v>
       </c>
-      <c r="L4" s="10"/>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -32568,7 +32596,7 @@
       <c r="K5" t="s">
         <v>2246</v>
       </c>
-      <c r="L5" s="10"/>
+      <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -32604,7 +32632,7 @@
       <c r="K6" t="s">
         <v>2261</v>
       </c>
-      <c r="L6" s="10"/>
+      <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -32640,7 +32668,7 @@
       <c r="K7" t="s">
         <v>2276</v>
       </c>
-      <c r="L7" s="10"/>
+      <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -32676,7 +32704,7 @@
       <c r="K8" t="s">
         <v>2261</v>
       </c>
-      <c r="L8" s="10"/>
+      <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -32712,7 +32740,7 @@
       <c r="K9" t="s">
         <v>2297</v>
       </c>
-      <c r="L9" s="10"/>
+      <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -32748,7 +32776,7 @@
       <c r="K10" t="s">
         <v>2297</v>
       </c>
-      <c r="L10" s="10"/>
+      <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -32784,7 +32812,7 @@
       <c r="K11" t="s">
         <v>2276</v>
       </c>
-      <c r="L11" s="10"/>
+      <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -32820,7 +32848,7 @@
       <c r="K12" t="s">
         <v>2276</v>
       </c>
-      <c r="L12" s="10"/>
+      <c r="L12" s="9"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -32856,7 +32884,7 @@
       <c r="K13" t="s">
         <v>2261</v>
       </c>
-      <c r="L13" s="10"/>
+      <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -32883,7 +32911,7 @@
       <c r="K14" t="s">
         <v>2491</v>
       </c>
-      <c r="L14" s="10"/>
+      <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -32919,7 +32947,7 @@
       <c r="K15" t="s">
         <v>2549</v>
       </c>
-      <c r="L15" s="10"/>
+      <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -32955,7 +32983,7 @@
       <c r="K16" t="s">
         <v>2600</v>
       </c>
-      <c r="L16" s="10"/>
+      <c r="L16" s="9"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -32991,7 +33019,7 @@
       <c r="K17" t="s">
         <v>2261</v>
       </c>
-      <c r="L17" s="10"/>
+      <c r="L17" s="9"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -33027,7 +33055,7 @@
       <c r="K18" t="s">
         <v>2238</v>
       </c>
-      <c r="L18" s="10"/>
+      <c r="L18" s="9"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -33063,7 +33091,7 @@
       <c r="K19" t="s">
         <v>2261</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="9">
         <v>0.31</v>
       </c>
     </row>
@@ -33101,7 +33129,7 @@
       <c r="K20" t="s">
         <v>2276</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="9">
         <v>2.5299999999999998</v>
       </c>
     </row>
@@ -33115,8 +33143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33208,7 +33236,7 @@
       <c r="L2" s="2" t="s">
         <v>2100</v>
       </c>
-      <c r="M2" s="10"/>
+      <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -33241,7 +33269,7 @@
       <c r="L3" s="2" t="s">
         <v>2100</v>
       </c>
-      <c r="M3" s="10"/>
+      <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -33274,7 +33302,7 @@
       <c r="L4" s="2" t="s">
         <v>2100</v>
       </c>
-      <c r="M4" s="10"/>
+      <c r="M4" s="9"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -33307,7 +33335,7 @@
       <c r="L5" s="2" t="s">
         <v>2100</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -33340,7 +33368,7 @@
       <c r="L6" s="2" t="s">
         <v>2100</v>
       </c>
-      <c r="M6" s="10"/>
+      <c r="M6" s="9"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -33373,7 +33401,7 @@
       <c r="L7" s="2" t="s">
         <v>2100</v>
       </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -33409,7 +33437,7 @@
       <c r="L8" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M8" s="10"/>
+      <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -33445,7 +33473,7 @@
       <c r="L9" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M9" s="10"/>
+      <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -33481,7 +33509,7 @@
       <c r="L10" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M10" s="10"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -33517,7 +33545,7 @@
       <c r="L11" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M11" s="10"/>
+      <c r="M11" s="9"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -33553,7 +33581,7 @@
       <c r="L12" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M12" s="10"/>
+      <c r="M12" s="9"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -33589,7 +33617,7 @@
       <c r="L13" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M13" s="10"/>
+      <c r="M13" s="9"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -33625,7 +33653,7 @@
       <c r="L14" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M14" s="10"/>
+      <c r="M14" s="9"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -33661,7 +33689,7 @@
       <c r="L15" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M15" s="10"/>
+      <c r="M15" s="9"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -33697,7 +33725,7 @@
       <c r="L16" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M16" s="10"/>
+      <c r="M16" s="9"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -33733,7 +33761,7 @@
       <c r="L17" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M17" s="10"/>
+      <c r="M17" s="9"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -33769,7 +33797,7 @@
       <c r="L18" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M18" s="10"/>
+      <c r="M18" s="9"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
@@ -33805,7 +33833,7 @@
       <c r="L19" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M19" s="10"/>
+      <c r="M19" s="9"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -33841,7 +33869,7 @@
       <c r="L20" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M20" s="10"/>
+      <c r="M20" s="9"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
@@ -33877,7 +33905,7 @@
       <c r="L21" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M21" s="10"/>
+      <c r="M21" s="9"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
@@ -33913,7 +33941,7 @@
       <c r="L22" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M22" s="10"/>
+      <c r="M22" s="9"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
@@ -33949,7 +33977,7 @@
       <c r="L23" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M23" s="10"/>
+      <c r="M23" s="9"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
@@ -33985,7 +34013,7 @@
       <c r="L24" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M24" s="10"/>
+      <c r="M24" s="9"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -34021,7 +34049,7 @@
       <c r="L25" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M25" s="10"/>
+      <c r="M25" s="9"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -34057,7 +34085,7 @@
       <c r="L26" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M26" s="10"/>
+      <c r="M26" s="9"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -34093,7 +34121,7 @@
       <c r="L27" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M27" s="10"/>
+      <c r="M27" s="9"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
@@ -34129,7 +34157,7 @@
       <c r="L28" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M28" s="10"/>
+      <c r="M28" s="9"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -34165,7 +34193,7 @@
       <c r="L29" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M29" s="10"/>
+      <c r="M29" s="9"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
@@ -34201,7 +34229,7 @@
       <c r="L30" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M30" s="10"/>
+      <c r="M30" s="9"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
@@ -34237,7 +34265,7 @@
       <c r="L31" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M31" s="10"/>
+      <c r="M31" s="9"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -34273,7 +34301,7 @@
       <c r="L32" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M32" s="10"/>
+      <c r="M32" s="9"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
@@ -34309,7 +34337,7 @@
       <c r="L33" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M33" s="10"/>
+      <c r="M33" s="9"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
@@ -34339,7 +34367,7 @@
       <c r="L34" s="2" t="s">
         <v>2403</v>
       </c>
-      <c r="M34" s="10"/>
+      <c r="M34" s="9"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
@@ -34369,7 +34397,7 @@
       <c r="L35" s="2" t="s">
         <v>2504</v>
       </c>
-      <c r="M35" s="10"/>
+      <c r="M35" s="9"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
@@ -34399,7 +34427,7 @@
       <c r="L36" s="2" t="s">
         <v>2505</v>
       </c>
-      <c r="M36" s="10"/>
+      <c r="M36" s="9"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
@@ -34429,7 +34457,7 @@
       <c r="L37" s="2" t="s">
         <v>2505</v>
       </c>
-      <c r="M37" s="10"/>
+      <c r="M37" s="9"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
@@ -34459,7 +34487,7 @@
       <c r="L38" s="2" t="s">
         <v>2949</v>
       </c>
-      <c r="M38" s="10"/>
+      <c r="M38" s="9"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
@@ -34489,7 +34517,7 @@
       <c r="L39" s="2" t="s">
         <v>2949</v>
       </c>
-      <c r="M39" s="10"/>
+      <c r="M39" s="9"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
@@ -34525,7 +34553,7 @@
       <c r="L40" s="2" t="s">
         <v>2982</v>
       </c>
-      <c r="M40" s="10">
+      <c r="M40" s="9">
         <v>0.19</v>
       </c>
     </row>
@@ -34560,7 +34588,7 @@
       <c r="L41" s="2" t="s">
         <v>4286</v>
       </c>
-      <c r="M41" s="10"/>
+      <c r="M41" s="9"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
@@ -34596,7 +34624,7 @@
       <c r="L42" s="2" t="s">
         <v>2505</v>
       </c>
-      <c r="M42" s="10">
+      <c r="M42" s="9">
         <v>0.34</v>
       </c>
     </row>
@@ -34608,16 +34636,16 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
     <col min="3" max="4" width="14.5546875" customWidth="1"/>
     <col min="5" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
@@ -34693,7 +34721,7 @@
       <c r="J2" t="s">
         <v>2386</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="9">
         <v>1.19</v>
       </c>
     </row>
@@ -34728,7 +34756,7 @@
       <c r="J3" t="s">
         <v>2393</v>
       </c>
-      <c r="K3" s="10"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -34752,7 +34780,7 @@
       <c r="J4" t="s">
         <v>2400</v>
       </c>
-      <c r="K4" s="10"/>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -34773,7 +34801,7 @@
       <c r="J5" t="s">
         <v>2449</v>
       </c>
-      <c r="K5" s="10"/>
+      <c r="K5" s="9"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -34794,7 +34822,7 @@
       <c r="J6" t="s">
         <v>2456</v>
       </c>
-      <c r="K6" s="10"/>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -34815,7 +34843,7 @@
       <c r="J7" t="s">
         <v>2457</v>
       </c>
-      <c r="K7" s="10"/>
+      <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -34848,7 +34876,7 @@
       <c r="J8" t="s">
         <v>2386</v>
       </c>
-      <c r="K8" s="10"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -34872,7 +34900,7 @@
       <c r="J9" t="s">
         <v>2515</v>
       </c>
-      <c r="K9" s="10"/>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -34893,7 +34921,7 @@
       <c r="J10" t="s">
         <v>2577</v>
       </c>
-      <c r="K10" s="10"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -34926,7 +34954,7 @@
       <c r="J11" t="s">
         <v>2386</v>
       </c>
-      <c r="K11" s="10"/>
+      <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -34959,7 +34987,7 @@
       <c r="J12" t="s">
         <v>2393</v>
       </c>
-      <c r="K12" s="10"/>
+      <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -34992,7 +35020,7 @@
       <c r="J13" t="s">
         <v>2910</v>
       </c>
-      <c r="K13" s="10"/>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -35016,7 +35044,7 @@
       <c r="J14" t="s">
         <v>2965</v>
       </c>
-      <c r="K14" s="10"/>
+      <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -35040,7 +35068,7 @@
       <c r="J15" t="s">
         <v>2972</v>
       </c>
-      <c r="K15" s="10"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -35073,7 +35101,7 @@
       <c r="J16" t="s">
         <v>2393</v>
       </c>
-      <c r="K16" s="10"/>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -35094,7 +35122,7 @@
       <c r="G17" t="s">
         <v>3378</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="7">
         <v>605240</v>
       </c>
       <c r="I17" t="s">
@@ -35103,7 +35131,7 @@
       <c r="J17" t="s">
         <v>3380</v>
       </c>
-      <c r="K17" s="10"/>
+      <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -35130,7 +35158,7 @@
       <c r="J18" t="s">
         <v>4260</v>
       </c>
-      <c r="K18" s="10"/>
+      <c r="K18" s="9"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -35157,7 +35185,7 @@
       <c r="J19" t="s">
         <v>2577</v>
       </c>
-      <c r="K19" s="10"/>
+      <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -35184,7 +35212,7 @@
       <c r="J20" t="s">
         <v>4259</v>
       </c>
-      <c r="K20" s="10"/>
+      <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -35208,7 +35236,7 @@
       <c r="J21" t="s">
         <v>4271</v>
       </c>
-      <c r="K21" s="10"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -35238,7 +35266,7 @@
       <c r="J22" t="s">
         <v>4303</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="9">
         <v>4.45</v>
       </c>
     </row>
@@ -35273,7 +35301,7 @@
       <c r="J23" t="s">
         <v>2386</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K23" s="9">
         <v>0.79</v>
       </c>
     </row>
@@ -35308,7 +35336,7 @@
       <c r="J24" t="s">
         <v>2386</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="9">
         <v>1.19</v>
       </c>
     </row>
@@ -35343,8 +35371,43 @@
       <c r="J25" t="s">
         <v>2393</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="9">
         <v>0.79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>4552</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4553</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2385</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>16</v>
+      </c>
+      <c r="G26" t="s">
+        <v>2383</v>
+      </c>
+      <c r="H26">
+        <v>1861959</v>
+      </c>
+      <c r="I26" t="s">
+        <v>4554</v>
+      </c>
+      <c r="J26" t="s">
+        <v>2965</v>
+      </c>
+      <c r="K26" s="9">
+        <v>1.67</v>
       </c>
     </row>
   </sheetData>
@@ -35357,8 +35420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K537"/>
   <sheetViews>
-    <sheetView topLeftCell="A508" workbookViewId="0">
-      <selection activeCell="K536" sqref="K536"/>
+    <sheetView topLeftCell="A516" workbookViewId="0">
+      <selection activeCell="J539" sqref="J539"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35373,6 +35436,7 @@
     <col min="8" max="8" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -35406,7 +35470,7 @@
       <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="9" t="s">
         <v>4523</v>
       </c>
     </row>
@@ -53064,6 +53128,9 @@
       <c r="J536" t="s">
         <v>23</v>
       </c>
+      <c r="K536" s="9">
+        <v>0.187</v>
+      </c>
     </row>
     <row r="537" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
@@ -53097,7 +53164,7 @@
       <c r="J537" t="s">
         <v>23</v>
       </c>
-      <c r="K537" s="10">
+      <c r="K537" s="9">
         <v>0.88</v>
       </c>
     </row>
@@ -53108,10 +53175,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L95"/>
+  <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="M91" sqref="M91"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53130,7 +53197,7 @@
     <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -53167,8 +53234,11 @@
       <c r="L1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>4523</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -53193,8 +53263,11 @@
       <c r="L2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1386</v>
       </c>
@@ -53226,8 +53299,9 @@
       <c r="L3" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1387</v>
       </c>
@@ -53259,8 +53333,9 @@
       <c r="L4" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1388</v>
       </c>
@@ -53292,8 +53367,9 @@
       <c r="L5" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1389</v>
       </c>
@@ -53325,8 +53401,9 @@
       <c r="L6" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1390</v>
       </c>
@@ -53358,8 +53435,9 @@
       <c r="L7" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1391</v>
       </c>
@@ -53391,8 +53469,9 @@
       <c r="L8" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1392</v>
       </c>
@@ -53424,8 +53503,9 @@
       <c r="L9" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1393</v>
       </c>
@@ -53457,8 +53537,9 @@
       <c r="L10" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1394</v>
       </c>
@@ -53490,8 +53571,9 @@
       <c r="L11" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1395</v>
       </c>
@@ -53523,8 +53605,9 @@
       <c r="L12" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12" s="9"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1396</v>
       </c>
@@ -53556,8 +53639,9 @@
       <c r="L13" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1397</v>
       </c>
@@ -53589,8 +53673,9 @@
       <c r="L14" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1398</v>
       </c>
@@ -53622,8 +53707,9 @@
       <c r="L15" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1399</v>
       </c>
@@ -53655,8 +53741,9 @@
       <c r="L16" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1400</v>
       </c>
@@ -53688,8 +53775,9 @@
       <c r="L17" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17" s="9"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1401</v>
       </c>
@@ -53721,8 +53809,9 @@
       <c r="L18" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18" s="9"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1402</v>
       </c>
@@ -53754,8 +53843,9 @@
       <c r="L19" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19" s="9"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1403</v>
       </c>
@@ -53787,8 +53877,9 @@
       <c r="L20" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20" s="9"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1404</v>
       </c>
@@ -53820,8 +53911,9 @@
       <c r="L21" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21" s="9"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1405</v>
       </c>
@@ -53853,8 +53945,9 @@
       <c r="L22" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22" s="9"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1406</v>
       </c>
@@ -53886,8 +53979,9 @@
       <c r="L23" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23" s="9"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1407</v>
       </c>
@@ -53919,8 +54013,9 @@
       <c r="L24" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M24" s="9"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1408</v>
       </c>
@@ -53952,8 +54047,9 @@
       <c r="L25" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M25" s="9"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1409</v>
       </c>
@@ -53985,8 +54081,9 @@
       <c r="L26" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M26" s="9"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1410</v>
       </c>
@@ -54018,8 +54115,9 @@
       <c r="L27" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M27" s="9"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1411</v>
       </c>
@@ -54051,8 +54149,9 @@
       <c r="L28" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M28" s="9"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1412</v>
       </c>
@@ -54084,8 +54183,9 @@
       <c r="L29" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M29" s="9"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1413</v>
       </c>
@@ -54117,8 +54217,9 @@
       <c r="L30" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M30" s="9"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1414</v>
       </c>
@@ -54150,8 +54251,9 @@
       <c r="L31" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M31" s="9"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1415</v>
       </c>
@@ -54183,8 +54285,9 @@
       <c r="L32" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M32" s="9"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>1416</v>
       </c>
@@ -54216,8 +54319,9 @@
       <c r="L33" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M33" s="9"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1417</v>
       </c>
@@ -54249,8 +54353,9 @@
       <c r="L34" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M34" s="9"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>1418</v>
       </c>
@@ -54282,8 +54387,9 @@
       <c r="L35" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M35" s="9"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>1419</v>
       </c>
@@ -54315,8 +54421,9 @@
       <c r="L36" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M36" s="9"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>1420</v>
       </c>
@@ -54348,8 +54455,9 @@
       <c r="L37" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M37" s="9"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>1421</v>
       </c>
@@ -54381,8 +54489,9 @@
       <c r="L38" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M38" s="9"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1422</v>
       </c>
@@ -54414,8 +54523,9 @@
       <c r="L39" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M39" s="9"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>1423</v>
       </c>
@@ -54447,8 +54557,9 @@
       <c r="L40" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M40" s="9"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>1424</v>
       </c>
@@ -54480,8 +54591,9 @@
       <c r="L41" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M41" s="9"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>1425</v>
       </c>
@@ -54513,8 +54625,9 @@
       <c r="L42" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M42" s="9"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>1426</v>
       </c>
@@ -54546,8 +54659,9 @@
       <c r="L43" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M43" s="9"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>1427</v>
       </c>
@@ -54579,8 +54693,9 @@
       <c r="L44" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M44" s="9"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>1428</v>
       </c>
@@ -54612,8 +54727,9 @@
       <c r="L45" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M45" s="9"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>1429</v>
       </c>
@@ -54645,8 +54761,9 @@
       <c r="L46" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M46" s="9"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>1430</v>
       </c>
@@ -54678,8 +54795,9 @@
       <c r="L47" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M47" s="9"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>1431</v>
       </c>
@@ -54711,8 +54829,9 @@
       <c r="L48" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M48" s="9"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>1432</v>
       </c>
@@ -54744,8 +54863,9 @@
       <c r="L49" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M49" s="9"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>1433</v>
       </c>
@@ -54777,8 +54897,9 @@
       <c r="L50" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M50" s="9"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>1434</v>
       </c>
@@ -54810,8 +54931,9 @@
       <c r="L51" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M51" s="9"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>1435</v>
       </c>
@@ -54843,8 +54965,9 @@
       <c r="L52" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M52" s="9"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>1436</v>
       </c>
@@ -54876,8 +54999,9 @@
       <c r="L53" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M53" s="9"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>1437</v>
       </c>
@@ -54909,8 +55033,9 @@
       <c r="L54" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M54" s="9"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>1438</v>
       </c>
@@ -54942,8 +55067,9 @@
       <c r="L55" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M55" s="9"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>1439</v>
       </c>
@@ -54975,8 +55101,9 @@
       <c r="L56" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M56" s="9"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>1440</v>
       </c>
@@ -55008,8 +55135,9 @@
       <c r="L57" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M57" s="9"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>1441</v>
       </c>
@@ -55041,8 +55169,9 @@
       <c r="L58" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M58" s="9"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>1442</v>
       </c>
@@ -55074,8 +55203,9 @@
       <c r="L59" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M59" s="9"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>1443</v>
       </c>
@@ -55107,8 +55237,9 @@
       <c r="L60" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M60" s="9"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>1444</v>
       </c>
@@ -55140,8 +55271,9 @@
       <c r="L61" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M61" s="9"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>1445</v>
       </c>
@@ -55173,8 +55305,9 @@
       <c r="L62" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M62" s="9"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>1446</v>
       </c>
@@ -55206,8 +55339,9 @@
       <c r="L63" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M63" s="9"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>1447</v>
       </c>
@@ -55239,8 +55373,9 @@
       <c r="L64" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M64" s="9"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>1448</v>
       </c>
@@ -55272,8 +55407,9 @@
       <c r="L65" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M65" s="9"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>1449</v>
       </c>
@@ -55305,8 +55441,9 @@
       <c r="L66" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M66" s="9"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>1450</v>
       </c>
@@ -55338,8 +55475,9 @@
       <c r="L67" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M67" s="9"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>1451</v>
       </c>
@@ -55371,8 +55509,9 @@
       <c r="L68" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M68" s="9"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>1452</v>
       </c>
@@ -55404,8 +55543,9 @@
       <c r="L69" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M69" s="9"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>1453</v>
       </c>
@@ -55437,8 +55577,9 @@
       <c r="L70" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M70" s="9"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>1454</v>
       </c>
@@ -55470,8 +55611,9 @@
       <c r="L71" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M71" s="9"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>1455</v>
       </c>
@@ -55503,8 +55645,9 @@
       <c r="L72" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M72" s="9"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>1456</v>
       </c>
@@ -55536,8 +55679,9 @@
       <c r="L73" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M73" s="9"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>1457</v>
       </c>
@@ -55569,8 +55713,9 @@
       <c r="L74" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M74" s="9"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>1458</v>
       </c>
@@ -55602,8 +55747,9 @@
       <c r="L75" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M75" s="9"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>1459</v>
       </c>
@@ -55635,8 +55781,9 @@
       <c r="L76" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M76" s="9"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>1460</v>
       </c>
@@ -55668,8 +55815,9 @@
       <c r="L77" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M77" s="9"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>1461</v>
       </c>
@@ -55701,8 +55849,9 @@
       <c r="L78" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M78" s="9"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>1462</v>
       </c>
@@ -55734,8 +55883,9 @@
       <c r="L79" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M79" s="9"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>1463</v>
       </c>
@@ -55767,8 +55917,9 @@
       <c r="L80" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M80" s="9"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>1464</v>
       </c>
@@ -55800,8 +55951,9 @@
       <c r="L81" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M81" s="9"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>1465</v>
       </c>
@@ -55833,8 +55985,9 @@
       <c r="L82" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M82" s="9"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>1466</v>
       </c>
@@ -55866,8 +56019,9 @@
       <c r="L83" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M83" s="9"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>1467</v>
       </c>
@@ -55899,8 +56053,9 @@
       <c r="L84" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M84" s="9"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>1468</v>
       </c>
@@ -55932,8 +56087,9 @@
       <c r="L85" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M85" s="9"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>1469</v>
       </c>
@@ -55965,8 +56121,9 @@
       <c r="L86" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M86" s="9"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>2277</v>
       </c>
@@ -55997,8 +56154,9 @@
       <c r="L87" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M87" s="9"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>2310</v>
       </c>
@@ -56029,8 +56187,11 @@
       <c r="L88" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M88" s="9">
+        <v>9.07</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>2366</v>
       </c>
@@ -56058,8 +56219,9 @@
       <c r="L89" t="s">
         <v>2357</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M89" s="9"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>2367</v>
       </c>
@@ -56087,8 +56249,9 @@
       <c r="L90" t="s">
         <v>2357</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M90" s="9"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>2368</v>
       </c>
@@ -56116,8 +56279,9 @@
       <c r="L91" t="s">
         <v>2357</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M91" s="9"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>2427</v>
       </c>
@@ -56150,8 +56314,11 @@
       <c r="L92" s="2" t="s">
         <v>2421</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M92" s="9">
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>2588</v>
       </c>
@@ -56179,8 +56346,9 @@
       <c r="L93" t="s">
         <v>2583</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M93" s="9"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>2595</v>
       </c>
@@ -56208,8 +56376,9 @@
       <c r="L94" t="s">
         <v>2589</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M94" s="9"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>4345</v>
       </c>
@@ -56240,6 +56409,9 @@
       </c>
       <c r="L95" t="s">
         <v>1385</v>
+      </c>
+      <c r="M95" s="9">
+        <v>1.41</v>
       </c>
     </row>
   </sheetData>
@@ -56486,7 +56658,7 @@
       <c r="F2" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -56507,7 +56679,7 @@
       <c r="F3" t="s">
         <v>2465</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -56528,7 +56700,7 @@
       <c r="F4" t="s">
         <v>2718</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -56549,7 +56721,7 @@
       <c r="F5" t="s">
         <v>2903</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -56570,7 +56742,7 @@
       <c r="F6" t="s">
         <v>2974</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -56591,7 +56763,7 @@
       <c r="F7" t="s">
         <v>4265</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>4.5</v>
       </c>
     </row>
@@ -56614,7 +56786,7 @@
       <c r="F8" t="s">
         <v>4335</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <v>1.05</v>
       </c>
     </row>
@@ -56637,7 +56809,7 @@
       <c r="F9" t="s">
         <v>4500</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>1.73</v>
       </c>
     </row>
@@ -56651,7 +56823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -56749,7 +56921,7 @@
       <c r="L2" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="10"/>
+      <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -56785,7 +56957,7 @@
       <c r="L3" t="s">
         <v>2293</v>
       </c>
-      <c r="M3" s="10"/>
+      <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -56815,7 +56987,7 @@
       <c r="L4" t="s">
         <v>2351</v>
       </c>
-      <c r="M4" s="10"/>
+      <c r="M4" s="9"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -56848,7 +57020,7 @@
       <c r="L5" t="s">
         <v>2410</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -56878,7 +57050,7 @@
       <c r="L6" t="s">
         <v>2432</v>
       </c>
-      <c r="M6" s="10"/>
+      <c r="M6" s="9"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -56914,7 +57086,7 @@
       <c r="L7" t="s">
         <v>2524</v>
       </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -56941,7 +57113,7 @@
       <c r="L8" t="s">
         <v>2541</v>
       </c>
-      <c r="M8" s="10"/>
+      <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -56971,7 +57143,7 @@
       <c r="L9" t="s">
         <v>2552</v>
       </c>
-      <c r="M9" s="10"/>
+      <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -56992,7 +57164,7 @@
       <c r="L10" t="s">
         <v>2563</v>
       </c>
-      <c r="M10" s="10"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -57022,7 +57194,7 @@
       <c r="L11" t="s">
         <v>2596</v>
       </c>
-      <c r="M11" s="10"/>
+      <c r="M11" s="9"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -57052,7 +57224,7 @@
       <c r="L12" t="s">
         <v>2612</v>
       </c>
-      <c r="M12" s="10"/>
+      <c r="M12" s="9"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -57082,7 +57254,7 @@
       <c r="L13" t="s">
         <v>2901</v>
       </c>
-      <c r="M13" s="10"/>
+      <c r="M13" s="9"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -57118,7 +57290,7 @@
       <c r="L14" t="s">
         <v>4292</v>
       </c>
-      <c r="M14" s="10"/>
+      <c r="M14" s="9"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -57157,7 +57329,7 @@
       <c r="L15" t="s">
         <v>4354</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="9">
         <v>11.15</v>
       </c>
     </row>
@@ -57195,7 +57367,7 @@
       <c r="L16" t="s">
         <v>4546</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="9">
         <v>0.84</v>
       </c>
     </row>
@@ -57341,10 +57513,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57399,7 +57571,7 @@
       <c r="F2" t="s">
         <v>2317</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -57420,7 +57592,7 @@
       <c r="F3" t="s">
         <v>2321</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -57441,7 +57613,7 @@
       <c r="F4" t="s">
         <v>2327</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -57462,7 +57634,7 @@
       <c r="F5" t="s">
         <v>2338</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -57483,7 +57655,7 @@
       <c r="F6" t="s">
         <v>2462</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -57504,7 +57676,7 @@
       <c r="F7" t="s">
         <v>2481</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -57525,7 +57697,7 @@
       <c r="F8" t="s">
         <v>2482</v>
       </c>
-      <c r="G8" s="10"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -57546,7 +57718,7 @@
       <c r="F9" t="s">
         <v>2527</v>
       </c>
-      <c r="G9" s="10"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -57567,7 +57739,7 @@
       <c r="F10" t="s">
         <v>2529</v>
       </c>
-      <c r="G10" s="10"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -57588,7 +57760,7 @@
       <c r="F11" t="s">
         <v>2527</v>
       </c>
-      <c r="G11" s="10"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -57609,7 +57781,7 @@
       <c r="F12" t="s">
         <v>2559</v>
       </c>
-      <c r="G12" s="10"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -57630,7 +57802,7 @@
       <c r="F13" t="s">
         <v>2721</v>
       </c>
-      <c r="G13" s="10"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -57651,7 +57823,7 @@
       <c r="F14" t="s">
         <v>2726</v>
       </c>
-      <c r="G14" s="10"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -57672,7 +57844,7 @@
       <c r="F15" t="s">
         <v>2920</v>
       </c>
-      <c r="G15" s="10"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -57693,7 +57865,7 @@
       <c r="F16" t="s">
         <v>3371</v>
       </c>
-      <c r="G16" s="10"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -57714,7 +57886,7 @@
       <c r="F17" t="s">
         <v>3374</v>
       </c>
-      <c r="G17" s="10"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -57735,7 +57907,7 @@
       <c r="F18" t="s">
         <v>4263</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="9">
         <v>6.8</v>
       </c>
     </row>
@@ -57758,8 +57930,31 @@
       <c r="F19" t="s">
         <v>4516</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="9">
         <v>0.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>4548</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4549</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2290</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4551</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4514</v>
+      </c>
+      <c r="F20" t="s">
+        <v>4550</v>
+      </c>
+      <c r="G20" s="9">
+        <v>6.27</v>
       </c>
     </row>
   </sheetData>
@@ -57828,7 +58023,7 @@
       <c r="F2" t="s">
         <v>2374</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -57849,7 +58044,7 @@
       <c r="F3" t="s">
         <v>2471</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -57864,7 +58059,7 @@
       <c r="F4" t="s">
         <v>2715</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -57885,7 +58080,7 @@
       <c r="F5" t="s">
         <v>2908</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -57906,7 +58101,7 @@
       <c r="F6" t="s">
         <v>2931</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -57927,7 +58122,7 @@
       <c r="F7" t="s">
         <v>2992</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>3.12</v>
       </c>
     </row>
@@ -57950,7 +58145,7 @@
       <c r="F8" t="s">
         <v>4248</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <v>26.62</v>
       </c>
     </row>
@@ -57973,7 +58168,7 @@
       <c r="F9" t="s">
         <v>4274</v>
       </c>
-      <c r="G9" s="10"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -57994,7 +58189,7 @@
       <c r="F10" t="s">
         <v>4279</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>0.3</v>
       </c>
     </row>
@@ -58017,7 +58212,7 @@
       <c r="F11" t="s">
         <v>4505</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>5.0999999999999996</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add LMV331 in SOT-23 package to the library
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12279" uniqueCount="4555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12285" uniqueCount="4559">
   <si>
     <t>Part Number</t>
   </si>
@@ -13696,6 +13696,18 @@
   </si>
   <si>
     <t>TERM_3.50MM_4x1_0</t>
+  </si>
+  <si>
+    <t>ANLG-00019</t>
+  </si>
+  <si>
+    <t>Comparator, Single, LM331, SOT-23-5</t>
+  </si>
+  <si>
+    <t>LMV331IDBVR</t>
+  </si>
+  <si>
+    <t>LMV331</t>
   </si>
 </sst>
 </file>
@@ -34638,7 +34650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -57513,10 +57525,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57955,6 +57967,29 @@
       </c>
       <c r="G20" s="9">
         <v>6.27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>4555</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4556</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2290</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4557</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2525</v>
+      </c>
+      <c r="F21" t="s">
+        <v>4558</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add several new components
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12285" uniqueCount="4559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12329" uniqueCount="4588">
   <si>
     <t>Part Number</t>
   </si>
@@ -13708,6 +13708,93 @@
   </si>
   <si>
     <t>LMV331</t>
+  </si>
+  <si>
+    <t>3357-02</t>
+  </si>
+  <si>
+    <t>PWREG-00015</t>
+  </si>
+  <si>
+    <t>REG CNTRL, SW Buck, LM5085</t>
+  </si>
+  <si>
+    <t>LM5085</t>
+  </si>
+  <si>
+    <t>LM5085MY/NOPB</t>
+  </si>
+  <si>
+    <t>4.5 - 75V</t>
+  </si>
+  <si>
+    <t>MAG-00094</t>
+  </si>
+  <si>
+    <t>20.2A</t>
+  </si>
+  <si>
+    <t>6.9 mOhm</t>
+  </si>
+  <si>
+    <t>74437529203330</t>
+  </si>
+  <si>
+    <t>WURTH_74437529203330</t>
+  </si>
+  <si>
+    <t>XSTR-00019</t>
+  </si>
+  <si>
+    <t>23A</t>
+  </si>
+  <si>
+    <t>140W</t>
+  </si>
+  <si>
+    <t>IRF9540NPBF</t>
+  </si>
+  <si>
+    <t>TO-220_0</t>
+  </si>
+  <si>
+    <t>p-mosfet_2</t>
+  </si>
+  <si>
+    <t>1.1V</t>
+  </si>
+  <si>
+    <t>Bridge</t>
+  </si>
+  <si>
+    <t>GBPC3502W-E4/51</t>
+  </si>
+  <si>
+    <t>rect_0</t>
+  </si>
+  <si>
+    <t>35A</t>
+  </si>
+  <si>
+    <t>Dio Bridge Rect, 35A</t>
+  </si>
+  <si>
+    <t>rect_GBPC-W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuse Holder, Cartridge, 1/4" dia. </t>
+  </si>
+  <si>
+    <t>Littelfuse</t>
+  </si>
+  <si>
+    <t>LITTELFUSE_122_FUSE_CLIP</t>
+  </si>
+  <si>
+    <t>MISC-00010</t>
+  </si>
+  <si>
+    <t>01220093Z</t>
   </si>
 </sst>
 </file>
@@ -13769,7 +13856,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -13781,12 +13868,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -14070,7 +14158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J839"/>
   <sheetViews>
-    <sheetView topLeftCell="A285" workbookViewId="0">
+    <sheetView topLeftCell="A567" workbookViewId="0">
       <selection activeCell="J309" sqref="J309"/>
     </sheetView>
   </sheetViews>
@@ -14085,7 +14173,7 @@
     <col min="7" max="7" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="9"/>
+    <col min="10" max="10" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -14095,7 +14183,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>924</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -14116,7 +14204,7 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>4523</v>
       </c>
     </row>
@@ -14148,7 +14236,7 @@
       <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="10"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -23023,7 +23111,7 @@
       <c r="I308" t="s">
         <v>12</v>
       </c>
-      <c r="J308" s="9">
+      <c r="J308" s="8">
         <v>0.14399999999999999</v>
       </c>
     </row>
@@ -32154,7 +32242,7 @@
       <c r="F2" t="s">
         <v>2567</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -32175,7 +32263,7 @@
       <c r="F3" t="s">
         <v>2570</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -32196,7 +32284,7 @@
       <c r="F4" t="s">
         <v>2573</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -32217,7 +32305,7 @@
       <c r="F5" t="s">
         <v>2582</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -32238,7 +32326,7 @@
       <c r="F6" t="s">
         <v>4329</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -32259,7 +32347,7 @@
       <c r="F7" t="s">
         <v>4316</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -32280,7 +32368,7 @@
       <c r="F8" t="s">
         <v>4316</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -32301,7 +32389,7 @@
       <c r="F9" t="s">
         <v>4315</v>
       </c>
-      <c r="G9" s="9"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -32322,7 +32410,7 @@
       <c r="F10" t="s">
         <v>4315</v>
       </c>
-      <c r="G10" s="9"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -32343,7 +32431,7 @@
       <c r="F11" t="s">
         <v>4349</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>0.45</v>
       </c>
     </row>
@@ -32366,7 +32454,7 @@
       <c r="F12" t="s">
         <v>4349</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -32387,18 +32475,18 @@
       <c r="F13" t="s">
         <v>4539</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>0.84</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G14" s="9"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G15" s="9"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G16" s="9"/>
+      <c r="G16" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32408,10 +32496,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32500,7 +32588,7 @@
       <c r="K2" t="s">
         <v>2238</v>
       </c>
-      <c r="L2" s="9"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -32536,7 +32624,7 @@
       <c r="K3" t="s">
         <v>2238</v>
       </c>
-      <c r="L3" s="9"/>
+      <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -32572,7 +32660,7 @@
       <c r="K4" t="s">
         <v>2246</v>
       </c>
-      <c r="L4" s="9"/>
+      <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -32608,7 +32696,7 @@
       <c r="K5" t="s">
         <v>2246</v>
       </c>
-      <c r="L5" s="9"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -32644,7 +32732,7 @@
       <c r="K6" t="s">
         <v>2261</v>
       </c>
-      <c r="L6" s="9"/>
+      <c r="L6" s="8"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -32680,7 +32768,7 @@
       <c r="K7" t="s">
         <v>2276</v>
       </c>
-      <c r="L7" s="9"/>
+      <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -32716,7 +32804,7 @@
       <c r="K8" t="s">
         <v>2261</v>
       </c>
-      <c r="L8" s="9"/>
+      <c r="L8" s="8"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -32752,7 +32840,7 @@
       <c r="K9" t="s">
         <v>2297</v>
       </c>
-      <c r="L9" s="9"/>
+      <c r="L9" s="8"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -32788,7 +32876,7 @@
       <c r="K10" t="s">
         <v>2297</v>
       </c>
-      <c r="L10" s="9"/>
+      <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -32824,7 +32912,7 @@
       <c r="K11" t="s">
         <v>2276</v>
       </c>
-      <c r="L11" s="9"/>
+      <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -32860,7 +32948,7 @@
       <c r="K12" t="s">
         <v>2276</v>
       </c>
-      <c r="L12" s="9"/>
+      <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -32896,7 +32984,7 @@
       <c r="K13" t="s">
         <v>2261</v>
       </c>
-      <c r="L13" s="9"/>
+      <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -32923,7 +33011,7 @@
       <c r="K14" t="s">
         <v>2491</v>
       </c>
-      <c r="L14" s="9"/>
+      <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -32959,7 +33047,7 @@
       <c r="K15" t="s">
         <v>2549</v>
       </c>
-      <c r="L15" s="9"/>
+      <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -32995,7 +33083,7 @@
       <c r="K16" t="s">
         <v>2600</v>
       </c>
-      <c r="L16" s="9"/>
+      <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -33031,7 +33119,7 @@
       <c r="K17" t="s">
         <v>2261</v>
       </c>
-      <c r="L17" s="9"/>
+      <c r="L17" s="8"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -33067,7 +33155,7 @@
       <c r="K18" t="s">
         <v>2238</v>
       </c>
-      <c r="L18" s="9"/>
+      <c r="L18" s="8"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -33103,7 +33191,7 @@
       <c r="K19" t="s">
         <v>2261</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="8">
         <v>0.31</v>
       </c>
     </row>
@@ -33141,8 +33229,47 @@
       <c r="K20" t="s">
         <v>2276</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="8">
         <v>2.5299999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>4570</v>
+      </c>
+      <c r="B21" t="str">
+        <f>CONCATENATE("XSTR ",F21,", ",D21,", ",C21,", Vgs ",G21,", ",LEFT(J21,6))</f>
+        <v>XSTR PFET, 23A, 100V, Vgs 20V, TO-220</v>
+      </c>
+      <c r="C21" t="s">
+        <v>947</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4571</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4572</v>
+      </c>
+      <c r="F21" t="s">
+        <v>2270</v>
+      </c>
+      <c r="G21" t="s">
+        <v>2178</v>
+      </c>
+      <c r="H21" t="s">
+        <v>2301</v>
+      </c>
+      <c r="I21" t="s">
+        <v>4573</v>
+      </c>
+      <c r="J21" t="s">
+        <v>4574</v>
+      </c>
+      <c r="K21" t="s">
+        <v>4575</v>
+      </c>
+      <c r="L21" s="8">
+        <v>1.36</v>
       </c>
     </row>
   </sheetData>
@@ -33153,10 +33280,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33248,7 +33375,7 @@
       <c r="L2" s="2" t="s">
         <v>2100</v>
       </c>
-      <c r="M2" s="9"/>
+      <c r="M2" s="8"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -33281,7 +33408,7 @@
       <c r="L3" s="2" t="s">
         <v>2100</v>
       </c>
-      <c r="M3" s="9"/>
+      <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -33314,7 +33441,7 @@
       <c r="L4" s="2" t="s">
         <v>2100</v>
       </c>
-      <c r="M4" s="9"/>
+      <c r="M4" s="8"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -33347,7 +33474,7 @@
       <c r="L5" s="2" t="s">
         <v>2100</v>
       </c>
-      <c r="M5" s="9"/>
+      <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -33380,7 +33507,7 @@
       <c r="L6" s="2" t="s">
         <v>2100</v>
       </c>
-      <c r="M6" s="9"/>
+      <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -33413,7 +33540,7 @@
       <c r="L7" s="2" t="s">
         <v>2100</v>
       </c>
-      <c r="M7" s="9"/>
+      <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -33449,7 +33576,7 @@
       <c r="L8" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M8" s="9"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -33485,7 +33612,7 @@
       <c r="L9" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M9" s="9"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -33521,7 +33648,7 @@
       <c r="L10" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M10" s="9"/>
+      <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -33557,7 +33684,7 @@
       <c r="L11" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M11" s="9"/>
+      <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -33593,7 +33720,7 @@
       <c r="L12" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M12" s="9"/>
+      <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -33629,7 +33756,7 @@
       <c r="L13" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M13" s="9"/>
+      <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -33665,7 +33792,7 @@
       <c r="L14" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M14" s="9"/>
+      <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -33701,7 +33828,7 @@
       <c r="L15" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M15" s="9"/>
+      <c r="M15" s="8"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -33737,7 +33864,7 @@
       <c r="L16" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M16" s="9"/>
+      <c r="M16" s="8"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -33773,7 +33900,7 @@
       <c r="L17" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M17" s="9"/>
+      <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -33809,7 +33936,7 @@
       <c r="L18" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M18" s="9"/>
+      <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
@@ -33845,7 +33972,7 @@
       <c r="L19" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M19" s="9"/>
+      <c r="M19" s="8"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -33881,7 +34008,7 @@
       <c r="L20" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M20" s="9"/>
+      <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
@@ -33917,7 +34044,7 @@
       <c r="L21" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M21" s="9"/>
+      <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
@@ -33953,7 +34080,7 @@
       <c r="L22" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M22" s="9"/>
+      <c r="M22" s="8"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
@@ -33989,7 +34116,7 @@
       <c r="L23" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M23" s="9"/>
+      <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
@@ -34025,7 +34152,7 @@
       <c r="L24" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M24" s="9"/>
+      <c r="M24" s="8"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -34061,7 +34188,7 @@
       <c r="L25" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M25" s="9"/>
+      <c r="M25" s="8"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -34097,7 +34224,7 @@
       <c r="L26" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M26" s="9"/>
+      <c r="M26" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -34133,7 +34260,7 @@
       <c r="L27" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M27" s="9"/>
+      <c r="M27" s="8"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
@@ -34169,7 +34296,7 @@
       <c r="L28" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M28" s="9"/>
+      <c r="M28" s="8"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -34205,7 +34332,7 @@
       <c r="L29" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M29" s="9"/>
+      <c r="M29" s="8"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
@@ -34241,7 +34368,7 @@
       <c r="L30" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M30" s="9"/>
+      <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
@@ -34277,7 +34404,7 @@
       <c r="L31" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M31" s="9"/>
+      <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -34313,7 +34440,7 @@
       <c r="L32" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M32" s="9"/>
+      <c r="M32" s="8"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
@@ -34349,7 +34476,7 @@
       <c r="L33" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="M33" s="9"/>
+      <c r="M33" s="8"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
@@ -34379,7 +34506,7 @@
       <c r="L34" s="2" t="s">
         <v>2403</v>
       </c>
-      <c r="M34" s="9"/>
+      <c r="M34" s="8"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
@@ -34409,7 +34536,7 @@
       <c r="L35" s="2" t="s">
         <v>2504</v>
       </c>
-      <c r="M35" s="9"/>
+      <c r="M35" s="8"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
@@ -34439,7 +34566,7 @@
       <c r="L36" s="2" t="s">
         <v>2505</v>
       </c>
-      <c r="M36" s="9"/>
+      <c r="M36" s="8"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
@@ -34469,7 +34596,7 @@
       <c r="L37" s="2" t="s">
         <v>2505</v>
       </c>
-      <c r="M37" s="9"/>
+      <c r="M37" s="8"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
@@ -34499,7 +34626,7 @@
       <c r="L38" s="2" t="s">
         <v>2949</v>
       </c>
-      <c r="M38" s="9"/>
+      <c r="M38" s="8"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
@@ -34529,7 +34656,7 @@
       <c r="L39" s="2" t="s">
         <v>2949</v>
       </c>
-      <c r="M39" s="9"/>
+      <c r="M39" s="8"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
@@ -34565,7 +34692,7 @@
       <c r="L40" s="2" t="s">
         <v>2982</v>
       </c>
-      <c r="M40" s="9">
+      <c r="M40" s="8">
         <v>0.19</v>
       </c>
     </row>
@@ -34600,7 +34727,7 @@
       <c r="L41" s="2" t="s">
         <v>4286</v>
       </c>
-      <c r="M41" s="9"/>
+      <c r="M41" s="8"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
@@ -34636,8 +34763,37 @@
       <c r="L42" s="2" t="s">
         <v>2505</v>
       </c>
-      <c r="M42" s="9">
+      <c r="M42" s="8">
         <v>0.34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B43" s="2" t="s">
+        <v>4581</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>4576</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>4580</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>4577</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>2433</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>4578</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>4582</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>4579</v>
+      </c>
+      <c r="M43" s="8">
+        <v>5.26</v>
       </c>
     </row>
   </sheetData>
@@ -34651,7 +34807,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34733,7 +34889,7 @@
       <c r="J2" t="s">
         <v>2386</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="8">
         <v>1.19</v>
       </c>
     </row>
@@ -34768,7 +34924,9 @@
       <c r="J3" t="s">
         <v>2393</v>
       </c>
-      <c r="K3" s="9"/>
+      <c r="K3" s="8">
+        <v>1.68</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -34786,13 +34944,24 @@
       <c r="E4">
         <v>2</v>
       </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2896</v>
+      </c>
+      <c r="H4">
+        <v>61300621121</v>
+      </c>
       <c r="I4" t="s">
         <v>2401</v>
       </c>
       <c r="J4" t="s">
         <v>2400</v>
       </c>
-      <c r="K4" s="9"/>
+      <c r="K4" s="8">
+        <v>0.54</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -34813,7 +34982,7 @@
       <c r="J5" t="s">
         <v>2449</v>
       </c>
-      <c r="K5" s="9"/>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -34834,7 +35003,7 @@
       <c r="J6" t="s">
         <v>2456</v>
       </c>
-      <c r="K6" s="9"/>
+      <c r="K6" s="8"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -34855,7 +35024,7 @@
       <c r="J7" t="s">
         <v>2457</v>
       </c>
-      <c r="K7" s="9"/>
+      <c r="K7" s="8"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -34888,7 +35057,7 @@
       <c r="J8" t="s">
         <v>2386</v>
       </c>
-      <c r="K8" s="9"/>
+      <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -34912,7 +35081,7 @@
       <c r="J9" t="s">
         <v>2515</v>
       </c>
-      <c r="K9" s="9"/>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -34933,7 +35102,7 @@
       <c r="J10" t="s">
         <v>2577</v>
       </c>
-      <c r="K10" s="9"/>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -34966,7 +35135,7 @@
       <c r="J11" t="s">
         <v>2386</v>
       </c>
-      <c r="K11" s="9"/>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -34999,7 +35168,7 @@
       <c r="J12" t="s">
         <v>2393</v>
       </c>
-      <c r="K12" s="9"/>
+      <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -35032,7 +35201,7 @@
       <c r="J13" t="s">
         <v>2910</v>
       </c>
-      <c r="K13" s="9"/>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -35056,7 +35225,7 @@
       <c r="J14" t="s">
         <v>2965</v>
       </c>
-      <c r="K14" s="9"/>
+      <c r="K14" s="8"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -35080,7 +35249,7 @@
       <c r="J15" t="s">
         <v>2972</v>
       </c>
-      <c r="K15" s="9"/>
+      <c r="K15" s="8"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -35113,7 +35282,7 @@
       <c r="J16" t="s">
         <v>2393</v>
       </c>
-      <c r="K16" s="9"/>
+      <c r="K16" s="8"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -35134,8 +35303,8 @@
       <c r="G17" t="s">
         <v>3378</v>
       </c>
-      <c r="H17" s="7">
-        <v>605240</v>
+      <c r="H17" s="10" t="s">
+        <v>4559</v>
       </c>
       <c r="I17" t="s">
         <v>3379</v>
@@ -35143,7 +35312,9 @@
       <c r="J17" t="s">
         <v>3380</v>
       </c>
-      <c r="K17" s="9"/>
+      <c r="K17" s="8">
+        <v>0.98</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -35170,7 +35341,7 @@
       <c r="J18" t="s">
         <v>4260</v>
       </c>
-      <c r="K18" s="9"/>
+      <c r="K18" s="8"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -35197,7 +35368,7 @@
       <c r="J19" t="s">
         <v>2577</v>
       </c>
-      <c r="K19" s="9"/>
+      <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -35224,7 +35395,7 @@
       <c r="J20" t="s">
         <v>4259</v>
       </c>
-      <c r="K20" s="9"/>
+      <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -35248,7 +35419,7 @@
       <c r="J21" t="s">
         <v>4271</v>
       </c>
-      <c r="K21" s="9"/>
+      <c r="K21" s="8"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -35278,7 +35449,7 @@
       <c r="J22" t="s">
         <v>4303</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="8">
         <v>4.45</v>
       </c>
     </row>
@@ -35313,7 +35484,7 @@
       <c r="J23" t="s">
         <v>2386</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="8">
         <v>0.79</v>
       </c>
     </row>
@@ -35348,7 +35519,7 @@
       <c r="J24" t="s">
         <v>2386</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="8">
         <v>1.19</v>
       </c>
     </row>
@@ -35383,7 +35554,7 @@
       <c r="J25" t="s">
         <v>2393</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="8">
         <v>0.79</v>
       </c>
     </row>
@@ -35418,7 +35589,7 @@
       <c r="J26" t="s">
         <v>2965</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K26" s="8">
         <v>1.67</v>
       </c>
     </row>
@@ -35448,7 +35619,7 @@
     <col min="8" max="8" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="9"/>
+    <col min="11" max="11" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -35482,7 +35653,7 @@
       <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>4523</v>
       </c>
     </row>
@@ -53140,7 +53311,7 @@
       <c r="J536" t="s">
         <v>23</v>
       </c>
-      <c r="K536" s="9">
+      <c r="K536" s="8">
         <v>0.187</v>
       </c>
     </row>
@@ -53176,7 +53347,7 @@
       <c r="J537" t="s">
         <v>23</v>
       </c>
-      <c r="K537" s="9">
+      <c r="K537" s="8">
         <v>0.88</v>
       </c>
     </row>
@@ -53187,10 +53358,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M95"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53275,7 +53446,7 @@
       <c r="L2" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="9">
+      <c r="M2" s="8">
         <v>0.1</v>
       </c>
     </row>
@@ -53311,7 +53482,7 @@
       <c r="L3" t="s">
         <v>1385</v>
       </c>
-      <c r="M3" s="9"/>
+      <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -53345,7 +53516,7 @@
       <c r="L4" t="s">
         <v>1385</v>
       </c>
-      <c r="M4" s="9"/>
+      <c r="M4" s="8"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -53379,7 +53550,7 @@
       <c r="L5" t="s">
         <v>1385</v>
       </c>
-      <c r="M5" s="9"/>
+      <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -53413,7 +53584,7 @@
       <c r="L6" t="s">
         <v>1385</v>
       </c>
-      <c r="M6" s="9"/>
+      <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -53447,7 +53618,7 @@
       <c r="L7" t="s">
         <v>1385</v>
       </c>
-      <c r="M7" s="9"/>
+      <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -53481,7 +53652,7 @@
       <c r="L8" t="s">
         <v>1385</v>
       </c>
-      <c r="M8" s="9"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -53515,7 +53686,7 @@
       <c r="L9" t="s">
         <v>1385</v>
       </c>
-      <c r="M9" s="9"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -53549,7 +53720,7 @@
       <c r="L10" t="s">
         <v>1385</v>
       </c>
-      <c r="M10" s="9"/>
+      <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -53583,7 +53754,7 @@
       <c r="L11" t="s">
         <v>1385</v>
       </c>
-      <c r="M11" s="9"/>
+      <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -53617,7 +53788,7 @@
       <c r="L12" t="s">
         <v>1385</v>
       </c>
-      <c r="M12" s="9"/>
+      <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -53651,7 +53822,7 @@
       <c r="L13" t="s">
         <v>1385</v>
       </c>
-      <c r="M13" s="9"/>
+      <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -53685,7 +53856,7 @@
       <c r="L14" t="s">
         <v>1385</v>
       </c>
-      <c r="M14" s="9"/>
+      <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -53719,7 +53890,7 @@
       <c r="L15" t="s">
         <v>1385</v>
       </c>
-      <c r="M15" s="9"/>
+      <c r="M15" s="8"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -53753,7 +53924,7 @@
       <c r="L16" t="s">
         <v>1385</v>
       </c>
-      <c r="M16" s="9"/>
+      <c r="M16" s="8"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -53787,7 +53958,7 @@
       <c r="L17" t="s">
         <v>1385</v>
       </c>
-      <c r="M17" s="9"/>
+      <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -53821,7 +53992,7 @@
       <c r="L18" t="s">
         <v>1385</v>
       </c>
-      <c r="M18" s="9"/>
+      <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -53855,7 +54026,7 @@
       <c r="L19" t="s">
         <v>1385</v>
       </c>
-      <c r="M19" s="9"/>
+      <c r="M19" s="8"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -53889,7 +54060,7 @@
       <c r="L20" t="s">
         <v>1385</v>
       </c>
-      <c r="M20" s="9"/>
+      <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -53923,7 +54094,7 @@
       <c r="L21" t="s">
         <v>1385</v>
       </c>
-      <c r="M21" s="9"/>
+      <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -53957,7 +54128,7 @@
       <c r="L22" t="s">
         <v>1385</v>
       </c>
-      <c r="M22" s="9"/>
+      <c r="M22" s="8"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -53991,7 +54162,7 @@
       <c r="L23" t="s">
         <v>1385</v>
       </c>
-      <c r="M23" s="9"/>
+      <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -54025,7 +54196,7 @@
       <c r="L24" t="s">
         <v>1385</v>
       </c>
-      <c r="M24" s="9"/>
+      <c r="M24" s="8"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -54059,7 +54230,7 @@
       <c r="L25" t="s">
         <v>1385</v>
       </c>
-      <c r="M25" s="9"/>
+      <c r="M25" s="8"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -54093,7 +54264,7 @@
       <c r="L26" t="s">
         <v>1385</v>
       </c>
-      <c r="M26" s="9"/>
+      <c r="M26" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -54127,7 +54298,7 @@
       <c r="L27" t="s">
         <v>1385</v>
       </c>
-      <c r="M27" s="9"/>
+      <c r="M27" s="8"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -54161,7 +54332,7 @@
       <c r="L28" t="s">
         <v>1385</v>
       </c>
-      <c r="M28" s="9"/>
+      <c r="M28" s="8"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -54195,7 +54366,7 @@
       <c r="L29" t="s">
         <v>1385</v>
       </c>
-      <c r="M29" s="9"/>
+      <c r="M29" s="8"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -54229,7 +54400,7 @@
       <c r="L30" t="s">
         <v>1385</v>
       </c>
-      <c r="M30" s="9"/>
+      <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -54263,7 +54434,7 @@
       <c r="L31" t="s">
         <v>1385</v>
       </c>
-      <c r="M31" s="9"/>
+      <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -54297,7 +54468,7 @@
       <c r="L32" t="s">
         <v>1385</v>
       </c>
-      <c r="M32" s="9"/>
+      <c r="M32" s="8"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -54331,7 +54502,7 @@
       <c r="L33" t="s">
         <v>1385</v>
       </c>
-      <c r="M33" s="9"/>
+      <c r="M33" s="8"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -54365,7 +54536,7 @@
       <c r="L34" t="s">
         <v>1385</v>
       </c>
-      <c r="M34" s="9"/>
+      <c r="M34" s="8"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
@@ -54399,7 +54570,7 @@
       <c r="L35" t="s">
         <v>1385</v>
       </c>
-      <c r="M35" s="9"/>
+      <c r="M35" s="8"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -54433,7 +54604,7 @@
       <c r="L36" t="s">
         <v>1385</v>
       </c>
-      <c r="M36" s="9"/>
+      <c r="M36" s="8"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -54467,7 +54638,7 @@
       <c r="L37" t="s">
         <v>1385</v>
       </c>
-      <c r="M37" s="9"/>
+      <c r="M37" s="8"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -54501,7 +54672,7 @@
       <c r="L38" t="s">
         <v>1385</v>
       </c>
-      <c r="M38" s="9"/>
+      <c r="M38" s="8"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -54535,7 +54706,7 @@
       <c r="L39" t="s">
         <v>1385</v>
       </c>
-      <c r="M39" s="9"/>
+      <c r="M39" s="8"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
@@ -54569,7 +54740,7 @@
       <c r="L40" t="s">
         <v>1385</v>
       </c>
-      <c r="M40" s="9"/>
+      <c r="M40" s="8"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
@@ -54603,7 +54774,7 @@
       <c r="L41" t="s">
         <v>1385</v>
       </c>
-      <c r="M41" s="9"/>
+      <c r="M41" s="8"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
@@ -54637,7 +54808,7 @@
       <c r="L42" t="s">
         <v>1385</v>
       </c>
-      <c r="M42" s="9"/>
+      <c r="M42" s="8"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
@@ -54671,7 +54842,7 @@
       <c r="L43" t="s">
         <v>1385</v>
       </c>
-      <c r="M43" s="9"/>
+      <c r="M43" s="8"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
@@ -54705,7 +54876,7 @@
       <c r="L44" t="s">
         <v>1385</v>
       </c>
-      <c r="M44" s="9"/>
+      <c r="M44" s="8"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
@@ -54739,7 +54910,7 @@
       <c r="L45" t="s">
         <v>1385</v>
       </c>
-      <c r="M45" s="9"/>
+      <c r="M45" s="8"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -54773,7 +54944,7 @@
       <c r="L46" t="s">
         <v>1385</v>
       </c>
-      <c r="M46" s="9"/>
+      <c r="M46" s="8"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -54807,7 +54978,7 @@
       <c r="L47" t="s">
         <v>1385</v>
       </c>
-      <c r="M47" s="9"/>
+      <c r="M47" s="8"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -54841,7 +55012,7 @@
       <c r="L48" t="s">
         <v>1385</v>
       </c>
-      <c r="M48" s="9"/>
+      <c r="M48" s="8"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
@@ -54875,7 +55046,7 @@
       <c r="L49" t="s">
         <v>1385</v>
       </c>
-      <c r="M49" s="9"/>
+      <c r="M49" s="8"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
@@ -54909,7 +55080,7 @@
       <c r="L50" t="s">
         <v>1385</v>
       </c>
-      <c r="M50" s="9"/>
+      <c r="M50" s="8"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
@@ -54943,7 +55114,7 @@
       <c r="L51" t="s">
         <v>1385</v>
       </c>
-      <c r="M51" s="9"/>
+      <c r="M51" s="8"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
@@ -54977,7 +55148,7 @@
       <c r="L52" t="s">
         <v>1385</v>
       </c>
-      <c r="M52" s="9"/>
+      <c r="M52" s="8"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
@@ -55011,7 +55182,7 @@
       <c r="L53" t="s">
         <v>1385</v>
       </c>
-      <c r="M53" s="9"/>
+      <c r="M53" s="8"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
@@ -55045,7 +55216,7 @@
       <c r="L54" t="s">
         <v>1385</v>
       </c>
-      <c r="M54" s="9"/>
+      <c r="M54" s="8"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
@@ -55079,7 +55250,7 @@
       <c r="L55" t="s">
         <v>1385</v>
       </c>
-      <c r="M55" s="9"/>
+      <c r="M55" s="8"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
@@ -55113,7 +55284,7 @@
       <c r="L56" t="s">
         <v>1385</v>
       </c>
-      <c r="M56" s="9"/>
+      <c r="M56" s="8"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
@@ -55147,7 +55318,7 @@
       <c r="L57" t="s">
         <v>1385</v>
       </c>
-      <c r="M57" s="9"/>
+      <c r="M57" s="8"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
@@ -55181,7 +55352,7 @@
       <c r="L58" t="s">
         <v>1385</v>
       </c>
-      <c r="M58" s="9"/>
+      <c r="M58" s="8"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
@@ -55215,7 +55386,7 @@
       <c r="L59" t="s">
         <v>1385</v>
       </c>
-      <c r="M59" s="9"/>
+      <c r="M59" s="8"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
@@ -55249,7 +55420,7 @@
       <c r="L60" t="s">
         <v>1385</v>
       </c>
-      <c r="M60" s="9"/>
+      <c r="M60" s="8"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
@@ -55283,7 +55454,7 @@
       <c r="L61" t="s">
         <v>1385</v>
       </c>
-      <c r="M61" s="9"/>
+      <c r="M61" s="8"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
@@ -55317,7 +55488,7 @@
       <c r="L62" t="s">
         <v>1385</v>
       </c>
-      <c r="M62" s="9"/>
+      <c r="M62" s="8"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
@@ -55351,7 +55522,7 @@
       <c r="L63" t="s">
         <v>1385</v>
       </c>
-      <c r="M63" s="9"/>
+      <c r="M63" s="8"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
@@ -55385,7 +55556,7 @@
       <c r="L64" t="s">
         <v>1385</v>
       </c>
-      <c r="M64" s="9"/>
+      <c r="M64" s="8"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
@@ -55419,7 +55590,7 @@
       <c r="L65" t="s">
         <v>1385</v>
       </c>
-      <c r="M65" s="9"/>
+      <c r="M65" s="8"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
@@ -55453,7 +55624,7 @@
       <c r="L66" t="s">
         <v>1385</v>
       </c>
-      <c r="M66" s="9"/>
+      <c r="M66" s="8"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
@@ -55487,7 +55658,7 @@
       <c r="L67" t="s">
         <v>1385</v>
       </c>
-      <c r="M67" s="9"/>
+      <c r="M67" s="8"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
@@ -55521,7 +55692,7 @@
       <c r="L68" t="s">
         <v>1385</v>
       </c>
-      <c r="M68" s="9"/>
+      <c r="M68" s="8"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
@@ -55555,7 +55726,7 @@
       <c r="L69" t="s">
         <v>1385</v>
       </c>
-      <c r="M69" s="9"/>
+      <c r="M69" s="8"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
@@ -55589,7 +55760,7 @@
       <c r="L70" t="s">
         <v>1385</v>
       </c>
-      <c r="M70" s="9"/>
+      <c r="M70" s="8"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
@@ -55623,7 +55794,7 @@
       <c r="L71" t="s">
         <v>1385</v>
       </c>
-      <c r="M71" s="9"/>
+      <c r="M71" s="8"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
@@ -55657,7 +55828,7 @@
       <c r="L72" t="s">
         <v>1385</v>
       </c>
-      <c r="M72" s="9"/>
+      <c r="M72" s="8"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
@@ -55691,7 +55862,7 @@
       <c r="L73" t="s">
         <v>1385</v>
       </c>
-      <c r="M73" s="9"/>
+      <c r="M73" s="8"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
@@ -55725,7 +55896,7 @@
       <c r="L74" t="s">
         <v>1385</v>
       </c>
-      <c r="M74" s="9"/>
+      <c r="M74" s="8"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
@@ -55759,7 +55930,7 @@
       <c r="L75" t="s">
         <v>1385</v>
       </c>
-      <c r="M75" s="9"/>
+      <c r="M75" s="8"/>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
@@ -55793,7 +55964,7 @@
       <c r="L76" t="s">
         <v>1385</v>
       </c>
-      <c r="M76" s="9"/>
+      <c r="M76" s="8"/>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
@@ -55827,7 +55998,7 @@
       <c r="L77" t="s">
         <v>1385</v>
       </c>
-      <c r="M77" s="9"/>
+      <c r="M77" s="8"/>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
@@ -55861,7 +56032,7 @@
       <c r="L78" t="s">
         <v>1385</v>
       </c>
-      <c r="M78" s="9"/>
+      <c r="M78" s="8"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
@@ -55895,7 +56066,7 @@
       <c r="L79" t="s">
         <v>1385</v>
       </c>
-      <c r="M79" s="9"/>
+      <c r="M79" s="8"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
@@ -55929,7 +56100,7 @@
       <c r="L80" t="s">
         <v>1385</v>
       </c>
-      <c r="M80" s="9"/>
+      <c r="M80" s="8"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
@@ -55963,7 +56134,7 @@
       <c r="L81" t="s">
         <v>1385</v>
       </c>
-      <c r="M81" s="9"/>
+      <c r="M81" s="8"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
@@ -55997,7 +56168,7 @@
       <c r="L82" t="s">
         <v>1385</v>
       </c>
-      <c r="M82" s="9"/>
+      <c r="M82" s="8"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
@@ -56031,7 +56202,7 @@
       <c r="L83" t="s">
         <v>1385</v>
       </c>
-      <c r="M83" s="9"/>
+      <c r="M83" s="8"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
@@ -56065,7 +56236,7 @@
       <c r="L84" t="s">
         <v>1385</v>
       </c>
-      <c r="M84" s="9"/>
+      <c r="M84" s="8"/>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
@@ -56099,7 +56270,7 @@
       <c r="L85" t="s">
         <v>1385</v>
       </c>
-      <c r="M85" s="9"/>
+      <c r="M85" s="8"/>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
@@ -56133,7 +56304,7 @@
       <c r="L86" t="s">
         <v>1385</v>
       </c>
-      <c r="M86" s="9"/>
+      <c r="M86" s="8"/>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
@@ -56166,7 +56337,7 @@
       <c r="L87" t="s">
         <v>1385</v>
       </c>
-      <c r="M87" s="9"/>
+      <c r="M87" s="8"/>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
@@ -56199,7 +56370,7 @@
       <c r="L88" t="s">
         <v>1385</v>
       </c>
-      <c r="M88" s="9">
+      <c r="M88" s="8">
         <v>9.07</v>
       </c>
     </row>
@@ -56231,7 +56402,7 @@
       <c r="L89" t="s">
         <v>2357</v>
       </c>
-      <c r="M89" s="9"/>
+      <c r="M89" s="8"/>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
@@ -56261,7 +56432,7 @@
       <c r="L90" t="s">
         <v>2357</v>
       </c>
-      <c r="M90" s="9"/>
+      <c r="M90" s="8"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
@@ -56291,7 +56462,7 @@
       <c r="L91" t="s">
         <v>2357</v>
       </c>
-      <c r="M91" s="9"/>
+      <c r="M91" s="8"/>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
@@ -56326,7 +56497,7 @@
       <c r="L92" s="2" t="s">
         <v>2421</v>
       </c>
-      <c r="M92" s="9">
+      <c r="M92" s="8">
         <v>2.41</v>
       </c>
     </row>
@@ -56358,7 +56529,7 @@
       <c r="L93" t="s">
         <v>2583</v>
       </c>
-      <c r="M93" s="9"/>
+      <c r="M93" s="8"/>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
@@ -56388,7 +56559,7 @@
       <c r="L94" t="s">
         <v>2589</v>
       </c>
-      <c r="M94" s="9"/>
+      <c r="M94" s="8"/>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
@@ -56422,8 +56593,44 @@
       <c r="L95" t="s">
         <v>1385</v>
       </c>
-      <c r="M95" s="9">
+      <c r="M95" s="8">
         <v>1.41</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>4565</v>
+      </c>
+      <c r="B96" t="str">
+        <f>CONCATENATE("Ind",", ",C96,", ",D96,", ",E96,", ","Nonstandard")</f>
+        <v>Ind, 33uH, 20%, 20.2A, Nonstandard</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>1286</v>
+      </c>
+      <c r="E96" t="s">
+        <v>4566</v>
+      </c>
+      <c r="H96" t="s">
+        <v>4567</v>
+      </c>
+      <c r="I96" t="s">
+        <v>2423</v>
+      </c>
+      <c r="J96" s="11" t="s">
+        <v>4568</v>
+      </c>
+      <c r="K96" t="s">
+        <v>4569</v>
+      </c>
+      <c r="L96" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M96" s="8">
+        <v>8.85</v>
       </c>
     </row>
   </sheetData>
@@ -56670,7 +56877,7 @@
       <c r="F2" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -56691,7 +56898,7 @@
       <c r="F3" t="s">
         <v>2465</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -56712,7 +56919,7 @@
       <c r="F4" t="s">
         <v>2718</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -56733,7 +56940,7 @@
       <c r="F5" t="s">
         <v>2903</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -56754,7 +56961,7 @@
       <c r="F6" t="s">
         <v>2974</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -56775,7 +56982,7 @@
       <c r="F7" t="s">
         <v>4265</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>4.5</v>
       </c>
     </row>
@@ -56798,7 +57005,7 @@
       <c r="F8" t="s">
         <v>4335</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>1.05</v>
       </c>
     </row>
@@ -56821,7 +57028,7 @@
       <c r="F9" t="s">
         <v>4500</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>1.73</v>
       </c>
     </row>
@@ -56833,10 +57040,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -56933,7 +57140,7 @@
       <c r="L2" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="9"/>
+      <c r="M2" s="8"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -56969,7 +57176,7 @@
       <c r="L3" t="s">
         <v>2293</v>
       </c>
-      <c r="M3" s="9"/>
+      <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -56999,7 +57206,7 @@
       <c r="L4" t="s">
         <v>2351</v>
       </c>
-      <c r="M4" s="9"/>
+      <c r="M4" s="8"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -57032,7 +57239,7 @@
       <c r="L5" t="s">
         <v>2410</v>
       </c>
-      <c r="M5" s="9"/>
+      <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -57062,7 +57269,7 @@
       <c r="L6" t="s">
         <v>2432</v>
       </c>
-      <c r="M6" s="9"/>
+      <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -57098,7 +57305,7 @@
       <c r="L7" t="s">
         <v>2524</v>
       </c>
-      <c r="M7" s="9"/>
+      <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -57125,7 +57332,7 @@
       <c r="L8" t="s">
         <v>2541</v>
       </c>
-      <c r="M8" s="9"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -57155,7 +57362,7 @@
       <c r="L9" t="s">
         <v>2552</v>
       </c>
-      <c r="M9" s="9"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -57176,7 +57383,7 @@
       <c r="L10" t="s">
         <v>2563</v>
       </c>
-      <c r="M10" s="9"/>
+      <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -57206,7 +57413,7 @@
       <c r="L11" t="s">
         <v>2596</v>
       </c>
-      <c r="M11" s="9"/>
+      <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -57236,7 +57443,7 @@
       <c r="L12" t="s">
         <v>2612</v>
       </c>
-      <c r="M12" s="9"/>
+      <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -57266,7 +57473,7 @@
       <c r="L13" t="s">
         <v>2901</v>
       </c>
-      <c r="M13" s="9"/>
+      <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -57302,7 +57509,7 @@
       <c r="L14" t="s">
         <v>4292</v>
       </c>
-      <c r="M14" s="9"/>
+      <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -57341,7 +57548,7 @@
       <c r="L15" t="s">
         <v>4354</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="8">
         <v>11.15</v>
       </c>
     </row>
@@ -57379,8 +57586,40 @@
       <c r="L16" t="s">
         <v>4546</v>
       </c>
-      <c r="M16" s="9">
+      <c r="M16" s="8">
         <v>0.84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>4560</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4561</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4564</v>
+      </c>
+      <c r="G17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" t="s">
+        <v>2290</v>
+      </c>
+      <c r="J17" t="s">
+        <v>4563</v>
+      </c>
+      <c r="K17" t="s">
+        <v>2409</v>
+      </c>
+      <c r="L17" t="s">
+        <v>4562</v>
+      </c>
+      <c r="M17" s="8">
+        <v>2.27</v>
       </c>
     </row>
   </sheetData>
@@ -57527,7 +57766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -57583,7 +57822,7 @@
       <c r="F2" t="s">
         <v>2317</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -57604,7 +57843,7 @@
       <c r="F3" t="s">
         <v>2321</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -57625,7 +57864,7 @@
       <c r="F4" t="s">
         <v>2327</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -57646,7 +57885,7 @@
       <c r="F5" t="s">
         <v>2338</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -57667,7 +57906,7 @@
       <c r="F6" t="s">
         <v>2462</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -57688,7 +57927,7 @@
       <c r="F7" t="s">
         <v>2481</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -57709,7 +57948,7 @@
       <c r="F8" t="s">
         <v>2482</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -57730,7 +57969,7 @@
       <c r="F9" t="s">
         <v>2527</v>
       </c>
-      <c r="G9" s="9"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -57751,7 +57990,7 @@
       <c r="F10" t="s">
         <v>2529</v>
       </c>
-      <c r="G10" s="9"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -57772,7 +58011,7 @@
       <c r="F11" t="s">
         <v>2527</v>
       </c>
-      <c r="G11" s="9"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -57793,7 +58032,7 @@
       <c r="F12" t="s">
         <v>2559</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -57814,7 +58053,7 @@
       <c r="F13" t="s">
         <v>2721</v>
       </c>
-      <c r="G13" s="9"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -57835,7 +58074,7 @@
       <c r="F14" t="s">
         <v>2726</v>
       </c>
-      <c r="G14" s="9"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -57856,7 +58095,7 @@
       <c r="F15" t="s">
         <v>2920</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -57877,7 +58116,7 @@
       <c r="F16" t="s">
         <v>3371</v>
       </c>
-      <c r="G16" s="9"/>
+      <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -57898,7 +58137,7 @@
       <c r="F17" t="s">
         <v>3374</v>
       </c>
-      <c r="G17" s="9"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -57919,7 +58158,7 @@
       <c r="F18" t="s">
         <v>4263</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <v>6.8</v>
       </c>
     </row>
@@ -57942,7 +58181,7 @@
       <c r="F19" t="s">
         <v>4516</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <v>0.8</v>
       </c>
     </row>
@@ -57965,7 +58204,7 @@
       <c r="F20" t="s">
         <v>4550</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="8">
         <v>6.27</v>
       </c>
     </row>
@@ -57988,7 +58227,7 @@
       <c r="F21" t="s">
         <v>4558</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="8">
         <v>0.68</v>
       </c>
     </row>
@@ -58000,10 +58239,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -58058,7 +58297,7 @@
       <c r="F2" t="s">
         <v>2374</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -58079,7 +58318,7 @@
       <c r="F3" t="s">
         <v>2471</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -58094,7 +58333,7 @@
       <c r="F4" t="s">
         <v>2715</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -58115,7 +58354,7 @@
       <c r="F5" t="s">
         <v>2908</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -58136,7 +58375,7 @@
       <c r="F6" t="s">
         <v>2931</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -58157,7 +58396,7 @@
       <c r="F7" t="s">
         <v>2992</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>3.12</v>
       </c>
     </row>
@@ -58180,7 +58419,7 @@
       <c r="F8" t="s">
         <v>4248</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>26.62</v>
       </c>
     </row>
@@ -58203,7 +58442,7 @@
       <c r="F9" t="s">
         <v>4274</v>
       </c>
-      <c r="G9" s="9"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -58224,7 +58463,7 @@
       <c r="F10" t="s">
         <v>4279</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>0.3</v>
       </c>
     </row>
@@ -58247,8 +58486,31 @@
       <c r="F11" t="s">
         <v>4505</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4586</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4583</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4584</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4587</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4585</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2972</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0.76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issue with Analog.DbLib
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -34899,7 +34899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -57955,8 +57955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add some parts and such
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12359" uniqueCount="4607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12433" uniqueCount="4653">
   <si>
     <t>Part Number</t>
   </si>
@@ -13852,6 +13852,144 @@
   </si>
   <si>
     <t>conn-25x2_0</t>
+  </si>
+  <si>
+    <t>LOGIC-00012</t>
+  </si>
+  <si>
+    <t>Flip-Flop, Dual D-Type, TSSOP-14, SN74LVC74APWRG4</t>
+  </si>
+  <si>
+    <t>SN74LVC74APWRG4</t>
+  </si>
+  <si>
+    <t>SN74LVC74A</t>
+  </si>
+  <si>
+    <t>ANLG-00020</t>
+  </si>
+  <si>
+    <t>Analog Switch, Dual, SPST, SN74LVC2G66DCUR SO-8</t>
+  </si>
+  <si>
+    <t>SN74LVC2G66DCUR</t>
+  </si>
+  <si>
+    <t>SN74LVC2G66</t>
+  </si>
+  <si>
+    <t>MISC-00011</t>
+  </si>
+  <si>
+    <t>555 Timer, NE555DR, SO-8</t>
+  </si>
+  <si>
+    <t>NE555DR</t>
+  </si>
+  <si>
+    <t>NE555</t>
+  </si>
+  <si>
+    <t>CONN-00028</t>
+  </si>
+  <si>
+    <t>Barrel, 2.5x5.5mm</t>
+  </si>
+  <si>
+    <t>CUI</t>
+  </si>
+  <si>
+    <t>PJ-102B</t>
+  </si>
+  <si>
+    <t>BARREL_2.5x5.5MM_0</t>
+  </si>
+  <si>
+    <t>conn-barrel_2.5x5.5MM_0</t>
+  </si>
+  <si>
+    <t>MISC-00012</t>
+  </si>
+  <si>
+    <t>Accel &amp; Gyro, 3-Axis, SPI/I2C</t>
+  </si>
+  <si>
+    <t>STM</t>
+  </si>
+  <si>
+    <t>LSM6DS3TR</t>
+  </si>
+  <si>
+    <t>LGA14</t>
+  </si>
+  <si>
+    <t>LSM6DS3</t>
+  </si>
+  <si>
+    <t>MAG-00095</t>
+  </si>
+  <si>
+    <t>Ind, 33uH, 10%, 20A, Nonstandard</t>
+  </si>
+  <si>
+    <t>20A</t>
+  </si>
+  <si>
+    <t>17mOhm</t>
+  </si>
+  <si>
+    <t>ABRACON</t>
+  </si>
+  <si>
+    <t>AIRD-03-330K</t>
+  </si>
+  <si>
+    <t>ANLG-00021</t>
+  </si>
+  <si>
+    <t>OPA4170AIDR</t>
+  </si>
+  <si>
+    <t>Op Amp, Quad, Rail-Rail, 1.2-MHz, SO-14, 36V</t>
+  </si>
+  <si>
+    <t>OPA4170</t>
+  </si>
+  <si>
+    <t>XSTR-00021</t>
+  </si>
+  <si>
+    <t>XSTR NPN, 2A, 100V, Vce 0.15V, SOT-23</t>
+  </si>
+  <si>
+    <t>490mW</t>
+  </si>
+  <si>
+    <t>NSS1C201LT1G</t>
+  </si>
+  <si>
+    <t>NSS1C200LT1G</t>
+  </si>
+  <si>
+    <t>0.25V</t>
+  </si>
+  <si>
+    <t>0.15V</t>
+  </si>
+  <si>
+    <t>XSTR PNP, 2A, 100V, Vce 0.25V, SOT-23</t>
+  </si>
+  <si>
+    <t>XSTR-00022</t>
+  </si>
+  <si>
+    <t>CONN-00029</t>
+  </si>
+  <si>
+    <t>Header 4x1, 0.1"</t>
+  </si>
+  <si>
+    <t>HDDR_4x1_0</t>
   </si>
 </sst>
 </file>
@@ -32244,7 +32382,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32537,7 +32675,27 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G14" s="8"/>
+      <c r="A14" t="s">
+        <v>4607</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4608</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2290</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4609</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3375</v>
+      </c>
+      <c r="F14" t="s">
+        <v>4610</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0.42</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G15" s="8"/>
@@ -32553,10 +32711,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33363,6 +33521,82 @@
       </c>
       <c r="L22" s="8">
         <v>2.2599999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>4641</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4642</v>
+      </c>
+      <c r="C23" t="s">
+        <v>947</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2109</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4643</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2239</v>
+      </c>
+      <c r="G23" t="s">
+        <v>4647</v>
+      </c>
+      <c r="H23" t="s">
+        <v>2094</v>
+      </c>
+      <c r="I23" t="s">
+        <v>4644</v>
+      </c>
+      <c r="J23" t="s">
+        <v>2184</v>
+      </c>
+      <c r="K23" t="s">
+        <v>2238</v>
+      </c>
+      <c r="L23" s="8">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>4649</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4648</v>
+      </c>
+      <c r="C24" t="s">
+        <v>947</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2109</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4643</v>
+      </c>
+      <c r="F24" t="s">
+        <v>2247</v>
+      </c>
+      <c r="G24" t="s">
+        <v>4646</v>
+      </c>
+      <c r="H24" t="s">
+        <v>2094</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>4645</v>
+      </c>
+      <c r="J24" t="s">
+        <v>2184</v>
+      </c>
+      <c r="K24" t="s">
+        <v>2246</v>
+      </c>
+      <c r="L24" s="8">
+        <v>0.52</v>
       </c>
     </row>
   </sheetData>
@@ -34897,10 +35131,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35780,6 +36014,58 @@
       </c>
       <c r="K29" s="8">
         <v>10.210000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>4619</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4620</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2514</v>
+      </c>
+      <c r="F30">
+        <v>2.5</v>
+      </c>
+      <c r="G30" t="s">
+        <v>4621</v>
+      </c>
+      <c r="H30" t="s">
+        <v>4622</v>
+      </c>
+      <c r="I30" t="s">
+        <v>4623</v>
+      </c>
+      <c r="J30" t="s">
+        <v>4624</v>
+      </c>
+      <c r="K30" s="8">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>4650</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4651</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>4652</v>
+      </c>
+      <c r="J31" t="s">
+        <v>2965</v>
       </c>
     </row>
   </sheetData>
@@ -53547,10 +53833,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M96"/>
+  <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="M98" sqref="M98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -56820,6 +57106,41 @@
       </c>
       <c r="M96" s="8">
         <v>8.85</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>4631</v>
+      </c>
+      <c r="B97" t="s">
+        <v>4632</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="E97" t="s">
+        <v>4633</v>
+      </c>
+      <c r="H97" t="s">
+        <v>4634</v>
+      </c>
+      <c r="I97" t="s">
+        <v>4635</v>
+      </c>
+      <c r="J97" t="s">
+        <v>4636</v>
+      </c>
+      <c r="K97" t="s">
+        <v>4636</v>
+      </c>
+      <c r="L97" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M97" s="8">
+        <v>6.08</v>
       </c>
     </row>
   </sheetData>
@@ -57953,10 +58274,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -58420,6 +58741,52 @@
         <v>0.68</v>
       </c>
     </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>4611</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4612</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2290</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4613</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2320</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4614</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>4637</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4639</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2290</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4638</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2483</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4640</v>
+      </c>
+      <c r="G23" s="8">
+        <v>2.79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -58428,10 +58795,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -58702,6 +59069,52 @@
         <v>0.76</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4615</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4616</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2290</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4617</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2320</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4618</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>4625</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4626</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4627</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4628</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4629</v>
+      </c>
+      <c r="F14" t="s">
+        <v>4630</v>
+      </c>
+      <c r="G14" s="8">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add a few transistors and sw reg IC's
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12433" uniqueCount="4653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12529" uniqueCount="4700">
   <si>
     <t>Part Number</t>
   </si>
@@ -13107,48 +13107,9 @@
     <t>TERM_5.08MM_3X1</t>
   </si>
   <si>
-    <t>0.22µF</t>
-  </si>
-  <si>
     <t>±10%</t>
   </si>
   <si>
-    <t>0.33µF</t>
-  </si>
-  <si>
-    <t>0.47µF</t>
-  </si>
-  <si>
-    <t>0.1µF</t>
-  </si>
-  <si>
-    <t>0.15µF</t>
-  </si>
-  <si>
-    <t>0.39µF</t>
-  </si>
-  <si>
-    <t>0.56µF</t>
-  </si>
-  <si>
-    <t>0.68µF</t>
-  </si>
-  <si>
-    <t>0.12µF</t>
-  </si>
-  <si>
-    <t>0.18µF</t>
-  </si>
-  <si>
-    <t>2.2µF</t>
-  </si>
-  <si>
-    <t>0.022µF</t>
-  </si>
-  <si>
-    <t>0.27µF</t>
-  </si>
-  <si>
     <t>GRM188R71A224KA01D</t>
   </si>
   <si>
@@ -13990,6 +13951,186 @@
   </si>
   <si>
     <t>HDDR_4x1_0</t>
+  </si>
+  <si>
+    <t>MISC-00013</t>
+  </si>
+  <si>
+    <t>Relay, 12V, 16A</t>
+  </si>
+  <si>
+    <t>Omron</t>
+  </si>
+  <si>
+    <t>G2RL-1-E</t>
+  </si>
+  <si>
+    <t>RELAY_G2RL-1-E</t>
+  </si>
+  <si>
+    <t>relay_G2RL-1-E</t>
+  </si>
+  <si>
+    <t>UCTRL-00007</t>
+  </si>
+  <si>
+    <t>Arduino Nano, ATMega328 Dev Board</t>
+  </si>
+  <si>
+    <t>ARDUINO_NANO</t>
+  </si>
+  <si>
+    <t>2.0V</t>
+  </si>
+  <si>
+    <t>75mW</t>
+  </si>
+  <si>
+    <t>Kingbright</t>
+  </si>
+  <si>
+    <t>APA3010EC-GX</t>
+  </si>
+  <si>
+    <t>APA3010</t>
+  </si>
+  <si>
+    <t>LED, Red, 75mW, 30mA</t>
+  </si>
+  <si>
+    <t>LED, Green, 75mW, 30mA</t>
+  </si>
+  <si>
+    <t>2.1V</t>
+  </si>
+  <si>
+    <t>APA3010QGC-GX</t>
+  </si>
+  <si>
+    <t>MISC-00014</t>
+  </si>
+  <si>
+    <t>Switch, SPST, Tactile, Right-Angle</t>
+  </si>
+  <si>
+    <t>Uxcell</t>
+  </si>
+  <si>
+    <t>US-SA-AJD-09203</t>
+  </si>
+  <si>
+    <t>UXCELL_TACT_SWITCH</t>
+  </si>
+  <si>
+    <t>SW_1P1T_1</t>
+  </si>
+  <si>
+    <t>XSTR-00023</t>
+  </si>
+  <si>
+    <t>80V</t>
+  </si>
+  <si>
+    <t>100A</t>
+  </si>
+  <si>
+    <t>XSTR NMOS, 100A, 80V, Vgs 2.7V, SON-Q5B</t>
+  </si>
+  <si>
+    <t>2.7V</t>
+  </si>
+  <si>
+    <t>NMOS</t>
+  </si>
+  <si>
+    <t>195W</t>
+  </si>
+  <si>
+    <t>CSD19502Q5B</t>
+  </si>
+  <si>
+    <t>diode_8</t>
+  </si>
+  <si>
+    <t>MBRB40250TG</t>
+  </si>
+  <si>
+    <t>D2PAK-3_0</t>
+  </si>
+  <si>
+    <t>0.86V</t>
+  </si>
+  <si>
+    <t>Dio Schottky, 40A, 0.86V, 250V, D2PAK, 35ns Reverse Recovery</t>
+  </si>
+  <si>
+    <t>MAG-00096</t>
+  </si>
+  <si>
+    <t>Ind, 15uH, 0.0024, 30A, 7443641500</t>
+  </si>
+  <si>
+    <t>15%</t>
+  </si>
+  <si>
+    <t>30A</t>
+  </si>
+  <si>
+    <t>2.4mOhm</t>
+  </si>
+  <si>
+    <t>WURTH_7443641500</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>0.12uF</t>
+  </si>
+  <si>
+    <t>MAG-00097</t>
+  </si>
+  <si>
+    <t>Ind, 4.7uH, 0.0024, 30A, 7443640470</t>
+  </si>
+  <si>
+    <t>XSTR-00024</t>
+  </si>
+  <si>
+    <t>XSTR NMOS, 100A, 80V, Vgs 2.7V, TO-220AB</t>
+  </si>
+  <si>
+    <t>217W</t>
+  </si>
+  <si>
+    <t>CSD19501KCS</t>
+  </si>
+  <si>
+    <t>n-mosfet_5</t>
+  </si>
+  <si>
+    <t>PWREG-00016</t>
+  </si>
+  <si>
+    <t>REG CNTRL, SW Buck, LM5145</t>
+  </si>
+  <si>
+    <t>6 - 75V</t>
+  </si>
+  <si>
+    <t>0.8 - 60V</t>
+  </si>
+  <si>
+    <t>100kHz-1MHz</t>
+  </si>
+  <si>
+    <t>LM5145RGY</t>
+  </si>
+  <si>
+    <t>VQFN-20_0</t>
+  </si>
+  <si>
+    <t>LM5145</t>
   </si>
 </sst>
 </file>
@@ -14400,7 +14541,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>4523</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -32415,7 +32556,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>4523</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -32653,22 +32794,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4535</v>
+        <v>4522</v>
       </c>
       <c r="B13" t="s">
-        <v>4536</v>
+        <v>4523</v>
       </c>
       <c r="C13" t="s">
         <v>2290</v>
       </c>
       <c r="D13" t="s">
-        <v>4537</v>
+        <v>4524</v>
       </c>
       <c r="E13" t="s">
-        <v>4538</v>
+        <v>4525</v>
       </c>
       <c r="F13" t="s">
-        <v>4539</v>
+        <v>4526</v>
       </c>
       <c r="G13" s="8">
         <v>0.84</v>
@@ -32676,22 +32817,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4607</v>
+        <v>4594</v>
       </c>
       <c r="B14" t="s">
-        <v>4608</v>
+        <v>4595</v>
       </c>
       <c r="C14" t="s">
         <v>2290</v>
       </c>
       <c r="D14" t="s">
-        <v>4609</v>
+        <v>4596</v>
       </c>
       <c r="E14" t="s">
         <v>3375</v>
       </c>
       <c r="F14" t="s">
-        <v>4610</v>
+        <v>4597</v>
       </c>
       <c r="G14" s="8">
         <v>0.42</v>
@@ -32711,10 +32852,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32766,7 +32907,7 @@
         <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>4523</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -33412,7 +33553,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>4519</v>
+        <v>4506</v>
       </c>
       <c r="B20" t="s">
         <v>2419</v>
@@ -33421,10 +33562,10 @@
         <v>2123</v>
       </c>
       <c r="D20" t="s">
-        <v>4520</v>
+        <v>4507</v>
       </c>
       <c r="E20" t="s">
-        <v>4521</v>
+        <v>4508</v>
       </c>
       <c r="F20" t="s">
         <v>2270</v>
@@ -33436,7 +33577,7 @@
         <v>2094</v>
       </c>
       <c r="I20" t="s">
-        <v>4522</v>
+        <v>4509</v>
       </c>
       <c r="J20" t="s">
         <v>2416</v>
@@ -33450,7 +33591,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>4570</v>
+        <v>4557</v>
       </c>
       <c r="B21" t="str">
         <f>CONCATENATE("XSTR ",F21,", ",D21,", ",C21,", Vgs ",G21,", ",LEFT(J21,6))</f>
@@ -33460,10 +33601,10 @@
         <v>947</v>
       </c>
       <c r="D21" t="s">
-        <v>4571</v>
+        <v>4558</v>
       </c>
       <c r="E21" t="s">
-        <v>4572</v>
+        <v>4559</v>
       </c>
       <c r="F21" t="s">
         <v>2270</v>
@@ -33475,13 +33616,13 @@
         <v>2301</v>
       </c>
       <c r="I21" t="s">
-        <v>4573</v>
+        <v>4560</v>
       </c>
       <c r="J21" t="s">
-        <v>4574</v>
+        <v>4561</v>
       </c>
       <c r="K21" t="s">
-        <v>4575</v>
+        <v>4562</v>
       </c>
       <c r="L21" s="8">
         <v>1.36</v>
@@ -33489,7 +33630,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>4588</v>
+        <v>4575</v>
       </c>
       <c r="B22" t="str">
         <f>CONCATENATE("XSTR ",F22,", ",D22,", ",C22,", Vgs ",G22,", ",LEFT(J22,6))</f>
@@ -33499,7 +33640,7 @@
         <v>947</v>
       </c>
       <c r="D22" t="s">
-        <v>4589</v>
+        <v>4576</v>
       </c>
       <c r="F22" t="s">
         <v>2270</v>
@@ -33511,13 +33652,13 @@
         <v>2301</v>
       </c>
       <c r="I22" t="s">
-        <v>4590</v>
+        <v>4577</v>
       </c>
       <c r="J22" t="s">
-        <v>4574</v>
+        <v>4561</v>
       </c>
       <c r="K22" t="s">
-        <v>4575</v>
+        <v>4562</v>
       </c>
       <c r="L22" s="8">
         <v>2.2599999999999998</v>
@@ -33525,10 +33666,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>4641</v>
+        <v>4628</v>
       </c>
       <c r="B23" t="s">
-        <v>4642</v>
+        <v>4629</v>
       </c>
       <c r="C23" t="s">
         <v>947</v>
@@ -33537,19 +33678,19 @@
         <v>2109</v>
       </c>
       <c r="E23" t="s">
-        <v>4643</v>
+        <v>4630</v>
       </c>
       <c r="F23" t="s">
         <v>2239</v>
       </c>
       <c r="G23" t="s">
-        <v>4647</v>
+        <v>4634</v>
       </c>
       <c r="H23" t="s">
         <v>2094</v>
       </c>
       <c r="I23" t="s">
-        <v>4644</v>
+        <v>4631</v>
       </c>
       <c r="J23" t="s">
         <v>2184</v>
@@ -33563,10 +33704,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>4649</v>
+        <v>4636</v>
       </c>
       <c r="B24" t="s">
-        <v>4648</v>
+        <v>4635</v>
       </c>
       <c r="C24" t="s">
         <v>947</v>
@@ -33575,19 +33716,19 @@
         <v>2109</v>
       </c>
       <c r="E24" t="s">
-        <v>4643</v>
+        <v>4630</v>
       </c>
       <c r="F24" t="s">
         <v>2247</v>
       </c>
       <c r="G24" t="s">
-        <v>4646</v>
+        <v>4633</v>
       </c>
       <c r="H24" t="s">
         <v>2094</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>4645</v>
+        <v>4632</v>
       </c>
       <c r="J24" t="s">
         <v>2184</v>
@@ -33597,6 +33738,82 @@
       </c>
       <c r="L24" s="8">
         <v>0.52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>4664</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4667</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4665</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4666</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4670</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4669</v>
+      </c>
+      <c r="G25" t="s">
+        <v>4668</v>
+      </c>
+      <c r="H25" t="s">
+        <v>2290</v>
+      </c>
+      <c r="I25" t="s">
+        <v>4671</v>
+      </c>
+      <c r="J25" t="s">
+        <v>2606</v>
+      </c>
+      <c r="K25" t="s">
+        <v>2600</v>
+      </c>
+      <c r="L25" s="8">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>4687</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4688</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4665</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4666</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4689</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4669</v>
+      </c>
+      <c r="G26" t="s">
+        <v>4668</v>
+      </c>
+      <c r="H26" t="s">
+        <v>2290</v>
+      </c>
+      <c r="I26" t="s">
+        <v>4690</v>
+      </c>
+      <c r="J26" t="s">
+        <v>4561</v>
+      </c>
+      <c r="K26" t="s">
+        <v>4691</v>
+      </c>
+      <c r="L26" s="8">
+        <v>1.97</v>
       </c>
     </row>
   </sheetData>
@@ -33607,10 +33824,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33668,7 +33885,7 @@
         <v>7</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>4523</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -35058,10 +35275,10 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>4526</v>
+        <v>4513</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>4527</v>
+        <v>4514</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>2437</v>
@@ -35070,7 +35287,7 @@
         <v>2951</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>4530</v>
+        <v>4517</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>2511</v>
@@ -35079,10 +35296,10 @@
         <v>2500</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>4529</v>
+        <v>4516</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>4528</v>
+        <v>4515</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>35</v>
@@ -35096,31 +35313,127 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
-        <v>4581</v>
+        <v>4568</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>4576</v>
+        <v>4563</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>4580</v>
+        <v>4567</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>4577</v>
+        <v>4564</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>2433</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>4578</v>
+        <v>4565</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>4582</v>
+        <v>4569</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>4579</v>
+        <v>4566</v>
       </c>
       <c r="M43" s="8">
         <v>5.26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B44" s="2" t="s">
+        <v>4654</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>4649</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>2951</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>4650</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>4287</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>2500</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>4651</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>4652</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>4653</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>2505</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B45" s="2" t="s">
+        <v>4655</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>4656</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>2951</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>4650</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>4287</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>2500</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>4651</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>4657</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>4653</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>2505</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B46" s="2" t="s">
+        <v>4676</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>4675</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>4576</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>2095</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>2094</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>4673</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>4674</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>4672</v>
+      </c>
+      <c r="M46" s="8">
+        <v>2.0099999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -35133,8 +35446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35182,7 +35495,7 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>4523</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -35631,7 +35944,7 @@
         <v>3378</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>4559</v>
+        <v>4546</v>
       </c>
       <c r="I17" t="s">
         <v>3379</v>
@@ -35817,10 +36130,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>4506</v>
+        <v>4493</v>
       </c>
       <c r="B24" t="s">
-        <v>4508</v>
+        <v>4495</v>
       </c>
       <c r="C24" t="s">
         <v>2385</v>
@@ -35841,7 +36154,7 @@
         <v>1861946</v>
       </c>
       <c r="I24" t="s">
-        <v>4511</v>
+        <v>4498</v>
       </c>
       <c r="J24" t="s">
         <v>2386</v>
@@ -35852,10 +36165,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>4507</v>
+        <v>4494</v>
       </c>
       <c r="B25" t="s">
-        <v>4509</v>
+        <v>4496</v>
       </c>
       <c r="C25" t="s">
         <v>2385</v>
@@ -35876,7 +36189,7 @@
         <v>1861933</v>
       </c>
       <c r="I25" t="s">
-        <v>4510</v>
+        <v>4497</v>
       </c>
       <c r="J25" t="s">
         <v>2393</v>
@@ -35887,10 +36200,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>4552</v>
+        <v>4539</v>
       </c>
       <c r="B26" t="s">
-        <v>4553</v>
+        <v>4540</v>
       </c>
       <c r="C26" t="s">
         <v>2385</v>
@@ -35911,7 +36224,7 @@
         <v>1861959</v>
       </c>
       <c r="I26" t="s">
-        <v>4554</v>
+        <v>4541</v>
       </c>
       <c r="J26" t="s">
         <v>2965</v>
@@ -35922,10 +36235,10 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>4591</v>
+        <v>4578</v>
       </c>
       <c r="B27" t="s">
-        <v>4594</v>
+        <v>4581</v>
       </c>
       <c r="C27" t="s">
         <v>2514</v>
@@ -35937,16 +36250,16 @@
         <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>4595</v>
+        <v>4582</v>
       </c>
       <c r="H27" t="s">
-        <v>4596</v>
+        <v>4583</v>
       </c>
       <c r="I27" t="s">
-        <v>4598</v>
+        <v>4585</v>
       </c>
       <c r="J27" t="s">
-        <v>4597</v>
+        <v>4584</v>
       </c>
       <c r="K27" s="8">
         <v>7.32</v>
@@ -35954,10 +36267,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>4592</v>
+        <v>4579</v>
       </c>
       <c r="B28" t="s">
-        <v>4599</v>
+        <v>4586</v>
       </c>
       <c r="C28" t="s">
         <v>2514</v>
@@ -35969,16 +36282,16 @@
         <v>2</v>
       </c>
       <c r="G28" t="s">
-        <v>4595</v>
+        <v>4582</v>
       </c>
       <c r="H28" t="s">
-        <v>4600</v>
+        <v>4587</v>
       </c>
       <c r="I28" t="s">
-        <v>4601</v>
+        <v>4588</v>
       </c>
       <c r="J28" t="s">
-        <v>4602</v>
+        <v>4589</v>
       </c>
       <c r="K28" s="8">
         <v>9.34</v>
@@ -35986,10 +36299,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>4593</v>
+        <v>4580</v>
       </c>
       <c r="B29" t="s">
-        <v>4603</v>
+        <v>4590</v>
       </c>
       <c r="C29" t="s">
         <v>2514</v>
@@ -36001,16 +36314,16 @@
         <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>4595</v>
+        <v>4582</v>
       </c>
       <c r="H29" t="s">
-        <v>4604</v>
+        <v>4591</v>
       </c>
       <c r="I29" t="s">
-        <v>4605</v>
+        <v>4592</v>
       </c>
       <c r="J29" t="s">
-        <v>4606</v>
+        <v>4593</v>
       </c>
       <c r="K29" s="8">
         <v>10.210000000000001</v>
@@ -36018,10 +36331,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>4619</v>
+        <v>4606</v>
       </c>
       <c r="B30" t="s">
-        <v>4620</v>
+        <v>4607</v>
       </c>
       <c r="C30" t="s">
         <v>2514</v>
@@ -36030,16 +36343,16 @@
         <v>2.5</v>
       </c>
       <c r="G30" t="s">
-        <v>4621</v>
+        <v>4608</v>
       </c>
       <c r="H30" t="s">
-        <v>4622</v>
+        <v>4609</v>
       </c>
       <c r="I30" t="s">
-        <v>4623</v>
+        <v>4610</v>
       </c>
       <c r="J30" t="s">
-        <v>4624</v>
+        <v>4611</v>
       </c>
       <c r="K30" s="8">
         <v>0.64</v>
@@ -36047,10 +36360,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>4650</v>
+        <v>4637</v>
       </c>
       <c r="B31" t="s">
-        <v>4651</v>
+        <v>4638</v>
       </c>
       <c r="C31" t="s">
         <v>2399</v>
@@ -36062,7 +36375,7 @@
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>4652</v>
+        <v>4639</v>
       </c>
       <c r="J31" t="s">
         <v>2965</v>
@@ -36079,7 +36392,7 @@
   <dimension ref="A1:K537"/>
   <sheetViews>
     <sheetView topLeftCell="A516" workbookViewId="0">
-      <selection activeCell="J539" sqref="J539"/>
+      <selection activeCell="C533" sqref="C533"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36129,7 +36442,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>4523</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -51776,17 +52089,17 @@
     </row>
     <row r="476" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
-        <v>4432</v>
+        <v>4419</v>
       </c>
       <c r="B476" t="str">
         <f t="shared" si="8"/>
-        <v>CAP, 0.22µF, ±10%, 10V, X7R, 0603</v>
+        <v>CAP, 0.22uF, ±10%, 10V, X7R, 0603</v>
       </c>
       <c r="C476" t="s">
+        <v>1571</v>
+      </c>
+      <c r="D476" t="s">
         <v>4358</v>
-      </c>
-      <c r="D476" t="s">
-        <v>4359</v>
       </c>
       <c r="E476" t="s">
         <v>950</v>
@@ -51798,7 +52111,7 @@
         <v>21</v>
       </c>
       <c r="H476" t="s">
-        <v>4372</v>
+        <v>4359</v>
       </c>
       <c r="I476" t="s">
         <v>35</v>
@@ -51809,17 +52122,17 @@
     </row>
     <row r="477" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
-        <v>4433</v>
+        <v>4420</v>
       </c>
       <c r="B477" t="str">
         <f t="shared" si="8"/>
-        <v>CAP, 0.33µF, ±10%, 16V, X7R, 0603</v>
+        <v>CAP, 0.33uF, ±10%, 16V, X7R, 0603</v>
       </c>
       <c r="C477" t="s">
-        <v>4360</v>
+        <v>1573</v>
       </c>
       <c r="D477" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E477" t="s">
         <v>19</v>
@@ -51831,7 +52144,7 @@
         <v>21</v>
       </c>
       <c r="H477" t="s">
-        <v>4373</v>
+        <v>4360</v>
       </c>
       <c r="I477" t="s">
         <v>35</v>
@@ -51842,17 +52155,17 @@
     </row>
     <row r="478" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A478" t="s">
-        <v>4434</v>
+        <v>4421</v>
       </c>
       <c r="B478" t="str">
         <f t="shared" si="8"/>
-        <v>CAP, 0.47µF, ±10%, 25V, X7R, 0603</v>
+        <v>CAP, 0.47uF, ±10%, 25V, X7R, 0603</v>
       </c>
       <c r="C478" t="s">
-        <v>4361</v>
+        <v>1575</v>
       </c>
       <c r="D478" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E478" t="s">
         <v>27</v>
@@ -51864,7 +52177,7 @@
         <v>21</v>
       </c>
       <c r="H478" t="s">
-        <v>4374</v>
+        <v>4361</v>
       </c>
       <c r="I478" t="s">
         <v>35</v>
@@ -51875,17 +52188,17 @@
     </row>
     <row r="479" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
-        <v>4435</v>
+        <v>4422</v>
       </c>
       <c r="B479" t="str">
         <f t="shared" si="8"/>
-        <v>CAP, 0.1µF, ±10%, 100V, X7R, 0603</v>
+        <v>CAP, 0.1uF, ±10%, 100V, X7R, 0603</v>
       </c>
       <c r="C479" t="s">
-        <v>4362</v>
+        <v>4683</v>
       </c>
       <c r="D479" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E479" t="s">
         <v>947</v>
@@ -51897,7 +52210,7 @@
         <v>21</v>
       </c>
       <c r="H479" t="s">
-        <v>4375</v>
+        <v>4362</v>
       </c>
       <c r="I479" t="s">
         <v>35</v>
@@ -51908,7 +52221,7 @@
     </row>
     <row r="480" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
-        <v>4436</v>
+        <v>4423</v>
       </c>
       <c r="B480" t="str">
         <f t="shared" si="8"/>
@@ -51918,7 +52231,7 @@
         <v>933</v>
       </c>
       <c r="D480" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E480" t="s">
         <v>948</v>
@@ -51930,7 +52243,7 @@
         <v>21</v>
       </c>
       <c r="H480" t="s">
-        <v>4376</v>
+        <v>4363</v>
       </c>
       <c r="I480" t="s">
         <v>35</v>
@@ -51941,7 +52254,7 @@
     </row>
     <row r="481" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
-        <v>4437</v>
+        <v>4424</v>
       </c>
       <c r="B481" t="str">
         <f t="shared" si="8"/>
@@ -51951,7 +52264,7 @@
         <v>937</v>
       </c>
       <c r="D481" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E481" t="s">
         <v>948</v>
@@ -51963,7 +52276,7 @@
         <v>21</v>
       </c>
       <c r="H481" t="s">
-        <v>4377</v>
+        <v>4364</v>
       </c>
       <c r="I481" t="s">
         <v>35</v>
@@ -51974,7 +52287,7 @@
     </row>
     <row r="482" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
-        <v>4438</v>
+        <v>4425</v>
       </c>
       <c r="B482" t="str">
         <f t="shared" si="8"/>
@@ -51984,7 +52297,7 @@
         <v>2820</v>
       </c>
       <c r="D482" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E482" t="s">
         <v>947</v>
@@ -51996,7 +52309,7 @@
         <v>21</v>
       </c>
       <c r="H482" t="s">
-        <v>4378</v>
+        <v>4365</v>
       </c>
       <c r="I482" t="s">
         <v>35</v>
@@ -52007,7 +52320,7 @@
     </row>
     <row r="483" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
-        <v>4439</v>
+        <v>4426</v>
       </c>
       <c r="B483" t="str">
         <f t="shared" si="8"/>
@@ -52017,7 +52330,7 @@
         <v>926</v>
       </c>
       <c r="D483" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E483" t="s">
         <v>948</v>
@@ -52029,7 +52342,7 @@
         <v>21</v>
       </c>
       <c r="H483" t="s">
-        <v>4379</v>
+        <v>4366</v>
       </c>
       <c r="I483" t="s">
         <v>35</v>
@@ -52040,17 +52353,17 @@
     </row>
     <row r="484" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
-        <v>4440</v>
+        <v>4427</v>
       </c>
       <c r="B484" t="str">
         <f t="shared" si="8"/>
-        <v>CAP, 0.15µF, ±10%, 16V, X7R, 0603</v>
+        <v>CAP, 0.15uF, ±10%, 16V, X7R, 0603</v>
       </c>
       <c r="C484" t="s">
-        <v>4363</v>
+        <v>1569</v>
       </c>
       <c r="D484" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E484" t="s">
         <v>19</v>
@@ -52062,7 +52375,7 @@
         <v>21</v>
       </c>
       <c r="H484" t="s">
-        <v>4380</v>
+        <v>4367</v>
       </c>
       <c r="I484" t="s">
         <v>35</v>
@@ -52073,17 +52386,17 @@
     </row>
     <row r="485" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
-        <v>4441</v>
+        <v>4428</v>
       </c>
       <c r="B485" t="str">
         <f t="shared" si="8"/>
-        <v>CAP, 0.47µF, ±10%, 6.3V, X7R, 0603</v>
+        <v>CAP, 0.47uF, ±10%, 6.3V, X7R, 0603</v>
       </c>
       <c r="C485" t="s">
-        <v>4361</v>
+        <v>1575</v>
       </c>
       <c r="D485" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E485" t="s">
         <v>952</v>
@@ -52095,7 +52408,7 @@
         <v>21</v>
       </c>
       <c r="H485" t="s">
-        <v>4381</v>
+        <v>4368</v>
       </c>
       <c r="I485" t="s">
         <v>35</v>
@@ -52106,17 +52419,17 @@
     </row>
     <row r="486" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A486" t="s">
-        <v>4442</v>
+        <v>4429</v>
       </c>
       <c r="B486" t="str">
         <f t="shared" si="8"/>
-        <v>CAP, 0.47µF, ±10%, 10V, X7R, 0603</v>
+        <v>CAP, 0.47uF, ±10%, 10V, X7R, 0603</v>
       </c>
       <c r="C486" t="s">
-        <v>4361</v>
+        <v>1575</v>
       </c>
       <c r="D486" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E486" t="s">
         <v>950</v>
@@ -52128,7 +52441,7 @@
         <v>21</v>
       </c>
       <c r="H486" t="s">
-        <v>4382</v>
+        <v>4369</v>
       </c>
       <c r="I486" t="s">
         <v>35</v>
@@ -52139,17 +52452,17 @@
     </row>
     <row r="487" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
-        <v>4443</v>
+        <v>4430</v>
       </c>
       <c r="B487" t="str">
         <f t="shared" si="8"/>
-        <v>CAP, 0.33µF, ±10%, 10V, X7R, 0603</v>
+        <v>CAP, 0.33uF, ±10%, 10V, X7R, 0603</v>
       </c>
       <c r="C487" t="s">
-        <v>4360</v>
+        <v>1573</v>
       </c>
       <c r="D487" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E487" t="s">
         <v>950</v>
@@ -52161,7 +52474,7 @@
         <v>21</v>
       </c>
       <c r="H487" t="s">
-        <v>4383</v>
+        <v>4370</v>
       </c>
       <c r="I487" t="s">
         <v>35</v>
@@ -52172,17 +52485,17 @@
     </row>
     <row r="488" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A488" t="s">
-        <v>4444</v>
+        <v>4431</v>
       </c>
       <c r="B488" t="str">
         <f t="shared" si="8"/>
-        <v>CAP, 0.39µF, ±10%, 16V, X7R, 0603</v>
+        <v>CAP, 0.39uF, ±10%, 16V, X7R, 0603</v>
       </c>
       <c r="C488" t="s">
-        <v>4364</v>
+        <v>1574</v>
       </c>
       <c r="D488" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E488" t="s">
         <v>19</v>
@@ -52194,7 +52507,7 @@
         <v>21</v>
       </c>
       <c r="H488" t="s">
-        <v>4384</v>
+        <v>4371</v>
       </c>
       <c r="I488" t="s">
         <v>35</v>
@@ -52205,17 +52518,17 @@
     </row>
     <row r="489" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A489" t="s">
-        <v>4445</v>
+        <v>4432</v>
       </c>
       <c r="B489" t="str">
         <f t="shared" si="8"/>
-        <v>CAP, 0.56µF, ±10%, 10V, X7R, 0603</v>
+        <v>CAP, 0.56uF, ±10%, 10V, X7R, 0603</v>
       </c>
       <c r="C489" t="s">
-        <v>4365</v>
+        <v>1576</v>
       </c>
       <c r="D489" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E489" t="s">
         <v>950</v>
@@ -52227,7 +52540,7 @@
         <v>21</v>
       </c>
       <c r="H489" t="s">
-        <v>4385</v>
+        <v>4372</v>
       </c>
       <c r="I489" t="s">
         <v>35</v>
@@ -52238,7 +52551,7 @@
     </row>
     <row r="490" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A490" t="s">
-        <v>4446</v>
+        <v>4433</v>
       </c>
       <c r="B490" t="str">
         <f t="shared" si="8"/>
@@ -52248,7 +52561,7 @@
         <v>935</v>
       </c>
       <c r="D490" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E490" t="s">
         <v>948</v>
@@ -52260,7 +52573,7 @@
         <v>21</v>
       </c>
       <c r="H490" t="s">
-        <v>4386</v>
+        <v>4373</v>
       </c>
       <c r="I490" t="s">
         <v>35</v>
@@ -52271,7 +52584,7 @@
     </row>
     <row r="491" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
-        <v>4447</v>
+        <v>4434</v>
       </c>
       <c r="B491" t="str">
         <f t="shared" si="8"/>
@@ -52281,7 +52594,7 @@
         <v>929</v>
       </c>
       <c r="D491" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E491" t="s">
         <v>948</v>
@@ -52293,7 +52606,7 @@
         <v>21</v>
       </c>
       <c r="H491" t="s">
-        <v>4387</v>
+        <v>4374</v>
       </c>
       <c r="I491" t="s">
         <v>35</v>
@@ -52304,7 +52617,7 @@
     </row>
     <row r="492" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
-        <v>4448</v>
+        <v>4435</v>
       </c>
       <c r="B492" t="str">
         <f t="shared" si="8"/>
@@ -52314,7 +52627,7 @@
         <v>931</v>
       </c>
       <c r="D492" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E492" t="s">
         <v>948</v>
@@ -52326,7 +52639,7 @@
         <v>21</v>
       </c>
       <c r="H492" t="s">
-        <v>4388</v>
+        <v>4375</v>
       </c>
       <c r="I492" t="s">
         <v>35</v>
@@ -52337,7 +52650,7 @@
     </row>
     <row r="493" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
-        <v>4449</v>
+        <v>4436</v>
       </c>
       <c r="B493" t="str">
         <f t="shared" si="8"/>
@@ -52347,7 +52660,7 @@
         <v>937</v>
       </c>
       <c r="D493" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E493" t="s">
         <v>949</v>
@@ -52359,7 +52672,7 @@
         <v>21</v>
       </c>
       <c r="H493" t="s">
-        <v>4389</v>
+        <v>4376</v>
       </c>
       <c r="I493" t="s">
         <v>35</v>
@@ -52370,7 +52683,7 @@
     </row>
     <row r="494" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
-        <v>4450</v>
+        <v>4437</v>
       </c>
       <c r="B494" t="str">
         <f t="shared" si="8"/>
@@ -52380,7 +52693,7 @@
         <v>926</v>
       </c>
       <c r="D494" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E494" t="s">
         <v>947</v>
@@ -52392,7 +52705,7 @@
         <v>21</v>
       </c>
       <c r="H494" t="s">
-        <v>4390</v>
+        <v>4377</v>
       </c>
       <c r="I494" t="s">
         <v>35</v>
@@ -52403,17 +52716,17 @@
     </row>
     <row r="495" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
-        <v>4451</v>
+        <v>4438</v>
       </c>
       <c r="B495" t="str">
         <f t="shared" si="8"/>
-        <v>CAP, 0.68µF, ±10%, 10V, X7R, 0603</v>
+        <v>CAP, 0.68uF, ±10%, 10V, X7R, 0603</v>
       </c>
       <c r="C495" t="s">
-        <v>4366</v>
+        <v>1577</v>
       </c>
       <c r="D495" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E495" t="s">
         <v>950</v>
@@ -52425,7 +52738,7 @@
         <v>21</v>
       </c>
       <c r="H495" t="s">
-        <v>4391</v>
+        <v>4378</v>
       </c>
       <c r="I495" t="s">
         <v>35</v>
@@ -52436,17 +52749,17 @@
     </row>
     <row r="496" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
-        <v>4452</v>
+        <v>4439</v>
       </c>
       <c r="B496" t="str">
         <f t="shared" si="8"/>
-        <v>CAP, 0.22µF, ±10%, 16V, X7R, 0603</v>
+        <v>CAP, 0.22uF, ±10%, 16V, X7R, 0603</v>
       </c>
       <c r="C496" t="s">
+        <v>1571</v>
+      </c>
+      <c r="D496" t="s">
         <v>4358</v>
-      </c>
-      <c r="D496" t="s">
-        <v>4359</v>
       </c>
       <c r="E496" t="s">
         <v>19</v>
@@ -52458,7 +52771,7 @@
         <v>21</v>
       </c>
       <c r="H496" t="s">
-        <v>4392</v>
+        <v>4379</v>
       </c>
       <c r="I496" t="s">
         <v>35</v>
@@ -52469,17 +52782,17 @@
     </row>
     <row r="497" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
-        <v>4453</v>
+        <v>4440</v>
       </c>
       <c r="B497" t="str">
         <f t="shared" si="8"/>
-        <v>CAP, 0.22µF, ±10%, 6.3V, X7R, 0603</v>
+        <v>CAP, 0.22uF, ±10%, 6.3V, X7R, 0603</v>
       </c>
       <c r="C497" t="s">
+        <v>1571</v>
+      </c>
+      <c r="D497" t="s">
         <v>4358</v>
-      </c>
-      <c r="D497" t="s">
-        <v>4359</v>
       </c>
       <c r="E497" t="s">
         <v>952</v>
@@ -52491,7 +52804,7 @@
         <v>21</v>
       </c>
       <c r="H497" t="s">
-        <v>4393</v>
+        <v>4380</v>
       </c>
       <c r="I497" t="s">
         <v>35</v>
@@ -52502,17 +52815,17 @@
     </row>
     <row r="498" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
-        <v>4454</v>
+        <v>4441</v>
       </c>
       <c r="B498" t="str">
         <f t="shared" si="8"/>
-        <v>CAP, 0.47µF, ±10%, 25V, X7R, 0603</v>
+        <v>CAP, 0.47uF, ±10%, 25V, X7R, 0603</v>
       </c>
       <c r="C498" t="s">
-        <v>4361</v>
+        <v>1575</v>
       </c>
       <c r="D498" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E498" t="s">
         <v>27</v>
@@ -52524,7 +52837,7 @@
         <v>21</v>
       </c>
       <c r="H498" t="s">
-        <v>4394</v>
+        <v>4381</v>
       </c>
       <c r="I498" t="s">
         <v>35</v>
@@ -52535,7 +52848,7 @@
     </row>
     <row r="499" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
-        <v>4455</v>
+        <v>4442</v>
       </c>
       <c r="B499" t="str">
         <f t="shared" si="8"/>
@@ -52545,7 +52858,7 @@
         <v>930</v>
       </c>
       <c r="D499" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E499" t="s">
         <v>947</v>
@@ -52557,7 +52870,7 @@
         <v>21</v>
       </c>
       <c r="H499" t="s">
-        <v>4395</v>
+        <v>4382</v>
       </c>
       <c r="I499" t="s">
         <v>35</v>
@@ -52568,7 +52881,7 @@
     </row>
     <row r="500" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
-        <v>4456</v>
+        <v>4443</v>
       </c>
       <c r="B500" t="str">
         <f t="shared" si="8"/>
@@ -52578,7 +52891,7 @@
         <v>926</v>
       </c>
       <c r="D500" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E500" t="s">
         <v>949</v>
@@ -52590,7 +52903,7 @@
         <v>21</v>
       </c>
       <c r="H500" t="s">
-        <v>4396</v>
+        <v>4383</v>
       </c>
       <c r="I500" t="s">
         <v>35</v>
@@ -52601,7 +52914,7 @@
     </row>
     <row r="501" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
-        <v>4457</v>
+        <v>4444</v>
       </c>
       <c r="B501" t="str">
         <f t="shared" si="8"/>
@@ -52611,7 +52924,7 @@
         <v>928</v>
       </c>
       <c r="D501" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E501" t="s">
         <v>947</v>
@@ -52623,7 +52936,7 @@
         <v>21</v>
       </c>
       <c r="H501" t="s">
-        <v>4397</v>
+        <v>4384</v>
       </c>
       <c r="I501" t="s">
         <v>35</v>
@@ -52634,7 +52947,7 @@
     </row>
     <row r="502" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
-        <v>4458</v>
+        <v>4445</v>
       </c>
       <c r="B502" t="str">
         <f t="shared" si="8"/>
@@ -52644,7 +52957,7 @@
         <v>935</v>
       </c>
       <c r="D502" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E502" t="s">
         <v>947</v>
@@ -52656,7 +52969,7 @@
         <v>21</v>
       </c>
       <c r="H502" t="s">
-        <v>4398</v>
+        <v>4385</v>
       </c>
       <c r="I502" t="s">
         <v>35</v>
@@ -52667,7 +52980,7 @@
     </row>
     <row r="503" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
-        <v>4459</v>
+        <v>4446</v>
       </c>
       <c r="B503" t="str">
         <f t="shared" ref="B503:B537" si="9">CONCATENATE("CAP",", ",C503,", ",D503,", ",E503,", ",F503,", 0603")</f>
@@ -52677,7 +52990,7 @@
         <v>929</v>
       </c>
       <c r="D503" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E503" t="s">
         <v>947</v>
@@ -52689,7 +53002,7 @@
         <v>21</v>
       </c>
       <c r="H503" t="s">
-        <v>4399</v>
+        <v>4386</v>
       </c>
       <c r="I503" t="s">
         <v>35</v>
@@ -52700,7 +53013,7 @@
     </row>
     <row r="504" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
-        <v>4460</v>
+        <v>4447</v>
       </c>
       <c r="B504" t="str">
         <f t="shared" si="9"/>
@@ -52710,7 +53023,7 @@
         <v>943</v>
       </c>
       <c r="D504" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E504" t="s">
         <v>947</v>
@@ -52722,7 +53035,7 @@
         <v>21</v>
       </c>
       <c r="H504" t="s">
-        <v>4400</v>
+        <v>4387</v>
       </c>
       <c r="I504" t="s">
         <v>35</v>
@@ -52733,7 +53046,7 @@
     </row>
     <row r="505" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
-        <v>4461</v>
+        <v>4448</v>
       </c>
       <c r="B505" t="str">
         <f t="shared" si="9"/>
@@ -52743,7 +53056,7 @@
         <v>942</v>
       </c>
       <c r="D505" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E505" t="s">
         <v>947</v>
@@ -52755,7 +53068,7 @@
         <v>21</v>
       </c>
       <c r="H505" t="s">
-        <v>4401</v>
+        <v>4388</v>
       </c>
       <c r="I505" t="s">
         <v>35</v>
@@ -52766,7 +53079,7 @@
     </row>
     <row r="506" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
-        <v>4462</v>
+        <v>4449</v>
       </c>
       <c r="B506" t="str">
         <f t="shared" si="9"/>
@@ -52776,7 +53089,7 @@
         <v>929</v>
       </c>
       <c r="D506" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E506" t="s">
         <v>949</v>
@@ -52788,7 +53101,7 @@
         <v>21</v>
       </c>
       <c r="H506" t="s">
-        <v>4402</v>
+        <v>4389</v>
       </c>
       <c r="I506" t="s">
         <v>35</v>
@@ -52799,17 +53112,17 @@
     </row>
     <row r="507" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
-        <v>4463</v>
+        <v>4450</v>
       </c>
       <c r="B507" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.12µF, ±10%, 25V, X7R, 0603</v>
+        <v>CAP, 0.12uF, ±10%, 25V, X7R, 0603</v>
       </c>
       <c r="C507" t="s">
-        <v>4367</v>
+        <v>4684</v>
       </c>
       <c r="D507" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E507" t="s">
         <v>27</v>
@@ -52821,7 +53134,7 @@
         <v>21</v>
       </c>
       <c r="H507" t="s">
-        <v>4403</v>
+        <v>4390</v>
       </c>
       <c r="I507" t="s">
         <v>35</v>
@@ -52832,17 +53145,17 @@
     </row>
     <row r="508" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
-        <v>4464</v>
+        <v>4451</v>
       </c>
       <c r="B508" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.18µF, ±10%, 10V, X7R, 0603</v>
+        <v>CAP, 0.18uF, ±10%, 10V, X7R, 0603</v>
       </c>
       <c r="C508" t="s">
-        <v>4368</v>
+        <v>1570</v>
       </c>
       <c r="D508" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E508" t="s">
         <v>950</v>
@@ -52854,7 +53167,7 @@
         <v>21</v>
       </c>
       <c r="H508" t="s">
-        <v>4404</v>
+        <v>4391</v>
       </c>
       <c r="I508" t="s">
         <v>35</v>
@@ -52865,17 +53178,17 @@
     </row>
     <row r="509" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
-        <v>4465</v>
+        <v>4452</v>
       </c>
       <c r="B509" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.47µF, ±10%, 16V, X7R, 0603</v>
+        <v>CAP, 0.47uF, ±10%, 16V, X7R, 0603</v>
       </c>
       <c r="C509" t="s">
-        <v>4361</v>
+        <v>1575</v>
       </c>
       <c r="D509" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E509" t="s">
         <v>19</v>
@@ -52887,7 +53200,7 @@
         <v>21</v>
       </c>
       <c r="H509" t="s">
-        <v>4405</v>
+        <v>4392</v>
       </c>
       <c r="I509" t="s">
         <v>35</v>
@@ -52898,7 +53211,7 @@
     </row>
     <row r="510" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
-        <v>4466</v>
+        <v>4453</v>
       </c>
       <c r="B510" t="str">
         <f t="shared" si="9"/>
@@ -52908,7 +53221,7 @@
         <v>927</v>
       </c>
       <c r="D510" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E510" t="s">
         <v>948</v>
@@ -52920,7 +53233,7 @@
         <v>21</v>
       </c>
       <c r="H510" t="s">
-        <v>4406</v>
+        <v>4393</v>
       </c>
       <c r="I510" t="s">
         <v>35</v>
@@ -52931,7 +53244,7 @@
     </row>
     <row r="511" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
-        <v>4467</v>
+        <v>4454</v>
       </c>
       <c r="B511" t="str">
         <f t="shared" si="9"/>
@@ -52941,7 +53254,7 @@
         <v>933</v>
       </c>
       <c r="D511" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E511" t="s">
         <v>947</v>
@@ -52953,7 +53266,7 @@
         <v>21</v>
       </c>
       <c r="H511" t="s">
-        <v>4407</v>
+        <v>4394</v>
       </c>
       <c r="I511" t="s">
         <v>35</v>
@@ -52964,17 +53277,17 @@
     </row>
     <row r="512" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A512" t="s">
-        <v>4468</v>
+        <v>4455</v>
       </c>
       <c r="B512" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.22µF, ±10%, 16V, X7R, 0603</v>
+        <v>CAP, 0.22uF, ±10%, 16V, X7R, 0603</v>
       </c>
       <c r="C512" t="s">
+        <v>1571</v>
+      </c>
+      <c r="D512" t="s">
         <v>4358</v>
-      </c>
-      <c r="D512" t="s">
-        <v>4359</v>
       </c>
       <c r="E512" t="s">
         <v>19</v>
@@ -52986,7 +53299,7 @@
         <v>21</v>
       </c>
       <c r="H512" t="s">
-        <v>4408</v>
+        <v>4395</v>
       </c>
       <c r="I512" t="s">
         <v>35</v>
@@ -52997,17 +53310,17 @@
     </row>
     <row r="513" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
-        <v>4469</v>
+        <v>4456</v>
       </c>
       <c r="B513" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.22µF, ±10%, 25V, X7R, 0603</v>
+        <v>CAP, 0.22uF, ±10%, 25V, X7R, 0603</v>
       </c>
       <c r="C513" t="s">
+        <v>1571</v>
+      </c>
+      <c r="D513" t="s">
         <v>4358</v>
-      </c>
-      <c r="D513" t="s">
-        <v>4359</v>
       </c>
       <c r="E513" t="s">
         <v>27</v>
@@ -53019,7 +53332,7 @@
         <v>21</v>
       </c>
       <c r="H513" t="s">
-        <v>4409</v>
+        <v>4396</v>
       </c>
       <c r="I513" t="s">
         <v>35</v>
@@ -53030,17 +53343,17 @@
     </row>
     <row r="514" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
-        <v>4470</v>
+        <v>4457</v>
       </c>
       <c r="B514" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 2.2µF, ±10%, 10V, X7R, 0603</v>
+        <v>CAP, 2.2uF, ±10%, 10V, X7R, 0603</v>
       </c>
       <c r="C514" t="s">
-        <v>4369</v>
+        <v>1581</v>
       </c>
       <c r="D514" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E514" t="s">
         <v>950</v>
@@ -53052,7 +53365,7 @@
         <v>21</v>
       </c>
       <c r="H514" t="s">
-        <v>4410</v>
+        <v>4397</v>
       </c>
       <c r="I514" t="s">
         <v>35</v>
@@ -53063,7 +53376,7 @@
     </row>
     <row r="515" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
-        <v>4471</v>
+        <v>4458</v>
       </c>
       <c r="B515" t="str">
         <f t="shared" si="9"/>
@@ -53073,7 +53386,7 @@
         <v>937</v>
       </c>
       <c r="D515" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E515" t="s">
         <v>947</v>
@@ -53085,7 +53398,7 @@
         <v>21</v>
       </c>
       <c r="H515" t="s">
-        <v>4411</v>
+        <v>4398</v>
       </c>
       <c r="I515" t="s">
         <v>35</v>
@@ -53096,7 +53409,7 @@
     </row>
     <row r="516" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
-        <v>4472</v>
+        <v>4459</v>
       </c>
       <c r="B516" t="str">
         <f t="shared" si="9"/>
@@ -53106,7 +53419,7 @@
         <v>939</v>
       </c>
       <c r="D516" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E516" t="s">
         <v>947</v>
@@ -53118,7 +53431,7 @@
         <v>21</v>
       </c>
       <c r="H516" t="s">
-        <v>4412</v>
+        <v>4399</v>
       </c>
       <c r="I516" t="s">
         <v>35</v>
@@ -53129,7 +53442,7 @@
     </row>
     <row r="517" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A517" t="s">
-        <v>4473</v>
+        <v>4460</v>
       </c>
       <c r="B517" t="str">
         <f t="shared" si="9"/>
@@ -53139,7 +53452,7 @@
         <v>934</v>
       </c>
       <c r="D517" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E517" t="s">
         <v>947</v>
@@ -53151,7 +53464,7 @@
         <v>21</v>
       </c>
       <c r="H517" t="s">
-        <v>4413</v>
+        <v>4400</v>
       </c>
       <c r="I517" t="s">
         <v>35</v>
@@ -53162,7 +53475,7 @@
     </row>
     <row r="518" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A518" t="s">
-        <v>4474</v>
+        <v>4461</v>
       </c>
       <c r="B518" t="str">
         <f t="shared" si="9"/>
@@ -53172,7 +53485,7 @@
         <v>941</v>
       </c>
       <c r="D518" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E518" t="s">
         <v>947</v>
@@ -53184,7 +53497,7 @@
         <v>21</v>
       </c>
       <c r="H518" t="s">
-        <v>4414</v>
+        <v>4401</v>
       </c>
       <c r="I518" t="s">
         <v>35</v>
@@ -53195,7 +53508,7 @@
     </row>
     <row r="519" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A519" t="s">
-        <v>4475</v>
+        <v>4462</v>
       </c>
       <c r="B519" t="str">
         <f t="shared" si="9"/>
@@ -53205,7 +53518,7 @@
         <v>927</v>
       </c>
       <c r="D519" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E519" t="s">
         <v>947</v>
@@ -53217,7 +53530,7 @@
         <v>21</v>
       </c>
       <c r="H519" t="s">
-        <v>4415</v>
+        <v>4402</v>
       </c>
       <c r="I519" t="s">
         <v>35</v>
@@ -53228,7 +53541,7 @@
     </row>
     <row r="520" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A520" t="s">
-        <v>4476</v>
+        <v>4463</v>
       </c>
       <c r="B520" t="str">
         <f t="shared" si="9"/>
@@ -53238,7 +53551,7 @@
         <v>931</v>
       </c>
       <c r="D520" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E520" t="s">
         <v>947</v>
@@ -53250,7 +53563,7 @@
         <v>21</v>
       </c>
       <c r="H520" t="s">
-        <v>4416</v>
+        <v>4403</v>
       </c>
       <c r="I520" t="s">
         <v>35</v>
@@ -53261,7 +53574,7 @@
     </row>
     <row r="521" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A521" t="s">
-        <v>4477</v>
+        <v>4464</v>
       </c>
       <c r="B521" t="str">
         <f t="shared" si="9"/>
@@ -53271,7 +53584,7 @@
         <v>932</v>
       </c>
       <c r="D521" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E521" t="s">
         <v>947</v>
@@ -53283,7 +53596,7 @@
         <v>21</v>
       </c>
       <c r="H521" t="s">
-        <v>4417</v>
+        <v>4404</v>
       </c>
       <c r="I521" t="s">
         <v>35</v>
@@ -53294,7 +53607,7 @@
     </row>
     <row r="522" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A522" t="s">
-        <v>4478</v>
+        <v>4465</v>
       </c>
       <c r="B522" t="str">
         <f t="shared" si="9"/>
@@ -53304,7 +53617,7 @@
         <v>944</v>
       </c>
       <c r="D522" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E522" t="s">
         <v>947</v>
@@ -53316,7 +53629,7 @@
         <v>21</v>
       </c>
       <c r="H522" t="s">
-        <v>4418</v>
+        <v>4405</v>
       </c>
       <c r="I522" t="s">
         <v>35</v>
@@ -53327,7 +53640,7 @@
     </row>
     <row r="523" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A523" t="s">
-        <v>4479</v>
+        <v>4466</v>
       </c>
       <c r="B523" t="str">
         <f t="shared" si="9"/>
@@ -53337,7 +53650,7 @@
         <v>933</v>
       </c>
       <c r="D523" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E523" t="s">
         <v>949</v>
@@ -53349,7 +53662,7 @@
         <v>21</v>
       </c>
       <c r="H523" t="s">
-        <v>4419</v>
+        <v>4406</v>
       </c>
       <c r="I523" t="s">
         <v>35</v>
@@ -53360,17 +53673,17 @@
     </row>
     <row r="524" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A524" t="s">
-        <v>4480</v>
+        <v>4467</v>
       </c>
       <c r="B524" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.15µF, ±10%, 10V, X7R, 0603</v>
+        <v>CAP, 0.15uF, ±10%, 10V, X7R, 0603</v>
       </c>
       <c r="C524" t="s">
-        <v>4363</v>
+        <v>1569</v>
       </c>
       <c r="D524" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E524" t="s">
         <v>950</v>
@@ -53382,7 +53695,7 @@
         <v>21</v>
       </c>
       <c r="H524" t="s">
-        <v>4420</v>
+        <v>4407</v>
       </c>
       <c r="I524" t="s">
         <v>35</v>
@@ -53393,17 +53706,17 @@
     </row>
     <row r="525" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A525" t="s">
-        <v>4481</v>
+        <v>4468</v>
       </c>
       <c r="B525" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.12µF, ±10%, 16V, X7R, 0603</v>
+        <v>CAP, 0.12uF, ±10%, 16V, X7R, 0603</v>
       </c>
       <c r="C525" t="s">
-        <v>4367</v>
+        <v>4684</v>
       </c>
       <c r="D525" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E525" t="s">
         <v>19</v>
@@ -53415,7 +53728,7 @@
         <v>21</v>
       </c>
       <c r="H525" t="s">
-        <v>4421</v>
+        <v>4408</v>
       </c>
       <c r="I525" t="s">
         <v>35</v>
@@ -53426,17 +53739,17 @@
     </row>
     <row r="526" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A526" t="s">
-        <v>4482</v>
+        <v>4469</v>
       </c>
       <c r="B526" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.022µF, ±10%, 100V, X7R, 0603</v>
+        <v>CAP, 0.022uF, ±10%, 100V, X7R, 0603</v>
       </c>
       <c r="C526" t="s">
-        <v>4370</v>
+        <v>1562</v>
       </c>
       <c r="D526" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E526" t="s">
         <v>947</v>
@@ -53448,7 +53761,7 @@
         <v>21</v>
       </c>
       <c r="H526" t="s">
-        <v>4422</v>
+        <v>4409</v>
       </c>
       <c r="I526" t="s">
         <v>35</v>
@@ -53459,17 +53772,17 @@
     </row>
     <row r="527" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A527" t="s">
-        <v>4483</v>
+        <v>4470</v>
       </c>
       <c r="B527" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.18µF, ±10%, 16V, X7R, 0603</v>
+        <v>CAP, 0.18uF, ±10%, 16V, X7R, 0603</v>
       </c>
       <c r="C527" t="s">
-        <v>4368</v>
+        <v>1570</v>
       </c>
       <c r="D527" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E527" t="s">
         <v>19</v>
@@ -53481,7 +53794,7 @@
         <v>21</v>
       </c>
       <c r="H527" t="s">
-        <v>4423</v>
+        <v>4410</v>
       </c>
       <c r="I527" t="s">
         <v>35</v>
@@ -53492,17 +53805,17 @@
     </row>
     <row r="528" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A528" t="s">
-        <v>4484</v>
+        <v>4471</v>
       </c>
       <c r="B528" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.15µF, ±10%, 25V, X7R, 0603</v>
+        <v>CAP, 0.15uF, ±10%, 25V, X7R, 0603</v>
       </c>
       <c r="C528" t="s">
-        <v>4363</v>
+        <v>1569</v>
       </c>
       <c r="D528" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E528" t="s">
         <v>27</v>
@@ -53514,7 +53827,7 @@
         <v>21</v>
       </c>
       <c r="H528" t="s">
-        <v>4424</v>
+        <v>4411</v>
       </c>
       <c r="I528" t="s">
         <v>35</v>
@@ -53525,17 +53838,17 @@
     </row>
     <row r="529" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A529" t="s">
-        <v>4485</v>
+        <v>4472</v>
       </c>
       <c r="B529" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.22µF, ±10%, 10V, X7R, 0603</v>
+        <v>CAP, 0.22uF, ±10%, 10V, X7R, 0603</v>
       </c>
       <c r="C529" t="s">
+        <v>1571</v>
+      </c>
+      <c r="D529" t="s">
         <v>4358</v>
-      </c>
-      <c r="D529" t="s">
-        <v>4359</v>
       </c>
       <c r="E529" t="s">
         <v>950</v>
@@ -53547,7 +53860,7 @@
         <v>21</v>
       </c>
       <c r="H529" t="s">
-        <v>4425</v>
+        <v>4412</v>
       </c>
       <c r="I529" t="s">
         <v>35</v>
@@ -53558,17 +53871,17 @@
     </row>
     <row r="530" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A530" t="s">
-        <v>4486</v>
+        <v>4473</v>
       </c>
       <c r="B530" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.18µF, ±10%, 25V, X7R, 0603</v>
+        <v>CAP, 0.18uF, ±10%, 25V, X7R, 0603</v>
       </c>
       <c r="C530" t="s">
-        <v>4368</v>
+        <v>1570</v>
       </c>
       <c r="D530" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E530" t="s">
         <v>27</v>
@@ -53580,7 +53893,7 @@
         <v>21</v>
       </c>
       <c r="H530" t="s">
-        <v>4426</v>
+        <v>4413</v>
       </c>
       <c r="I530" t="s">
         <v>35</v>
@@ -53591,17 +53904,17 @@
     </row>
     <row r="531" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A531" t="s">
-        <v>4487</v>
+        <v>4474</v>
       </c>
       <c r="B531" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.27µF, ±10%, 16V, X7R, 0603</v>
+        <v>CAP, 0.27uF, ±10%, 16V, X7R, 0603</v>
       </c>
       <c r="C531" t="s">
-        <v>4371</v>
+        <v>1572</v>
       </c>
       <c r="D531" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E531" t="s">
         <v>19</v>
@@ -53613,7 +53926,7 @@
         <v>21</v>
       </c>
       <c r="H531" t="s">
-        <v>4427</v>
+        <v>4414</v>
       </c>
       <c r="I531" t="s">
         <v>35</v>
@@ -53624,17 +53937,17 @@
     </row>
     <row r="532" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
-        <v>4488</v>
+        <v>4475</v>
       </c>
       <c r="B532" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.1µF, ±10%, 100V, X7R, 0603</v>
+        <v>CAP, 0.1uF, ±10%, 100V, X7R, 0603</v>
       </c>
       <c r="C532" t="s">
-        <v>4362</v>
+        <v>4683</v>
       </c>
       <c r="D532" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E532" t="s">
         <v>947</v>
@@ -53646,7 +53959,7 @@
         <v>21</v>
       </c>
       <c r="H532" t="s">
-        <v>4428</v>
+        <v>4415</v>
       </c>
       <c r="I532" t="s">
         <v>35</v>
@@ -53657,17 +53970,17 @@
     </row>
     <row r="533" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A533" t="s">
-        <v>4489</v>
+        <v>4476</v>
       </c>
       <c r="B533" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 2.2µF, ±10%, 10V, X7R, 0603</v>
+        <v>CAP, 2.2uF, ±10%, 10V, X7R, 0603</v>
       </c>
       <c r="C533" t="s">
-        <v>4369</v>
+        <v>1581</v>
       </c>
       <c r="D533" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E533" t="s">
         <v>950</v>
@@ -53679,7 +53992,7 @@
         <v>21</v>
       </c>
       <c r="H533" t="s">
-        <v>4429</v>
+        <v>4416</v>
       </c>
       <c r="I533" t="s">
         <v>35</v>
@@ -53690,17 +54003,17 @@
     </row>
     <row r="534" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A534" t="s">
-        <v>4490</v>
+        <v>4477</v>
       </c>
       <c r="B534" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.22µF, ±10%, 25V, X7R, 0603</v>
+        <v>CAP, 0.22uF, ±10%, 25V, X7R, 0603</v>
       </c>
       <c r="C534" t="s">
+        <v>1571</v>
+      </c>
+      <c r="D534" t="s">
         <v>4358</v>
-      </c>
-      <c r="D534" t="s">
-        <v>4359</v>
       </c>
       <c r="E534" t="s">
         <v>27</v>
@@ -53712,7 +54025,7 @@
         <v>21</v>
       </c>
       <c r="H534" t="s">
-        <v>4430</v>
+        <v>4417</v>
       </c>
       <c r="I534" t="s">
         <v>35</v>
@@ -53723,17 +54036,17 @@
     </row>
     <row r="535" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
-        <v>4491</v>
+        <v>4478</v>
       </c>
       <c r="B535" t="str">
         <f t="shared" si="9"/>
-        <v>CAP, 0.15µF, ±10%, 25V, X7R, 0603</v>
+        <v>CAP, 0.15uF, ±10%, 25V, X7R, 0603</v>
       </c>
       <c r="C535" t="s">
-        <v>4363</v>
+        <v>1569</v>
       </c>
       <c r="D535" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E535" t="s">
         <v>27</v>
@@ -53745,7 +54058,7 @@
         <v>21</v>
       </c>
       <c r="H535" t="s">
-        <v>4431</v>
+        <v>4418</v>
       </c>
       <c r="I535" t="s">
         <v>35</v>
@@ -53756,17 +54069,17 @@
     </row>
     <row r="536" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A536" t="s">
-        <v>4517</v>
+        <v>4504</v>
       </c>
       <c r="B536" t="str">
-        <f t="shared" si="9"/>
-        <v>CAP, 0.1µF, ±10%, 100V, X7R, 0603</v>
+        <f>CONCATENATE("CAP",", ",C536,", ",D536,", ",E536,", ",F536,", 0603")</f>
+        <v>CAP, 0.1uF, ±10%, 100V, X7R, 0603</v>
       </c>
       <c r="C536" t="s">
-        <v>4362</v>
+        <v>4683</v>
       </c>
       <c r="D536" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="E536" t="s">
         <v>947</v>
@@ -53778,7 +54091,7 @@
         <v>21</v>
       </c>
       <c r="H536" t="s">
-        <v>4518</v>
+        <v>4505</v>
       </c>
       <c r="I536" t="s">
         <v>35</v>
@@ -53792,7 +54105,7 @@
     </row>
     <row r="537" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
-        <v>4524</v>
+        <v>4511</v>
       </c>
       <c r="B537" t="str">
         <f t="shared" si="9"/>
@@ -53814,7 +54127,7 @@
         <v>21</v>
       </c>
       <c r="H537" t="s">
-        <v>4525</v>
+        <v>4512</v>
       </c>
       <c r="I537" t="s">
         <v>35</v>
@@ -53833,10 +54146,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M97"/>
+  <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="M98" sqref="M98"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53851,7 +54164,7 @@
     <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" customWidth="1"/>
     <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -53893,7 +54206,7 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>4523</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -57074,7 +57387,7 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>4565</v>
+        <v>4552</v>
       </c>
       <c r="B96" t="str">
         <f>CONCATENATE("Ind",", ",C96,", ",D96,", ",E96,", ","Nonstandard")</f>
@@ -57087,19 +57400,19 @@
         <v>1286</v>
       </c>
       <c r="E96" t="s">
-        <v>4566</v>
+        <v>4553</v>
       </c>
       <c r="H96" t="s">
-        <v>4567</v>
+        <v>4554</v>
       </c>
       <c r="I96" t="s">
         <v>2423</v>
       </c>
       <c r="J96" s="11" t="s">
-        <v>4568</v>
+        <v>4555</v>
       </c>
       <c r="K96" t="s">
-        <v>4569</v>
+        <v>4556</v>
       </c>
       <c r="L96" t="s">
         <v>1385</v>
@@ -57110,10 +57423,10 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>4631</v>
+        <v>4618</v>
       </c>
       <c r="B97" t="s">
-        <v>4632</v>
+        <v>4619</v>
       </c>
       <c r="C97" t="s">
         <v>1296</v>
@@ -57122,25 +57435,95 @@
         <v>953</v>
       </c>
       <c r="E97" t="s">
-        <v>4633</v>
+        <v>4620</v>
       </c>
       <c r="H97" t="s">
-        <v>4634</v>
+        <v>4621</v>
       </c>
       <c r="I97" t="s">
-        <v>4635</v>
+        <v>4622</v>
       </c>
       <c r="J97" t="s">
-        <v>4636</v>
+        <v>4623</v>
       </c>
       <c r="K97" t="s">
-        <v>4636</v>
+        <v>4623</v>
       </c>
       <c r="L97" t="s">
         <v>1385</v>
       </c>
       <c r="M97" s="8">
         <v>6.08</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>4677</v>
+      </c>
+      <c r="B98" t="s">
+        <v>4678</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>4679</v>
+      </c>
+      <c r="E98" t="s">
+        <v>4680</v>
+      </c>
+      <c r="H98" t="s">
+        <v>4681</v>
+      </c>
+      <c r="I98" t="s">
+        <v>2423</v>
+      </c>
+      <c r="J98">
+        <v>7443641500</v>
+      </c>
+      <c r="K98" t="s">
+        <v>4682</v>
+      </c>
+      <c r="L98" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M98" s="8">
+        <v>9.5299999999999994</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>4685</v>
+      </c>
+      <c r="B99" t="s">
+        <v>4686</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>4679</v>
+      </c>
+      <c r="E99" t="s">
+        <v>4680</v>
+      </c>
+      <c r="H99" t="s">
+        <v>4681</v>
+      </c>
+      <c r="I99" t="s">
+        <v>2423</v>
+      </c>
+      <c r="J99">
+        <v>7443640470</v>
+      </c>
+      <c r="K99" t="s">
+        <v>4682</v>
+      </c>
+      <c r="L99" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M99" s="8">
+        <v>9.5299999999999994</v>
       </c>
     </row>
   </sheetData>
@@ -57151,10 +57534,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57289,36 +57672,50 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4492</v>
+        <v>4479</v>
       </c>
       <c r="B7" t="s">
-        <v>4494</v>
+        <v>4481</v>
       </c>
       <c r="C7" t="s">
         <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>4495</v>
+        <v>4482</v>
       </c>
       <c r="E7" t="s">
-        <v>4496</v>
+        <v>4483</v>
       </c>
       <c r="F7" t="s">
-        <v>4493</v>
+        <v>4480</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4531</v>
+        <v>4518</v>
       </c>
       <c r="B8" t="s">
-        <v>4532</v>
+        <v>4519</v>
       </c>
       <c r="E8" t="s">
-        <v>4533</v>
+        <v>4520</v>
       </c>
       <c r="F8" t="s">
-        <v>4534</v>
+        <v>4521</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4646</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4647</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4648</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4648</v>
       </c>
     </row>
   </sheetData>
@@ -57365,7 +57762,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>4523</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -57521,22 +57918,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4497</v>
+        <v>4484</v>
       </c>
       <c r="B9" t="s">
-        <v>4498</v>
+        <v>4485</v>
       </c>
       <c r="C9" t="s">
         <v>2290</v>
       </c>
       <c r="D9" t="s">
-        <v>4499</v>
+        <v>4486</v>
       </c>
       <c r="E9" t="s">
         <v>2339</v>
       </c>
       <c r="F9" t="s">
-        <v>4500</v>
+        <v>4487</v>
       </c>
       <c r="G9" s="8">
         <v>1.73</v>
@@ -57550,10 +57947,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57610,7 +58007,7 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>4523</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -58064,16 +58461,16 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4540</v>
+        <v>4527</v>
       </c>
       <c r="B16" t="s">
-        <v>4541</v>
+        <v>4528</v>
       </c>
       <c r="C16" t="s">
-        <v>4547</v>
+        <v>4534</v>
       </c>
       <c r="D16" t="s">
-        <v>4542</v>
+        <v>4529</v>
       </c>
       <c r="E16" t="s">
         <v>2335</v>
@@ -58082,19 +58479,19 @@
         <v>2564</v>
       </c>
       <c r="H16" t="s">
-        <v>4543</v>
+        <v>4530</v>
       </c>
       <c r="I16" t="s">
         <v>2290</v>
       </c>
       <c r="J16" t="s">
-        <v>4544</v>
+        <v>4531</v>
       </c>
       <c r="K16" t="s">
-        <v>4545</v>
+        <v>4532</v>
       </c>
       <c r="L16" t="s">
-        <v>4546</v>
+        <v>4533</v>
       </c>
       <c r="M16" s="8">
         <v>0.84</v>
@@ -58102,13 +58499,13 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>4560</v>
+        <v>4547</v>
       </c>
       <c r="B17" t="s">
-        <v>4561</v>
+        <v>4548</v>
       </c>
       <c r="C17" t="s">
-        <v>4564</v>
+        <v>4551</v>
       </c>
       <c r="G17" t="s">
         <v>73</v>
@@ -58120,16 +58517,54 @@
         <v>2290</v>
       </c>
       <c r="J17" t="s">
-        <v>4563</v>
+        <v>4550</v>
       </c>
       <c r="K17" t="s">
         <v>2409</v>
       </c>
       <c r="L17" t="s">
-        <v>4562</v>
+        <v>4549</v>
       </c>
       <c r="M17" s="8">
         <v>2.27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>4692</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4693</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4694</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4695</v>
+      </c>
+      <c r="F18" t="s">
+        <v>4696</v>
+      </c>
+      <c r="G18" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" t="s">
+        <v>74</v>
+      </c>
+      <c r="I18" t="s">
+        <v>2290</v>
+      </c>
+      <c r="J18" t="s">
+        <v>4697</v>
+      </c>
+      <c r="K18" t="s">
+        <v>4698</v>
+      </c>
+      <c r="L18" t="s">
+        <v>4699</v>
+      </c>
+      <c r="M18" s="8">
+        <v>6.35</v>
       </c>
     </row>
   </sheetData>
@@ -58310,7 +58745,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>4523</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -58674,22 +59109,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>4512</v>
+        <v>4499</v>
       </c>
       <c r="B19" t="s">
-        <v>4515</v>
+        <v>4502</v>
       </c>
       <c r="C19" t="s">
         <v>2290</v>
       </c>
       <c r="D19" t="s">
-        <v>4513</v>
+        <v>4500</v>
       </c>
       <c r="E19" t="s">
-        <v>4514</v>
+        <v>4501</v>
       </c>
       <c r="F19" t="s">
-        <v>4516</v>
+        <v>4503</v>
       </c>
       <c r="G19" s="8">
         <v>0.8</v>
@@ -58697,22 +59132,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>4548</v>
+        <v>4535</v>
       </c>
       <c r="B20" t="s">
-        <v>4549</v>
+        <v>4536</v>
       </c>
       <c r="C20" t="s">
         <v>2290</v>
       </c>
       <c r="D20" t="s">
-        <v>4551</v>
+        <v>4538</v>
       </c>
       <c r="E20" t="s">
-        <v>4514</v>
+        <v>4501</v>
       </c>
       <c r="F20" t="s">
-        <v>4550</v>
+        <v>4537</v>
       </c>
       <c r="G20" s="8">
         <v>6.27</v>
@@ -58720,22 +59155,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>4555</v>
+        <v>4542</v>
       </c>
       <c r="B21" t="s">
-        <v>4556</v>
+        <v>4543</v>
       </c>
       <c r="C21" t="s">
         <v>2290</v>
       </c>
       <c r="D21" t="s">
-        <v>4557</v>
+        <v>4544</v>
       </c>
       <c r="E21" t="s">
         <v>2525</v>
       </c>
       <c r="F21" t="s">
-        <v>4558</v>
+        <v>4545</v>
       </c>
       <c r="G21" s="8">
         <v>0.68</v>
@@ -58743,22 +59178,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>4611</v>
+        <v>4598</v>
       </c>
       <c r="B22" t="s">
-        <v>4612</v>
+        <v>4599</v>
       </c>
       <c r="C22" t="s">
         <v>2290</v>
       </c>
       <c r="D22" t="s">
-        <v>4613</v>
+        <v>4600</v>
       </c>
       <c r="E22" t="s">
         <v>2320</v>
       </c>
       <c r="F22" t="s">
-        <v>4614</v>
+        <v>4601</v>
       </c>
       <c r="G22" s="8">
         <v>0.53</v>
@@ -58766,22 +59201,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>4637</v>
+        <v>4624</v>
       </c>
       <c r="B23" t="s">
-        <v>4639</v>
+        <v>4626</v>
       </c>
       <c r="C23" t="s">
         <v>2290</v>
       </c>
       <c r="D23" t="s">
-        <v>4638</v>
+        <v>4625</v>
       </c>
       <c r="E23" t="s">
         <v>2483</v>
       </c>
       <c r="F23" t="s">
-        <v>4640</v>
+        <v>4627</v>
       </c>
       <c r="G23" s="8">
         <v>2.79</v>
@@ -58795,10 +59230,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -58831,7 +59266,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>4523</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -59025,22 +59460,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4501</v>
+        <v>4488</v>
       </c>
       <c r="B11" t="s">
-        <v>4502</v>
+        <v>4489</v>
       </c>
       <c r="C11" t="s">
-        <v>4503</v>
+        <v>4490</v>
       </c>
       <c r="D11" t="s">
-        <v>4504</v>
+        <v>4491</v>
       </c>
       <c r="E11" t="s">
-        <v>4504</v>
+        <v>4491</v>
       </c>
       <c r="F11" t="s">
-        <v>4505</v>
+        <v>4492</v>
       </c>
       <c r="G11" s="8">
         <v>5.0999999999999996</v>
@@ -59048,19 +59483,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4586</v>
+        <v>4573</v>
       </c>
       <c r="B12" t="s">
-        <v>4583</v>
+        <v>4570</v>
       </c>
       <c r="C12" t="s">
-        <v>4584</v>
+        <v>4571</v>
       </c>
       <c r="D12" t="s">
-        <v>4587</v>
+        <v>4574</v>
       </c>
       <c r="E12" t="s">
-        <v>4585</v>
+        <v>4572</v>
       </c>
       <c r="F12" t="s">
         <v>2972</v>
@@ -59071,22 +59506,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4615</v>
+        <v>4602</v>
       </c>
       <c r="B13" t="s">
-        <v>4616</v>
+        <v>4603</v>
       </c>
       <c r="C13" t="s">
         <v>2290</v>
       </c>
       <c r="D13" t="s">
-        <v>4617</v>
+        <v>4604</v>
       </c>
       <c r="E13" t="s">
         <v>2320</v>
       </c>
       <c r="F13" t="s">
-        <v>4618</v>
+        <v>4605</v>
       </c>
       <c r="G13" s="8">
         <v>0.48</v>
@@ -59094,25 +59529,68 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4625</v>
+        <v>4612</v>
       </c>
       <c r="B14" t="s">
-        <v>4626</v>
+        <v>4613</v>
       </c>
       <c r="C14" t="s">
-        <v>4627</v>
+        <v>4614</v>
       </c>
       <c r="D14" t="s">
-        <v>4628</v>
+        <v>4615</v>
       </c>
       <c r="E14" t="s">
-        <v>4629</v>
+        <v>4616</v>
       </c>
       <c r="F14" t="s">
-        <v>4630</v>
+        <v>4617</v>
       </c>
       <c r="G14" s="8">
         <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>4640</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4641</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4642</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4643</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4644</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4645</v>
+      </c>
+      <c r="G15" s="8">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>4658</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4659</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4660</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4661</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4662</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 2.2uF 100V capacitor
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12529" uniqueCount="4700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12538" uniqueCount="4702">
   <si>
     <t>Part Number</t>
   </si>
@@ -14131,6 +14131,12 @@
   </si>
   <si>
     <t>LM5145</t>
+  </si>
+  <si>
+    <t>CAP-00536</t>
+  </si>
+  <si>
+    <t>C3225X7R2A225M230AB</t>
   </si>
 </sst>
 </file>
@@ -36389,10 +36395,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K537"/>
+  <dimension ref="A1:K538"/>
   <sheetViews>
-    <sheetView topLeftCell="A516" workbookViewId="0">
-      <selection activeCell="C533" sqref="C533"/>
+    <sheetView tabSelected="1" topLeftCell="A516" workbookViewId="0">
+      <selection activeCell="K539" sqref="K539"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52983,7 +52989,7 @@
         <v>4446</v>
       </c>
       <c r="B503" t="str">
-        <f t="shared" ref="B503:B537" si="9">CONCATENATE("CAP",", ",C503,", ",D503,", ",E503,", ",F503,", 0603")</f>
+        <f t="shared" ref="B503:B538" si="9">CONCATENATE("CAP",", ",C503,", ",D503,", ",E503,", ",F503,", 0603")</f>
         <v>CAP, 470pF, ±10%, 100V, X7R, 0603</v>
       </c>
       <c r="C503" t="s">
@@ -54139,8 +54145,45 @@
         <v>0.88</v>
       </c>
     </row>
+    <row r="538" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A538" t="s">
+        <v>4700</v>
+      </c>
+      <c r="B538" t="str">
+        <f t="shared" si="9"/>
+        <v>CAP, 2.2uF, ±20%, 100V, X7R, 0603</v>
+      </c>
+      <c r="C538" t="s">
+        <v>1581</v>
+      </c>
+      <c r="D538" t="s">
+        <v>4339</v>
+      </c>
+      <c r="E538" t="s">
+        <v>947</v>
+      </c>
+      <c r="F538" t="s">
+        <v>20</v>
+      </c>
+      <c r="G538" t="s">
+        <v>1384</v>
+      </c>
+      <c r="H538" t="s">
+        <v>4701</v>
+      </c>
+      <c r="I538" t="s">
+        <v>4337</v>
+      </c>
+      <c r="J538" t="s">
+        <v>23</v>
+      </c>
+      <c r="K538" s="8">
+        <v>0.88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -57949,7 +57992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add 330nH inductor from Vishay
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12538" uniqueCount="4702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12548" uniqueCount="4708">
   <si>
     <t>Part Number</t>
   </si>
@@ -14137,6 +14137,24 @@
   </si>
   <si>
     <t>C3225X7R2A225M230AB</t>
+  </si>
+  <si>
+    <t>MAG-00098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ind, 330nH, 0.0024, 29.5A, </t>
+  </si>
+  <si>
+    <t>330nH</t>
+  </si>
+  <si>
+    <t>29.5A</t>
+  </si>
+  <si>
+    <t>IHLP3232DZERR33M01</t>
+  </si>
+  <si>
+    <t>VISHAY_IHLP3232DZERR33M01</t>
   </si>
 </sst>
 </file>
@@ -36397,7 +36415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K538"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A516" workbookViewId="0">
+    <sheetView topLeftCell="A516" workbookViewId="0">
       <selection activeCell="K539" sqref="K539"/>
     </sheetView>
   </sheetViews>
@@ -54189,10 +54207,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M99"/>
+  <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57567,6 +57585,41 @@
       </c>
       <c r="M99" s="8">
         <v>9.5299999999999994</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>4702</v>
+      </c>
+      <c r="B100" t="s">
+        <v>4703</v>
+      </c>
+      <c r="C100" t="s">
+        <v>4704</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>1286</v>
+      </c>
+      <c r="E100" t="s">
+        <v>4705</v>
+      </c>
+      <c r="H100" t="s">
+        <v>4681</v>
+      </c>
+      <c r="I100" t="s">
+        <v>2442</v>
+      </c>
+      <c r="J100" t="s">
+        <v>4706</v>
+      </c>
+      <c r="K100" t="s">
+        <v>4707</v>
+      </c>
+      <c r="L100" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M100" s="8">
+        <v>1.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add/modify some components, add Arduino Nano snippit
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13317" uniqueCount="5134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13442" uniqueCount="5201">
   <si>
     <t>Part Number</t>
   </si>
@@ -15433,6 +15433,207 @@
   </si>
   <si>
     <t>T495X476K035ATE300</t>
+  </si>
+  <si>
+    <t>PWREG-00027</t>
+  </si>
+  <si>
+    <t>10 - 20V</t>
+  </si>
+  <si>
+    <t>FAN7391MXCT-ND</t>
+  </si>
+  <si>
+    <t>Half Bridge Driver, 4.5A, 600V, FAN7391, SO-14</t>
+  </si>
+  <si>
+    <t>FAN7391</t>
+  </si>
+  <si>
+    <t>RES-00603</t>
+  </si>
+  <si>
+    <t>RES SMD 0.04 OHM 1% 1/2W 2010</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>WSL2010R0400FEA</t>
+  </si>
+  <si>
+    <t>ANLG-00039</t>
+  </si>
+  <si>
+    <t>Comparator, Quad, TLV1704, 2.2V-36V, TSSOP-14</t>
+  </si>
+  <si>
+    <t>TLV1704AIPWR</t>
+  </si>
+  <si>
+    <t>comp_q_0</t>
+  </si>
+  <si>
+    <t>RES-00604</t>
+  </si>
+  <si>
+    <t>0.56</t>
+  </si>
+  <si>
+    <t>ERJ-6RQFR56V</t>
+  </si>
+  <si>
+    <t>RES SMD 0.56 OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>LOGIC-00019</t>
+  </si>
+  <si>
+    <t>IC, NAND Gate, Quad 2-Input, Schmitt Trigger, SOIC-14, CD4093</t>
+  </si>
+  <si>
+    <t>CD4093BM96</t>
+  </si>
+  <si>
+    <t>CONN-00038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banana Jack, </t>
+  </si>
+  <si>
+    <t>25A</t>
+  </si>
+  <si>
+    <t>Cal Test Electronics</t>
+  </si>
+  <si>
+    <t>CT3151SP-0</t>
+  </si>
+  <si>
+    <t>CT3151SP_0</t>
+  </si>
+  <si>
+    <t>MISC-00023</t>
+  </si>
+  <si>
+    <t>MOV, 39V, 80A, 0805</t>
+  </si>
+  <si>
+    <t>VC080531C650DP</t>
+  </si>
+  <si>
+    <t>ANLG-00040</t>
+  </si>
+  <si>
+    <t>Op Amp, Dual, Rail-Rail, 45MHz, 45V/us, SOIC-8, LT1632</t>
+  </si>
+  <si>
+    <t>LT1632CS8</t>
+  </si>
+  <si>
+    <t>700mV</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>B560C-13-F</t>
+  </si>
+  <si>
+    <t>Dio, Schottky, 5A, 700mV, 60V, SMC</t>
+  </si>
+  <si>
+    <t>CONN-00039</t>
+  </si>
+  <si>
+    <t>Header, 16x1, 0.1"</t>
+  </si>
+  <si>
+    <t>HDDR_16x1_0</t>
+  </si>
+  <si>
+    <t>conn-16x1_0</t>
+  </si>
+  <si>
+    <t>LED, Blue, 0603, Low current, HELI2 Series</t>
+  </si>
+  <si>
+    <t>2.65V</t>
+  </si>
+  <si>
+    <t>120mW</t>
+  </si>
+  <si>
+    <t>APT1608LVBC/D</t>
+  </si>
+  <si>
+    <t>DIO-00048</t>
+  </si>
+  <si>
+    <t>DIO-00049</t>
+  </si>
+  <si>
+    <t>DIO-00050</t>
+  </si>
+  <si>
+    <t>LED, Green, 0603, Low current, HELI2 Series</t>
+  </si>
+  <si>
+    <t>APT1608LZGCK</t>
+  </si>
+  <si>
+    <t>CONN-00040</t>
+  </si>
+  <si>
+    <t>Header, 15x1, 0x1"</t>
+  </si>
+  <si>
+    <t>HDDR_15x1_0</t>
+  </si>
+  <si>
+    <t>conn-15x1_0</t>
+  </si>
+  <si>
+    <t>CONN-00041</t>
+  </si>
+  <si>
+    <t>USB Mini B, Surface Mount</t>
+  </si>
+  <si>
+    <t>USB Mini B</t>
+  </si>
+  <si>
+    <t>10033526-N3212LF</t>
+  </si>
+  <si>
+    <t>I10033526</t>
+  </si>
+  <si>
+    <t>PWREG-00028</t>
+  </si>
+  <si>
+    <t>REG, Linear, Fixed 5V, 800mA, SOT-223, LM1117-5.0</t>
+  </si>
+  <si>
+    <t>LM1117MPX-5.0/NOPB</t>
+  </si>
+  <si>
+    <t>6.2 - 20V</t>
+  </si>
+  <si>
+    <t>MISC-00024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch, SPST, Tactile, 32V 50mA </t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>KMR6</t>
+  </si>
+  <si>
+    <t>KMR621NG LFS</t>
   </si>
 </sst>
 </file>
@@ -15796,8 +15997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J839"/>
   <sheetViews>
-    <sheetView topLeftCell="A586" workbookViewId="0">
-      <selection activeCell="A605" sqref="A605"/>
+    <sheetView topLeftCell="A592" workbookViewId="0">
+      <selection activeCell="B607" sqref="B607"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33290,10 +33491,62 @@
       </c>
     </row>
     <row r="605" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D605" s="1"/>
+      <c r="A605" t="s">
+        <v>5139</v>
+      </c>
+      <c r="B605" t="s">
+        <v>5140</v>
+      </c>
+      <c r="C605" s="1" t="s">
+        <v>5141</v>
+      </c>
+      <c r="D605" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E605" t="s">
+        <v>4941</v>
+      </c>
+      <c r="F605" t="s">
+        <v>2440</v>
+      </c>
+      <c r="G605" t="s">
+        <v>5142</v>
+      </c>
+      <c r="H605" t="s">
+        <v>5024</v>
+      </c>
+      <c r="I605" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="606" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D606" s="1"/>
+      <c r="A606" t="s">
+        <v>5147</v>
+      </c>
+      <c r="B606" t="s">
+        <v>5150</v>
+      </c>
+      <c r="C606" s="1" t="s">
+        <v>5148</v>
+      </c>
+      <c r="D606" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E606" t="s">
+        <v>2997</v>
+      </c>
+      <c r="F606" t="s">
+        <v>2368</v>
+      </c>
+      <c r="G606" t="s">
+        <v>5149</v>
+      </c>
+      <c r="H606" t="s">
+        <v>11</v>
+      </c>
+      <c r="I606" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="607" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D607" s="1"/>
@@ -34138,10 +34391,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34588,6 +34841,29 @@
         <v>5095</v>
       </c>
       <c r="G20" s="8">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>5151</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5152</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5153</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4308</v>
+      </c>
+      <c r="F21">
+        <v>4093</v>
+      </c>
+      <c r="G21" s="8">
         <v>0.42</v>
       </c>
     </row>
@@ -35685,10 +35961,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView topLeftCell="C31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37423,6 +37699,117 @@
         <v>2.2599999999999998</v>
       </c>
     </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>5178</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>5169</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>5166</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>2121</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>2112</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>5167</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>5168</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>2116</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>2098</v>
+      </c>
+      <c r="M50" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>5179</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>5174</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>5175</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>2948</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>5176</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>4284</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>2498</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>4647</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>5177</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>2503</v>
+      </c>
+      <c r="M51" s="8">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>5180</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>5181</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>5175</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>2948</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>5176</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>4284</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>2498</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>4647</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>5182</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>2503</v>
+      </c>
+      <c r="M52" s="8">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -37431,10 +37818,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38612,6 +38999,122 @@
         <v>2384</v>
       </c>
     </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>5154</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5155</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2512</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>5156</v>
+      </c>
+      <c r="G40" t="s">
+        <v>5157</v>
+      </c>
+      <c r="H40" t="s">
+        <v>5158</v>
+      </c>
+      <c r="I40" t="s">
+        <v>5159</v>
+      </c>
+      <c r="J40" t="s">
+        <v>2969</v>
+      </c>
+      <c r="K40" s="8">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>5170</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5171</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2397</v>
+      </c>
+      <c r="D41">
+        <v>16</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>5172</v>
+      </c>
+      <c r="J41" t="s">
+        <v>5173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>5183</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5184</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2397</v>
+      </c>
+      <c r="D42">
+        <v>15</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>5185</v>
+      </c>
+      <c r="J42" t="s">
+        <v>5186</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>5187</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5188</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5189</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>70</v>
+      </c>
+      <c r="G43" t="s">
+        <v>2911</v>
+      </c>
+      <c r="H43" t="s">
+        <v>5190</v>
+      </c>
+      <c r="I43" t="s">
+        <v>5191</v>
+      </c>
+      <c r="J43" t="s">
+        <v>2908</v>
+      </c>
+      <c r="K43" s="8">
+        <v>0.77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -38622,8 +39125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K554"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="M529" sqref="M529"/>
+    <sheetView topLeftCell="A528" workbookViewId="0">
+      <selection activeCell="A554" sqref="A554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -61110,10 +61613,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -62093,6 +62596,76 @@
       </c>
       <c r="M28" s="8">
         <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>5134</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5137</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5135</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4711</v>
+      </c>
+      <c r="G29" t="s">
+        <v>2428</v>
+      </c>
+      <c r="I29" t="s">
+        <v>2092</v>
+      </c>
+      <c r="J29" t="s">
+        <v>5136</v>
+      </c>
+      <c r="K29" t="s">
+        <v>2481</v>
+      </c>
+      <c r="L29" t="s">
+        <v>5138</v>
+      </c>
+      <c r="M29" s="8">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>5192</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5193</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5195</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2948</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G30" t="s">
+        <v>2562</v>
+      </c>
+      <c r="H30" t="s">
+        <v>2521</v>
+      </c>
+      <c r="I30" t="s">
+        <v>2288</v>
+      </c>
+      <c r="J30" t="s">
+        <v>5194</v>
+      </c>
+      <c r="K30" t="s">
+        <v>4288</v>
+      </c>
+      <c r="L30" t="s">
+        <v>4782</v>
+      </c>
+      <c r="M30" s="8">
+        <v>1.1399999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -62304,10 +62877,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -63208,6 +63781,52 @@
         <v>2.52</v>
       </c>
     </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>5143</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5144</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5145</v>
+      </c>
+      <c r="E41" t="s">
+        <v>3372</v>
+      </c>
+      <c r="F41" t="s">
+        <v>5146</v>
+      </c>
+      <c r="G41" s="8">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>5163</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5164</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4322</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5165</v>
+      </c>
+      <c r="E42" t="s">
+        <v>2318</v>
+      </c>
+      <c r="F42" t="s">
+        <v>4730</v>
+      </c>
+      <c r="G42" s="8">
+        <v>7.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -63216,10 +63835,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -63736,6 +64355,52 @@
         <v>1.53</v>
       </c>
     </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>5160</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5161</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4987</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5162</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4952</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>5196</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5197</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5198</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5200</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5199</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2469</v>
+      </c>
+      <c r="G26" s="8">
+        <v>0.33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Mid-October update. Add many circuits-lab components
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13442" uniqueCount="5201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14126" uniqueCount="5413">
   <si>
     <t>Part Number</t>
   </si>
@@ -15634,6 +15634,642 @@
   </si>
   <si>
     <t>KMR621NG LFS</t>
+  </si>
+  <si>
+    <t>ANLG-00041</t>
+  </si>
+  <si>
+    <t>LTC2057IS8#PBF</t>
+  </si>
+  <si>
+    <t>LTC2057</t>
+  </si>
+  <si>
+    <t>Op Amp, Single, High-Voltage (4.5 - 36V), Low Noise, Zero-Drift, SOIC-8, LTC2057</t>
+  </si>
+  <si>
+    <t>Triac Driver Opto-Coupler, 800V peak voltage</t>
+  </si>
+  <si>
+    <t>MOC3072SVM</t>
+  </si>
+  <si>
+    <t>MDIP_6_SMD</t>
+  </si>
+  <si>
+    <t>MOC3072</t>
+  </si>
+  <si>
+    <t>XSTR-00028</t>
+  </si>
+  <si>
+    <t>CLA80MT1200NHB</t>
+  </si>
+  <si>
+    <t>triac</t>
+  </si>
+  <si>
+    <t>1.26V</t>
+  </si>
+  <si>
+    <t>Ixys</t>
+  </si>
+  <si>
+    <t>TRIAC</t>
+  </si>
+  <si>
+    <t>TRIAC, 40A, 1200V, Vt 1.26V, TO-247</t>
+  </si>
+  <si>
+    <t>CS45-16IO1R</t>
+  </si>
+  <si>
+    <t>scr_0</t>
+  </si>
+  <si>
+    <t>SCR</t>
+  </si>
+  <si>
+    <t>48A</t>
+  </si>
+  <si>
+    <t>1.6kV</t>
+  </si>
+  <si>
+    <t>1.64V</t>
+  </si>
+  <si>
+    <t>SCR, 1.6kV 48A, 100mA trigger, TO-247</t>
+  </si>
+  <si>
+    <t>DIO-00051</t>
+  </si>
+  <si>
+    <t>ANLG-00042</t>
+  </si>
+  <si>
+    <t>Comparator, Quad, LM339, DIP-14</t>
+  </si>
+  <si>
+    <t>LM339N</t>
+  </si>
+  <si>
+    <t>DIP14</t>
+  </si>
+  <si>
+    <t>LOGIC-00020</t>
+  </si>
+  <si>
+    <t>IC, NAND Gate, Quad 2-Input, Schmitt Trigger, DIP-14, CD4093</t>
+  </si>
+  <si>
+    <t>CD4093BE</t>
+  </si>
+  <si>
+    <t>RES-00605</t>
+  </si>
+  <si>
+    <t>RES-00606</t>
+  </si>
+  <si>
+    <t>RES-00607</t>
+  </si>
+  <si>
+    <t>axial_0.3</t>
+  </si>
+  <si>
+    <t>axial_0.4</t>
+  </si>
+  <si>
+    <t>RES-00608</t>
+  </si>
+  <si>
+    <t>RES-00609</t>
+  </si>
+  <si>
+    <t>RES-00610</t>
+  </si>
+  <si>
+    <t>RES-00611</t>
+  </si>
+  <si>
+    <t>RES-00612</t>
+  </si>
+  <si>
+    <t>RES THT 1K OHM 1% 1/4W 0.3" AXIAL</t>
+  </si>
+  <si>
+    <t>RES THT 1K OHM 1% 1/4W 0.4" AXIAL</t>
+  </si>
+  <si>
+    <t>RES THT 1M OHM 1% 1/4W 0.3" AXIAL</t>
+  </si>
+  <si>
+    <t>RES THT 1M OHM 1% 1/4W 0.4" AXIAL</t>
+  </si>
+  <si>
+    <t>RES THT 10K OHM 1% 1/4W 0.3" AXIAL</t>
+  </si>
+  <si>
+    <t>RES THT 10K OHM 1% 1/4W 0.4" AXIAL</t>
+  </si>
+  <si>
+    <t>RES THT 100K OHM 1% 1/4W 0.3" AXIAL</t>
+  </si>
+  <si>
+    <t>RES THT 100K OHM 1% 1/4W 0.4" AXIAL</t>
+  </si>
+  <si>
+    <t>RES-00613</t>
+  </si>
+  <si>
+    <t>RES-00614</t>
+  </si>
+  <si>
+    <t>RES THT 10M OHM 1% 1/4W 0.3" AXIAL</t>
+  </si>
+  <si>
+    <t>RES THT 10M OHM 1% 1/4W 0.4" AXIAL</t>
+  </si>
+  <si>
+    <t>ANLG-00043</t>
+  </si>
+  <si>
+    <t>4N25M</t>
+  </si>
+  <si>
+    <t>DIP6</t>
+  </si>
+  <si>
+    <t>4N25</t>
+  </si>
+  <si>
+    <t>ANLG-00044</t>
+  </si>
+  <si>
+    <t>Opto-Coupler, Photo-Transistor output, 5000 Vrms Isolation</t>
+  </si>
+  <si>
+    <t>XSTR-00029</t>
+  </si>
+  <si>
+    <t>XSTR-00030</t>
+  </si>
+  <si>
+    <t>XSTR NPN, 600mA, 40V, Vce 1V, TO-92</t>
+  </si>
+  <si>
+    <t>625mW</t>
+  </si>
+  <si>
+    <t>2N4401TAR</t>
+  </si>
+  <si>
+    <t>TO-92_0</t>
+  </si>
+  <si>
+    <t>XSTR PNP, 600mA, 40V, Vce 0.75V, TO-92</t>
+  </si>
+  <si>
+    <t>2N4403BU</t>
+  </si>
+  <si>
+    <t>TO-92_1</t>
+  </si>
+  <si>
+    <t>RES-00615</t>
+  </si>
+  <si>
+    <t>1/4W</t>
+  </si>
+  <si>
+    <t>RES-00616</t>
+  </si>
+  <si>
+    <t>RES-00617</t>
+  </si>
+  <si>
+    <t>RES-00618</t>
+  </si>
+  <si>
+    <t>RES-00619</t>
+  </si>
+  <si>
+    <t>RES-00620</t>
+  </si>
+  <si>
+    <t>RES-00621</t>
+  </si>
+  <si>
+    <t>RES-00622</t>
+  </si>
+  <si>
+    <t>RES-00623</t>
+  </si>
+  <si>
+    <t>RES-00624</t>
+  </si>
+  <si>
+    <t>RES-00625</t>
+  </si>
+  <si>
+    <t>RES-00626</t>
+  </si>
+  <si>
+    <t>RES-00627</t>
+  </si>
+  <si>
+    <t>RES-00628</t>
+  </si>
+  <si>
+    <t>RES-00629</t>
+  </si>
+  <si>
+    <t>RES-00630</t>
+  </si>
+  <si>
+    <t>RES-00631</t>
+  </si>
+  <si>
+    <t>RES-00632</t>
+  </si>
+  <si>
+    <t>RES-00633</t>
+  </si>
+  <si>
+    <t>RES-00634</t>
+  </si>
+  <si>
+    <t>RES-00635</t>
+  </si>
+  <si>
+    <t>RES-00636</t>
+  </si>
+  <si>
+    <t>RES-00637</t>
+  </si>
+  <si>
+    <t>RES-00638</t>
+  </si>
+  <si>
+    <t>RES-00639</t>
+  </si>
+  <si>
+    <t>RES-00640</t>
+  </si>
+  <si>
+    <t>RES-00641</t>
+  </si>
+  <si>
+    <t>RES-00642</t>
+  </si>
+  <si>
+    <t>RES-00643</t>
+  </si>
+  <si>
+    <t>RES-00644</t>
+  </si>
+  <si>
+    <t>RES-00645</t>
+  </si>
+  <si>
+    <t>RES-00646</t>
+  </si>
+  <si>
+    <t>RES-00647</t>
+  </si>
+  <si>
+    <t>RES-00648</t>
+  </si>
+  <si>
+    <t>RES-00649</t>
+  </si>
+  <si>
+    <t>RES-00650</t>
+  </si>
+  <si>
+    <t>RES-00651</t>
+  </si>
+  <si>
+    <t>RES-00652</t>
+  </si>
+  <si>
+    <t>RES-00653</t>
+  </si>
+  <si>
+    <t>RES-00654</t>
+  </si>
+  <si>
+    <t>RES-00655</t>
+  </si>
+  <si>
+    <t>RES-00656</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>RES-00657</t>
+  </si>
+  <si>
+    <t>RES-00658</t>
+  </si>
+  <si>
+    <t>RES-00659</t>
+  </si>
+  <si>
+    <t>RES-00660</t>
+  </si>
+  <si>
+    <t>RES-00661</t>
+  </si>
+  <si>
+    <t>RES-00662</t>
+  </si>
+  <si>
+    <t>RES-00663</t>
+  </si>
+  <si>
+    <t>RES-00664</t>
+  </si>
+  <si>
+    <t>RES-00665</t>
+  </si>
+  <si>
+    <t>RES-00666</t>
+  </si>
+  <si>
+    <t>RES-00667</t>
+  </si>
+  <si>
+    <t>RES-00668</t>
+  </si>
+  <si>
+    <t>RES-00669</t>
+  </si>
+  <si>
+    <t>RES-00670</t>
+  </si>
+  <si>
+    <t>RES-00671</t>
+  </si>
+  <si>
+    <t>RES-00672</t>
+  </si>
+  <si>
+    <t>RES-00673</t>
+  </si>
+  <si>
+    <t>RES-00674</t>
+  </si>
+  <si>
+    <t>RES-00675</t>
+  </si>
+  <si>
+    <t>RES-00676</t>
+  </si>
+  <si>
+    <t>RES-00677</t>
+  </si>
+  <si>
+    <t>RES-00678</t>
+  </si>
+  <si>
+    <t>RES-00679</t>
+  </si>
+  <si>
+    <t>RES-00680</t>
+  </si>
+  <si>
+    <t>RES-00681</t>
+  </si>
+  <si>
+    <t>RES-00682</t>
+  </si>
+  <si>
+    <t>RES-00683</t>
+  </si>
+  <si>
+    <t>RES-00684</t>
+  </si>
+  <si>
+    <t>Op Amp, Quad, Rail-Rail, 3-MHz, DIP-14, TLV274</t>
+  </si>
+  <si>
+    <t>TLV274IN</t>
+  </si>
+  <si>
+    <t>ANLG-00045</t>
+  </si>
+  <si>
+    <t>PWREG-00029</t>
+  </si>
+  <si>
+    <t>REG, Linear, Fixed 5V, 1A, TO-220</t>
+  </si>
+  <si>
+    <t>LM7805CT/NOPB</t>
+  </si>
+  <si>
+    <t>LOGIC-00021</t>
+  </si>
+  <si>
+    <t>ANLG-00046</t>
+  </si>
+  <si>
+    <t>IC, 555 Timer, DIP-8</t>
+  </si>
+  <si>
+    <t>NE555P</t>
+  </si>
+  <si>
+    <t>DIP8</t>
+  </si>
+  <si>
+    <t>LOGIC-00022</t>
+  </si>
+  <si>
+    <t>IC, Hex Inverter, Schmitt Triggered Inputs, DIP-14, CD40106</t>
+  </si>
+  <si>
+    <t>CD40106BE</t>
+  </si>
+  <si>
+    <t>PWREG-00030</t>
+  </si>
+  <si>
+    <t>REG, SW AC/DC Converter Module, Fixed 5V, 1.2A</t>
+  </si>
+  <si>
+    <t>85 - 264VAC</t>
+  </si>
+  <si>
+    <t>1.2A</t>
+  </si>
+  <si>
+    <t>70kHz</t>
+  </si>
+  <si>
+    <t>VOF-6B-S5</t>
+  </si>
+  <si>
+    <t>VOF-6B</t>
+  </si>
+  <si>
+    <t>AC-DC-conv-0</t>
+  </si>
+  <si>
+    <t>RES-00685</t>
+  </si>
+  <si>
+    <t>0.6W</t>
+  </si>
+  <si>
+    <t>axial_0.4_1</t>
+  </si>
+  <si>
+    <t>MBB02070C1005FCT00</t>
+  </si>
+  <si>
+    <t>Vishay BC Components</t>
+  </si>
+  <si>
+    <t>MBB02070C1004FRP00</t>
+  </si>
+  <si>
+    <t>RES-00686</t>
+  </si>
+  <si>
+    <t>RES-00687</t>
+  </si>
+  <si>
+    <t>100M</t>
+  </si>
+  <si>
+    <t>RNX025100MFKEE</t>
+  </si>
+  <si>
+    <t>axial_0.5</t>
+  </si>
+  <si>
+    <t>LOGIC-00023</t>
+  </si>
+  <si>
+    <t>IC, Dual Up-Down Counter, CD4518</t>
+  </si>
+  <si>
+    <t>CD4518BE</t>
+  </si>
+  <si>
+    <t>DIP16</t>
+  </si>
+  <si>
+    <t>LOGIC-00024</t>
+  </si>
+  <si>
+    <t>IC, Divide-by-N-Counter, CD4018</t>
+  </si>
+  <si>
+    <t>CD4018BE</t>
+  </si>
+  <si>
+    <t>LOGIC-00025</t>
+  </si>
+  <si>
+    <t>IC, Quad Bilateral Switch, DIP-14, CD4066B</t>
+  </si>
+  <si>
+    <t>CD4066BE</t>
+  </si>
+  <si>
+    <t>IC, Flip-Flop, Dual D-Type,  DIP-14, CD4013</t>
+  </si>
+  <si>
+    <t>CD4013BE</t>
+  </si>
+  <si>
+    <t>LOGIC-00026</t>
+  </si>
+  <si>
+    <t>IC, NOR gate, Quad 2-input, DIP-14, CD4001</t>
+  </si>
+  <si>
+    <t>CD4001BE</t>
+  </si>
+  <si>
+    <t>MAG-00103</t>
+  </si>
+  <si>
+    <t>Pulse Xfmr, 2.5mH, 1A, 2.2kV isolation</t>
+  </si>
+  <si>
+    <t>2.5mH</t>
+  </si>
+  <si>
+    <t>Schurter</t>
+  </si>
+  <si>
+    <t>ILR-11-0001</t>
+  </si>
+  <si>
+    <t>xfmr_4</t>
+  </si>
+  <si>
+    <t>SCHURTER_ILR</t>
+  </si>
+  <si>
+    <t>DIO-00052</t>
+  </si>
+  <si>
+    <t>Dio, Silicon, 30A, 1.25V, 1.6kV, D2PAK</t>
+  </si>
+  <si>
+    <t>1.25V</t>
+  </si>
+  <si>
+    <t>160W</t>
+  </si>
+  <si>
+    <t>DSI30-16AS-TRL</t>
+  </si>
+  <si>
+    <t>diode_10</t>
+  </si>
+  <si>
+    <t>D2PAK-3_1</t>
+  </si>
+  <si>
+    <t>MOV, 300V 2.5kA, 10mm disc</t>
+  </si>
+  <si>
+    <t>MOV-10D301KTR</t>
+  </si>
+  <si>
+    <t>BOURNS-MOV-10D301K</t>
+  </si>
+  <si>
+    <t>MISC-00025</t>
+  </si>
+  <si>
+    <t>MAG-00104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common Mode Choke, 2.6mH 0.1 Ohm 2.2A </t>
+  </si>
+  <si>
+    <t>2.6mH</t>
+  </si>
+  <si>
+    <t>100mOhm</t>
+  </si>
+  <si>
+    <t>SSR10HS-22026</t>
+  </si>
+  <si>
+    <t>KEMET-SSR10HS-22026</t>
+  </si>
+  <si>
+    <t>cmd_0</t>
   </si>
 </sst>
 </file>
@@ -15997,8 +16633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J839"/>
   <sheetViews>
-    <sheetView topLeftCell="A592" workbookViewId="0">
-      <selection activeCell="B607" sqref="B607"/>
+    <sheetView topLeftCell="A667" workbookViewId="0">
+      <selection activeCell="H691" sqref="H691"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33549,297 +34185,2048 @@
       </c>
     </row>
     <row r="607" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D607" s="1"/>
+      <c r="A607" t="s">
+        <v>5231</v>
+      </c>
+      <c r="B607" t="s">
+        <v>5241</v>
+      </c>
+      <c r="C607" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="D607" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E607" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H607" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I607" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="608" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D608" s="1"/>
-    </row>
-    <row r="609" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D609" s="1"/>
-    </row>
-    <row r="610" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D610" s="1"/>
-    </row>
-    <row r="611" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D611" s="1"/>
-    </row>
-    <row r="612" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D612" s="1"/>
-    </row>
-    <row r="613" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D613" s="1"/>
-    </row>
-    <row r="614" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D614" s="1"/>
-    </row>
-    <row r="615" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D615" s="1"/>
-    </row>
-    <row r="616" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D616" s="1"/>
-    </row>
-    <row r="617" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D617" s="1"/>
-    </row>
-    <row r="618" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D618" s="1"/>
-    </row>
-    <row r="619" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D619" s="1"/>
-    </row>
-    <row r="620" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D620" s="1"/>
-    </row>
-    <row r="621" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D621" s="1"/>
-    </row>
-    <row r="622" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D622" s="1"/>
-    </row>
-    <row r="623" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D623" s="1"/>
-    </row>
-    <row r="624" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D624" s="1"/>
-    </row>
-    <row r="625" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D625" s="1"/>
-    </row>
-    <row r="626" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D626" s="1"/>
-    </row>
-    <row r="627" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D627" s="1"/>
-    </row>
-    <row r="628" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D628" s="1"/>
-    </row>
-    <row r="629" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D629" s="1"/>
-    </row>
-    <row r="630" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D630" s="1"/>
-    </row>
-    <row r="631" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D631" s="1"/>
-    </row>
-    <row r="632" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D632" s="1"/>
-    </row>
-    <row r="633" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D633" s="1"/>
-    </row>
-    <row r="634" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D634" s="1"/>
-    </row>
-    <row r="635" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D635" s="1"/>
-    </row>
-    <row r="636" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D636" s="1"/>
-    </row>
-    <row r="637" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D637" s="1"/>
-    </row>
-    <row r="638" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D638" s="1"/>
-    </row>
-    <row r="639" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D639" s="1"/>
-    </row>
-    <row r="640" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D640" s="1"/>
-    </row>
-    <row r="641" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D641" s="1"/>
-    </row>
-    <row r="642" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D642" s="1"/>
-    </row>
-    <row r="643" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D643" s="1"/>
-    </row>
-    <row r="644" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D644" s="1"/>
-    </row>
-    <row r="645" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D645" s="1"/>
-    </row>
-    <row r="646" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D646" s="1"/>
-    </row>
-    <row r="647" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D647" s="1"/>
-    </row>
-    <row r="648" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D648" s="1"/>
-    </row>
-    <row r="649" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D649" s="1"/>
-    </row>
-    <row r="650" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D650" s="1"/>
-    </row>
-    <row r="651" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D651" s="1"/>
-    </row>
-    <row r="652" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D652" s="1"/>
-    </row>
-    <row r="653" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D653" s="1"/>
-    </row>
-    <row r="654" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D654" s="1"/>
-    </row>
-    <row r="655" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D655" s="1"/>
-    </row>
-    <row r="656" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D656" s="1"/>
-    </row>
-    <row r="657" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D657" s="1"/>
-    </row>
-    <row r="658" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D658" s="1"/>
-    </row>
-    <row r="659" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D659" s="1"/>
-    </row>
-    <row r="660" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D660" s="1"/>
-    </row>
-    <row r="661" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D661" s="1"/>
-    </row>
-    <row r="662" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D662" s="1"/>
-    </row>
-    <row r="663" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D663" s="1"/>
-    </row>
-    <row r="664" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D664" s="1"/>
-    </row>
-    <row r="665" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D665" s="1"/>
-    </row>
-    <row r="666" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D666" s="1"/>
-    </row>
-    <row r="667" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D667" s="1"/>
-    </row>
-    <row r="668" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D668" s="1"/>
-    </row>
-    <row r="669" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D669" s="1"/>
-    </row>
-    <row r="670" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D670" s="1"/>
-    </row>
-    <row r="671" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D671" s="1"/>
-    </row>
-    <row r="672" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D672" s="1"/>
-    </row>
-    <row r="673" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D673" s="1"/>
-    </row>
-    <row r="674" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D674" s="1"/>
-    </row>
-    <row r="675" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D675" s="1"/>
-    </row>
-    <row r="676" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D676" s="1"/>
-    </row>
-    <row r="677" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D677" s="1"/>
-    </row>
-    <row r="678" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D678" s="1"/>
-    </row>
-    <row r="679" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D679" s="1"/>
-    </row>
-    <row r="680" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D680" s="1"/>
-    </row>
-    <row r="681" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D681" s="1"/>
-    </row>
-    <row r="682" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D682" s="1"/>
-    </row>
-    <row r="683" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D683" s="1"/>
-    </row>
-    <row r="684" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D684" s="1"/>
-    </row>
-    <row r="685" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D685" s="1"/>
-    </row>
-    <row r="686" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D686" s="1"/>
-    </row>
-    <row r="687" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D687" s="1"/>
-    </row>
-    <row r="688" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D688" s="1"/>
-    </row>
-    <row r="689" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D689" s="1"/>
-    </row>
-    <row r="690" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="A608" t="s">
+        <v>5232</v>
+      </c>
+      <c r="B608" t="s">
+        <v>5242</v>
+      </c>
+      <c r="C608" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="D608" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E608" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H608" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I608" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="609" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A609" t="s">
+        <v>5233</v>
+      </c>
+      <c r="B609" t="s">
+        <v>5245</v>
+      </c>
+      <c r="C609" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="D609" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E609" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H609" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I609" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="610" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A610" t="s">
+        <v>5236</v>
+      </c>
+      <c r="B610" t="s">
+        <v>5246</v>
+      </c>
+      <c r="C610" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="D610" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E610" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H610" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I610" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="611" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A611" t="s">
+        <v>5237</v>
+      </c>
+      <c r="B611" t="s">
+        <v>5247</v>
+      </c>
+      <c r="C611" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D611" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E611" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H611" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I611" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="612" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A612" t="s">
+        <v>5238</v>
+      </c>
+      <c r="B612" t="s">
+        <v>5248</v>
+      </c>
+      <c r="C612" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D612" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E612" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H612" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I612" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="613" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A613" t="s">
+        <v>5239</v>
+      </c>
+      <c r="B613" t="s">
+        <v>5243</v>
+      </c>
+      <c r="C613" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="D613" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E613" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H613" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I613" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="614" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A614" t="s">
+        <v>5240</v>
+      </c>
+      <c r="B614" t="s">
+        <v>5244</v>
+      </c>
+      <c r="C614" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="D614" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E614" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H614" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I614" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="615" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A615" t="s">
+        <v>5249</v>
+      </c>
+      <c r="B615" t="s">
+        <v>5251</v>
+      </c>
+      <c r="C615" s="1" t="s">
+        <v>3797</v>
+      </c>
+      <c r="D615" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E615" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H615" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I615" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="616" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A616" t="s">
+        <v>5250</v>
+      </c>
+      <c r="B616" t="s">
+        <v>5252</v>
+      </c>
+      <c r="C616" s="1" t="s">
+        <v>3797</v>
+      </c>
+      <c r="D616" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E616" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H616" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I616" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="617" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A617" t="s">
+        <v>5268</v>
+      </c>
+      <c r="B617" t="str">
+        <f>CONCATENATE("RES THT ",C617," OHM ",D617," ",E617," 0.3 AXIAL")</f>
+        <v>RES THT 1.5k OHM 1% 1/4W 0.3 AXIAL</v>
+      </c>
+      <c r="C617" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D617" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E617" t="s">
+        <v>5269</v>
+      </c>
+      <c r="H617" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I617" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="618" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A618" t="s">
+        <v>5270</v>
+      </c>
+      <c r="B618" t="str">
+        <f t="shared" ref="B618:B637" si="0">CONCATENATE("RES THT ",C618," OHM ",D618," ",E618," 0.3 AXIAL")</f>
+        <v>RES THT 2.2k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C618" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="D618" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E618" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H618" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I618" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="619" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A619" t="s">
+        <v>5271</v>
+      </c>
+      <c r="B619" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 3.3k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C619" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D619" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E619" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H619" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I619" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="620" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A620" t="s">
+        <v>5272</v>
+      </c>
+      <c r="B620" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 4.7k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C620" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D620" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E620" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H620" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I620" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="621" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A621" t="s">
+        <v>5273</v>
+      </c>
+      <c r="B621" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 5.6k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C621" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D621" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E621" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H621" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I621" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="622" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A622" t="s">
+        <v>5274</v>
+      </c>
+      <c r="B622" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 6.8k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C622" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="D622" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E622" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H622" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I622" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="623" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A623" t="s">
+        <v>5275</v>
+      </c>
+      <c r="B623" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 8.2k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C623" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D623" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E623" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H623" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I623" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="624" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A624" t="s">
+        <v>5276</v>
+      </c>
+      <c r="B624" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 22k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C624" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D624" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E624" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H624" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I624" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="625" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A625" t="s">
+        <v>5277</v>
+      </c>
+      <c r="B625" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 33k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C625" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="D625" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E625" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H625" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I625" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="626" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A626" t="s">
+        <v>5278</v>
+      </c>
+      <c r="B626" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 47k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C626" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D626" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E626" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H626" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I626" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="627" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A627" t="s">
+        <v>5279</v>
+      </c>
+      <c r="B627" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 56k OHM 1% 1/4W 0.3 AXIAL</v>
+      </c>
+      <c r="C627" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="D627" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E627" t="s">
+        <v>5269</v>
+      </c>
+      <c r="H627" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I627" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="628" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A628" t="s">
+        <v>5280</v>
+      </c>
+      <c r="B628" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 68k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C628" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D628" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E628" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H628" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I628" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="629" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A629" t="s">
+        <v>5281</v>
+      </c>
+      <c r="B629" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 82k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C629" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D629" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E629" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H629" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I629" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="630" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A630" t="s">
+        <v>5282</v>
+      </c>
+      <c r="B630" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 150k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C630" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D630" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E630" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H630" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I630" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="631" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A631" t="s">
+        <v>5283</v>
+      </c>
+      <c r="B631" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 220k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C631" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D631" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E631" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H631" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I631" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="632" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A632" t="s">
+        <v>5284</v>
+      </c>
+      <c r="B632" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 330k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C632" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="D632" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E632" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H632" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I632" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="633" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A633" t="s">
+        <v>5285</v>
+      </c>
+      <c r="B633" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 470k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C633" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D633" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E633" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H633" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I633" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="634" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A634" t="s">
+        <v>5286</v>
+      </c>
+      <c r="B634" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 560k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C634" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D634" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E634" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H634" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I634" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="635" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A635" t="s">
+        <v>5287</v>
+      </c>
+      <c r="B635" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 680k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C635" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D635" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E635" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H635" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I635" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="636" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A636" t="s">
+        <v>5288</v>
+      </c>
+      <c r="B636" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 820k OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C636" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D636" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E636" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H636" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I636" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="637" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A637" t="s">
+        <v>5289</v>
+      </c>
+      <c r="B637" t="str">
+        <f t="shared" si="0"/>
+        <v>RES THT 3M OHM 1% 1/4W 0.3 AXIAL</v>
+      </c>
+      <c r="C637" s="1" t="s">
+        <v>4030</v>
+      </c>
+      <c r="D637" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E637" t="s">
+        <v>5269</v>
+      </c>
+      <c r="H637" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I637" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="638" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A638" t="s">
+        <v>5290</v>
+      </c>
+      <c r="B638" t="str">
+        <f>CONCATENATE("RES THT ",C638," OHM ",D638," ",E638," 0.4 AXIAL")</f>
+        <v>RES THT 1.5k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C638" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D638" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E638" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H638" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I638" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="639" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A639" t="s">
+        <v>5291</v>
+      </c>
+      <c r="B639" t="str">
+        <f t="shared" ref="B639:B658" si="1">CONCATENATE("RES THT ",C639," OHM ",D639," ",E639," 0.4 AXIAL")</f>
+        <v>RES THT 2.2k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C639" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="D639" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E639" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H639" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I639" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="640" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A640" t="s">
+        <v>5292</v>
+      </c>
+      <c r="B640" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 3.3k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C640" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D640" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E640" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H640" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I640" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="641" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A641" t="s">
+        <v>5293</v>
+      </c>
+      <c r="B641" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 4.7k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C641" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D641" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E641" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H641" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I641" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="642" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A642" t="s">
+        <v>5294</v>
+      </c>
+      <c r="B642" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 5.6k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C642" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D642" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E642" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H642" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I642" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="643" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A643" t="s">
+        <v>5295</v>
+      </c>
+      <c r="B643" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 6.8k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C643" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="D643" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E643" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H643" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I643" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="644" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A644" t="s">
+        <v>5296</v>
+      </c>
+      <c r="B644" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 8.2k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C644" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D644" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E644" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H644" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I644" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="645" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A645" t="s">
+        <v>5297</v>
+      </c>
+      <c r="B645" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 22k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C645" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D645" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E645" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H645" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I645" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="646" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A646" t="s">
+        <v>5298</v>
+      </c>
+      <c r="B646" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 33k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C646" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="D646" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E646" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H646" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I646" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="647" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A647" t="s">
+        <v>5299</v>
+      </c>
+      <c r="B647" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 47k OHM 1% 1/4W 0.4 AXIAL</v>
+      </c>
+      <c r="C647" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D647" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E647" t="s">
+        <v>5269</v>
+      </c>
+      <c r="H647" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I647" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="648" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A648" t="s">
+        <v>5300</v>
+      </c>
+      <c r="B648" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 56k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C648" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="D648" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E648" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H648" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I648" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="649" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A649" t="s">
+        <v>5301</v>
+      </c>
+      <c r="B649" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 68k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C649" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D649" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E649" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H649" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I649" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="650" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A650" t="s">
+        <v>5302</v>
+      </c>
+      <c r="B650" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 82k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C650" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D650" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E650" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H650" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I650" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="651" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A651" t="s">
+        <v>5303</v>
+      </c>
+      <c r="B651" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 150k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C651" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D651" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E651" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H651" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I651" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="652" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A652" t="s">
+        <v>5304</v>
+      </c>
+      <c r="B652" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 220k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C652" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D652" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E652" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H652" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I652" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="653" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A653" t="s">
+        <v>5305</v>
+      </c>
+      <c r="B653" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 330k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C653" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="D653" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E653" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H653" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I653" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="654" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A654" t="s">
+        <v>5306</v>
+      </c>
+      <c r="B654" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 470k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C654" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D654" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E654" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H654" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I654" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="655" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A655" t="s">
+        <v>5307</v>
+      </c>
+      <c r="B655" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 560k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C655" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D655" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E655" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H655" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I655" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="656" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A656" t="s">
+        <v>5308</v>
+      </c>
+      <c r="B656" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 680k OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C656" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D656" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E656" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H656" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I656" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="657" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A657" t="s">
+        <v>5309</v>
+      </c>
+      <c r="B657" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 820k OHM 1% 1/4W 0.4 AXIAL</v>
+      </c>
+      <c r="C657" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D657" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E657" t="s">
+        <v>5269</v>
+      </c>
+      <c r="H657" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I657" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="658" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A658" t="s">
+        <v>5310</v>
+      </c>
+      <c r="B658" t="str">
+        <f t="shared" si="1"/>
+        <v>RES THT 3M OHM 1% 1/4W 0.4 AXIAL</v>
+      </c>
+      <c r="C658" s="1" t="s">
+        <v>4030</v>
+      </c>
+      <c r="D658" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E658" t="s">
+        <v>5269</v>
+      </c>
+      <c r="H658" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I658" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="659" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A659" t="s">
+        <v>5312</v>
+      </c>
+      <c r="B659" t="str">
+        <f>CONCATENATE("RES THT ",C659," OHM ",D659," ",E659," 0.3 AXIAL")</f>
+        <v>RES THT 22 OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C659" s="1" t="s">
+        <v>3230</v>
+      </c>
+      <c r="D659" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E659" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H659" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I659" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="660" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A660" t="s">
+        <v>5313</v>
+      </c>
+      <c r="B660" t="str">
+        <f t="shared" ref="B660:B672" si="2">CONCATENATE("RES THT ",C660," OHM ",D660," ",E660," 0.3 AXIAL")</f>
+        <v>RES THT 33 OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C660" s="1" t="s">
+        <v>3015</v>
+      </c>
+      <c r="D660" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E660" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H660" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I660" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="661" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A661" t="s">
+        <v>5314</v>
+      </c>
+      <c r="B661" t="str">
+        <f t="shared" si="2"/>
+        <v>RES THT 46 OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C661" s="1" t="s">
+        <v>5311</v>
+      </c>
+      <c r="D661" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E661" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H661" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I661" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="662" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A662" t="s">
+        <v>5315</v>
+      </c>
+      <c r="B662" t="str">
+        <f t="shared" si="2"/>
+        <v>RES THT 56 OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C662" s="1" t="s">
+        <v>3279</v>
+      </c>
+      <c r="D662" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E662" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H662" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I662" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="663" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A663" t="s">
+        <v>5316</v>
+      </c>
+      <c r="B663" t="str">
+        <f t="shared" si="2"/>
+        <v>RES THT 68 OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C663" s="1" t="s">
+        <v>3285</v>
+      </c>
+      <c r="D663" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E663" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H663" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I663" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="664" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A664" t="s">
+        <v>5317</v>
+      </c>
+      <c r="B664" t="str">
+        <f t="shared" si="2"/>
+        <v>RES THT 82 OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C664" s="1" t="s">
+        <v>3294</v>
+      </c>
+      <c r="D664" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E664" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H664" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I664" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="665" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A665" t="s">
+        <v>5318</v>
+      </c>
+      <c r="B665" t="str">
+        <f t="shared" si="2"/>
+        <v>RES THT 100 OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C665" s="1" t="s">
+        <v>3160</v>
+      </c>
+      <c r="D665" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E665" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H665" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I665" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="666" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A666" t="s">
+        <v>5319</v>
+      </c>
+      <c r="B666" t="str">
+        <f t="shared" si="2"/>
+        <v>RES THT 150 OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C666" s="1" t="s">
+        <v>3194</v>
+      </c>
+      <c r="D666" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E666" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H666" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I666" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="667" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A667" t="s">
+        <v>5320</v>
+      </c>
+      <c r="B667" t="str">
+        <f t="shared" si="2"/>
+        <v>RES THT 220 OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C667" s="1" t="s">
+        <v>3225</v>
+      </c>
+      <c r="D667" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E667" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H667" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I667" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="668" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A668" t="s">
+        <v>5321</v>
+      </c>
+      <c r="B668" t="str">
+        <f t="shared" si="2"/>
+        <v>RES THT 330 OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C668" s="1" t="s">
+        <v>3252</v>
+      </c>
+      <c r="D668" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E668" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H668" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I668" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="669" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A669" t="s">
+        <v>5322</v>
+      </c>
+      <c r="B669" t="str">
+        <f t="shared" si="2"/>
+        <v>RES THT 470 OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C669" s="1" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D669" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E669" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H669" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I669" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="670" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A670" t="s">
+        <v>5323</v>
+      </c>
+      <c r="B670" t="str">
+        <f t="shared" si="2"/>
+        <v>RES THT 560 OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C670" s="1" t="s">
+        <v>3274</v>
+      </c>
+      <c r="D670" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E670" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H670" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I670" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="671" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A671" t="s">
+        <v>5324</v>
+      </c>
+      <c r="B671" t="str">
+        <f t="shared" si="2"/>
+        <v>RES THT 680 OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C671" s="1" t="s">
+        <v>3347</v>
+      </c>
+      <c r="D671" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E671" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H671" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I671" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="672" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A672" t="s">
+        <v>5325</v>
+      </c>
+      <c r="B672" t="str">
+        <f t="shared" si="2"/>
+        <v>RES THT 820 OHM 1% 0.25W 0.3 AXIAL</v>
+      </c>
+      <c r="C672" s="1" t="s">
+        <v>3352</v>
+      </c>
+      <c r="D672" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E672" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H672" t="s">
+        <v>5234</v>
+      </c>
+      <c r="I672" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="673" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A673" t="s">
+        <v>5326</v>
+      </c>
+      <c r="B673" t="str">
+        <f t="shared" ref="B673:B686" si="3">CONCATENATE("RES THT ",C673," OHM ",D673," ",E673," 0.4 AXIAL")</f>
+        <v>RES THT 22 OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C673" s="1" t="s">
+        <v>3230</v>
+      </c>
+      <c r="D673" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E673" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H673" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I673" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="674" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A674" t="s">
+        <v>5327</v>
+      </c>
+      <c r="B674" t="str">
+        <f t="shared" si="3"/>
+        <v>RES THT 33 OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C674" s="1" t="s">
+        <v>3015</v>
+      </c>
+      <c r="D674" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E674" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H674" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I674" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="675" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A675" t="s">
+        <v>5328</v>
+      </c>
+      <c r="B675" t="str">
+        <f t="shared" si="3"/>
+        <v>RES THT 46 OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C675" s="1" t="s">
+        <v>5311</v>
+      </c>
+      <c r="D675" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E675" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H675" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I675" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="676" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A676" t="s">
+        <v>5329</v>
+      </c>
+      <c r="B676" t="str">
+        <f t="shared" si="3"/>
+        <v>RES THT 56 OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C676" s="1" t="s">
+        <v>3279</v>
+      </c>
+      <c r="D676" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E676" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H676" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I676" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="677" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A677" t="s">
+        <v>5330</v>
+      </c>
+      <c r="B677" t="str">
+        <f t="shared" si="3"/>
+        <v>RES THT 68 OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C677" s="1" t="s">
+        <v>3285</v>
+      </c>
+      <c r="D677" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E677" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H677" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I677" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="678" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A678" t="s">
+        <v>5331</v>
+      </c>
+      <c r="B678" t="str">
+        <f t="shared" si="3"/>
+        <v>RES THT 82 OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C678" s="1" t="s">
+        <v>3294</v>
+      </c>
+      <c r="D678" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E678" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H678" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I678" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="679" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A679" t="s">
+        <v>5332</v>
+      </c>
+      <c r="B679" t="str">
+        <f t="shared" si="3"/>
+        <v>RES THT 100 OHM 1% 1/4W 0.4 AXIAL</v>
+      </c>
+      <c r="C679" s="1" t="s">
+        <v>3160</v>
+      </c>
+      <c r="D679" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E679" t="s">
+        <v>5269</v>
+      </c>
+      <c r="H679" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I679" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="680" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A680" t="s">
+        <v>5333</v>
+      </c>
+      <c r="B680" t="str">
+        <f t="shared" si="3"/>
+        <v>RES THT 150 OHM 1% 1/4W 0.4 AXIAL</v>
+      </c>
+      <c r="C680" s="1" t="s">
+        <v>3194</v>
+      </c>
+      <c r="D680" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E680" t="s">
+        <v>5269</v>
+      </c>
+      <c r="H680" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I680" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="681" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A681" t="s">
+        <v>5334</v>
+      </c>
+      <c r="B681" t="str">
+        <f t="shared" si="3"/>
+        <v>RES THT 220 OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C681" s="1" t="s">
+        <v>3225</v>
+      </c>
+      <c r="D681" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E681" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H681" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I681" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="682" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A682" t="s">
+        <v>5335</v>
+      </c>
+      <c r="B682" t="str">
+        <f t="shared" si="3"/>
+        <v>RES THT 330 OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C682" s="1" t="s">
+        <v>3252</v>
+      </c>
+      <c r="D682" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E682" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H682" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I682" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="683" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A683" t="s">
+        <v>5336</v>
+      </c>
+      <c r="B683" t="str">
+        <f t="shared" si="3"/>
+        <v>RES THT 470 OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C683" s="1" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D683" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E683" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H683" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I683" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="684" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A684" t="s">
+        <v>5337</v>
+      </c>
+      <c r="B684" t="str">
+        <f t="shared" si="3"/>
+        <v>RES THT 560 OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C684" s="1" t="s">
+        <v>3274</v>
+      </c>
+      <c r="D684" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E684" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H684" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I684" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="685" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A685" t="s">
+        <v>5338</v>
+      </c>
+      <c r="B685" t="str">
+        <f t="shared" si="3"/>
+        <v>RES THT 680 OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C685" s="1" t="s">
+        <v>3347</v>
+      </c>
+      <c r="D685" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E685" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H685" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I685" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="686" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A686" t="s">
+        <v>5339</v>
+      </c>
+      <c r="B686" t="str">
+        <f t="shared" si="3"/>
+        <v>RES THT 820 OHM 1% 0.25W 0.4 AXIAL</v>
+      </c>
+      <c r="C686" s="1" t="s">
+        <v>3352</v>
+      </c>
+      <c r="D686" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E686" t="s">
+        <v>3004</v>
+      </c>
+      <c r="H686" t="s">
+        <v>5235</v>
+      </c>
+      <c r="I686" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="687" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A687" t="s">
+        <v>5362</v>
+      </c>
+      <c r="B687" t="str">
+        <f>CONCATENATE("RES THT ",C687," OHM ",D687," ",E687," 0.4 AXIAL")</f>
+        <v>RES THT 10M OHM 1% 0.6W 0.4 AXIAL</v>
+      </c>
+      <c r="C687" s="1" t="s">
+        <v>3797</v>
+      </c>
+      <c r="D687" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E687" t="s">
+        <v>5363</v>
+      </c>
+      <c r="F687" t="s">
+        <v>5366</v>
+      </c>
+      <c r="G687" t="s">
+        <v>5365</v>
+      </c>
+      <c r="H687" t="s">
+        <v>5364</v>
+      </c>
+      <c r="I687" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="688" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A688" t="s">
+        <v>5368</v>
+      </c>
+      <c r="B688" t="str">
+        <f>CONCATENATE("RES THT ",C688," OHM ",D688," ",E688," 0.4 AXIAL")</f>
+        <v>RES THT 1M OHM 1% 0.6W 0.4 AXIAL</v>
+      </c>
+      <c r="C688" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="D688" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E688" t="s">
+        <v>5363</v>
+      </c>
+      <c r="F688" t="s">
+        <v>5366</v>
+      </c>
+      <c r="G688" t="s">
+        <v>5367</v>
+      </c>
+      <c r="H688" t="s">
+        <v>5364</v>
+      </c>
+      <c r="I688" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="689" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A689" t="s">
+        <v>5369</v>
+      </c>
+      <c r="B689" t="str">
+        <f>CONCATENATE("RES THT ",C689," OHM ",D689," ",E689," 0.4 AXIAL")</f>
+        <v>RES THT 100M OHM 1% 0.5W 0.4 AXIAL</v>
+      </c>
+      <c r="C689" s="1" t="s">
+        <v>5370</v>
+      </c>
+      <c r="D689" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E689" t="s">
+        <v>4941</v>
+      </c>
+      <c r="F689" t="s">
+        <v>2440</v>
+      </c>
+      <c r="G689" t="s">
+        <v>5371</v>
+      </c>
+      <c r="H689" t="s">
+        <v>5372</v>
+      </c>
+      <c r="I689" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="690" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C690"/>
     </row>
-    <row r="693" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="693" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C693"/>
     </row>
-    <row r="695" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="695" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C695"/>
       <c r="D695"/>
     </row>
-    <row r="696" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="696" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C696"/>
       <c r="D696"/>
     </row>
-    <row r="697" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="697" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C697"/>
       <c r="D697"/>
     </row>
-    <row r="698" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="698" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C698"/>
       <c r="D698"/>
     </row>
-    <row r="699" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="699" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C699"/>
       <c r="D699"/>
     </row>
-    <row r="700" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="700" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C700"/>
       <c r="D700"/>
     </row>
-    <row r="701" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="701" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C701"/>
       <c r="D701"/>
     </row>
-    <row r="702" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="702" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C702"/>
       <c r="D702"/>
     </row>
-    <row r="703" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="703" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C703"/>
       <c r="D703"/>
     </row>
-    <row r="704" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="704" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C704"/>
       <c r="D704"/>
     </row>
@@ -34391,16 +36778,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.88671875" customWidth="1"/>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.88671875" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
@@ -34867,6 +37254,155 @@
         <v>0.42</v>
       </c>
     </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>5228</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5229</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5230</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5227</v>
+      </c>
+      <c r="F22">
+        <v>4093</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5346</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5381</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5382</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5227</v>
+      </c>
+      <c r="F23">
+        <v>4066</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>5351</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5352</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5353</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5227</v>
+      </c>
+      <c r="F24">
+        <v>40106</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>5373</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5374</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5375</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5376</v>
+      </c>
+      <c r="F25">
+        <v>4518</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>5377</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5378</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5379</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5376</v>
+      </c>
+      <c r="F26">
+        <v>4018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>5380</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5383</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5384</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5227</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4964</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>5385</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5386</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5387</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5227</v>
+      </c>
+      <c r="F28">
+        <v>4001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -34875,10 +37411,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35953,6 +38489,114 @@
         <v>2.99</v>
       </c>
     </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>5209</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5215</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5027</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4572</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5214</v>
+      </c>
+      <c r="G30" t="s">
+        <v>5212</v>
+      </c>
+      <c r="H30" t="s">
+        <v>5213</v>
+      </c>
+      <c r="I30" t="s">
+        <v>5210</v>
+      </c>
+      <c r="J30" t="s">
+        <v>4816</v>
+      </c>
+      <c r="K30" t="s">
+        <v>5211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>5259</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5261</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2101</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1225</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5262</v>
+      </c>
+      <c r="F31" t="s">
+        <v>2237</v>
+      </c>
+      <c r="G31" t="s">
+        <v>2253</v>
+      </c>
+      <c r="H31" t="s">
+        <v>2092</v>
+      </c>
+      <c r="I31" t="s">
+        <v>5263</v>
+      </c>
+      <c r="J31" t="s">
+        <v>5264</v>
+      </c>
+      <c r="K31" t="s">
+        <v>2236</v>
+      </c>
+      <c r="L31" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>5260</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5265</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2101</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1225</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5262</v>
+      </c>
+      <c r="F32" t="s">
+        <v>2245</v>
+      </c>
+      <c r="G32" t="s">
+        <v>2253</v>
+      </c>
+      <c r="H32" t="s">
+        <v>2092</v>
+      </c>
+      <c r="I32" t="s">
+        <v>5266</v>
+      </c>
+      <c r="J32" t="s">
+        <v>5267</v>
+      </c>
+      <c r="K32" t="s">
+        <v>2244</v>
+      </c>
+      <c r="L32" s="8">
+        <v>0.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -35961,10 +38605,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView topLeftCell="C31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N52" sqref="N52"/>
+    <sheetView topLeftCell="B34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37808,6 +40452,79 @@
       </c>
       <c r="M52" s="8">
         <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>5223</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>5222</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>5221</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>5220</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>5219</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>5218</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>5213</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>5216</v>
+      </c>
+      <c r="K53" t="s">
+        <v>4816</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>5217</v>
+      </c>
+      <c r="M53" s="8">
+        <v>6.23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>5395</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>5396</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>5397</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>5220</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>5398</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>4676</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>4869</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>5213</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>5399</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>5401</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>5400</v>
+      </c>
+      <c r="M54" s="8">
+        <v>2.19</v>
       </c>
     </row>
   </sheetData>
@@ -39126,7 +41843,7 @@
   <dimension ref="A1:K554"/>
   <sheetViews>
     <sheetView topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="A554" sqref="A554"/>
+      <selection activeCell="B555" sqref="B555"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57442,10 +60159,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M104"/>
+  <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="K105" sqref="K105"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="K107" sqref="K107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -60992,6 +63709,67 @@
       </c>
       <c r="M104" s="8">
         <v>2.41</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>5388</v>
+      </c>
+      <c r="B105" t="s">
+        <v>5389</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5390</v>
+      </c>
+      <c r="E105" t="s">
+        <v>70</v>
+      </c>
+      <c r="I105" t="s">
+        <v>5391</v>
+      </c>
+      <c r="J105" t="s">
+        <v>5392</v>
+      </c>
+      <c r="K105" t="s">
+        <v>5394</v>
+      </c>
+      <c r="L105" t="s">
+        <v>5393</v>
+      </c>
+      <c r="M105" s="8">
+        <v>4.62</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>5406</v>
+      </c>
+      <c r="B106" t="s">
+        <v>5407</v>
+      </c>
+      <c r="C106" t="s">
+        <v>5408</v>
+      </c>
+      <c r="E106" t="s">
+        <v>2265</v>
+      </c>
+      <c r="H106" t="s">
+        <v>5409</v>
+      </c>
+      <c r="I106" t="s">
+        <v>4917</v>
+      </c>
+      <c r="J106" t="s">
+        <v>5410</v>
+      </c>
+      <c r="K106" t="s">
+        <v>5411</v>
+      </c>
+      <c r="L106" t="s">
+        <v>5412</v>
+      </c>
+      <c r="M106" s="8">
+        <v>1.97</v>
       </c>
     </row>
   </sheetData>
@@ -61214,10 +63992,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -61605,6 +64383,9 @@
         <v>2.87</v>
       </c>
     </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G18" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -61613,10 +64394,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -62668,6 +65449,85 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>5343</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5344</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4286</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2948</v>
+      </c>
+      <c r="E31" t="s">
+        <v>70</v>
+      </c>
+      <c r="G31" t="s">
+        <v>2562</v>
+      </c>
+      <c r="H31" t="s">
+        <v>2521</v>
+      </c>
+      <c r="I31" t="s">
+        <v>2288</v>
+      </c>
+      <c r="J31" t="s">
+        <v>5345</v>
+      </c>
+      <c r="K31" t="s">
+        <v>4557</v>
+      </c>
+      <c r="L31" t="s">
+        <v>4289</v>
+      </c>
+      <c r="M31" s="8">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>5354</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5355</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5356</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2948</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5357</v>
+      </c>
+      <c r="F32" t="s">
+        <v>5358</v>
+      </c>
+      <c r="G32" t="s">
+        <v>5089</v>
+      </c>
+      <c r="H32" t="s">
+        <v>2521</v>
+      </c>
+      <c r="I32" t="s">
+        <v>4604</v>
+      </c>
+      <c r="J32" t="s">
+        <v>5359</v>
+      </c>
+      <c r="K32" t="s">
+        <v>5360</v>
+      </c>
+      <c r="L32" t="s">
+        <v>5361</v>
+      </c>
+      <c r="M32" s="8">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -62679,7 +65539,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -62877,10 +65737,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -63827,6 +66687,144 @@
         <v>7.75</v>
       </c>
     </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>5201</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5204</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4322</v>
+      </c>
+      <c r="D43" t="s">
+        <v>5202</v>
+      </c>
+      <c r="E43" t="s">
+        <v>2318</v>
+      </c>
+      <c r="F43" t="s">
+        <v>5203</v>
+      </c>
+      <c r="G43" s="8">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>5224</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5225</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5226</v>
+      </c>
+      <c r="E44" t="s">
+        <v>5227</v>
+      </c>
+      <c r="F44" t="s">
+        <v>5146</v>
+      </c>
+      <c r="G44" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>5253</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5258</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2092</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5254</v>
+      </c>
+      <c r="E45" t="s">
+        <v>5255</v>
+      </c>
+      <c r="F45" t="s">
+        <v>5256</v>
+      </c>
+      <c r="G45" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>5257</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5205</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2092</v>
+      </c>
+      <c r="D46" t="s">
+        <v>5206</v>
+      </c>
+      <c r="E46" t="s">
+        <v>5207</v>
+      </c>
+      <c r="F46" t="s">
+        <v>5208</v>
+      </c>
+      <c r="G46" s="8">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>5342</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5340</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5341</v>
+      </c>
+      <c r="E47" t="s">
+        <v>5227</v>
+      </c>
+      <c r="F47" t="s">
+        <v>4743</v>
+      </c>
+      <c r="G47" s="8">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>5347</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5348</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5349</v>
+      </c>
+      <c r="E48" t="s">
+        <v>5350</v>
+      </c>
+      <c r="F48">
+        <v>555</v>
+      </c>
+      <c r="G48" s="8">
+        <v>0.45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -63835,10 +66833,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -64401,6 +67399,29 @@
         <v>0.33</v>
       </c>
     </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>5405</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5402</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4905</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5403</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5404</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4952</v>
+      </c>
+      <c r="G27" s="8">
+        <v>0.49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
More updates for big pulse
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="8052" tabRatio="763"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14142" uniqueCount="5421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14168" uniqueCount="5434">
   <si>
     <t>Part Number</t>
   </si>
@@ -16269,9 +16274,6 @@
     <t>KEMET-SSR10HS-22026</t>
   </si>
   <si>
-    <t>cmd_0</t>
-  </si>
-  <si>
     <t>CONN-00042</t>
   </si>
   <si>
@@ -16294,6 +16296,48 @@
   </si>
   <si>
     <t>RES THT 0.075 OHM 1% 100W TO-247-2 Board Mounted</t>
+  </si>
+  <si>
+    <t>ANLG-00047</t>
+  </si>
+  <si>
+    <t>Opto-Triac, 800V peak voltage, 5300 Vrms isolation</t>
+  </si>
+  <si>
+    <t>VOT8121AG</t>
+  </si>
+  <si>
+    <t>VOT8121</t>
+  </si>
+  <si>
+    <t>DIP4_0.4</t>
+  </si>
+  <si>
+    <t>Dio, Silicon, 200mA, 1V, 75V, Axial 0.2"</t>
+  </si>
+  <si>
+    <t>1N4148</t>
+  </si>
+  <si>
+    <t>AXIAL_DIO_0.2</t>
+  </si>
+  <si>
+    <t>DIO-00053</t>
+  </si>
+  <si>
+    <t>PWREG-00031</t>
+  </si>
+  <si>
+    <t>REG, SW AC/DC Converter Module, Fixed 12V, 1.25A</t>
+  </si>
+  <si>
+    <t>86 - 264VAC</t>
+  </si>
+  <si>
+    <t>1.25A</t>
+  </si>
+  <si>
+    <t>VOF-15-12</t>
   </si>
 </sst>
 </file>
@@ -16303,7 +16347,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -16329,6 +16373,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -16657,7 +16707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J839"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A667" workbookViewId="0">
+    <sheetView topLeftCell="A667" workbookViewId="0">
       <selection activeCell="B691" sqref="B691"/>
     </sheetView>
   </sheetViews>
@@ -36210,10 +36260,10 @@
     </row>
     <row r="690" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A690" t="s">
-        <v>5418</v>
+        <v>5417</v>
       </c>
       <c r="B690" t="s">
-        <v>5420</v>
+        <v>5419</v>
       </c>
       <c r="C690" s="1" t="s">
         <v>5082</v>
@@ -36231,7 +36281,7 @@
         <v>5085</v>
       </c>
       <c r="H690" t="s">
-        <v>5419</v>
+        <v>5418</v>
       </c>
       <c r="I690" t="s">
         <v>12</v>
@@ -38655,10 +38705,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView topLeftCell="B34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40577,7 +40627,37 @@
         <v>2.19</v>
       </c>
     </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>5428</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>5425</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>2252</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>4868</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>2959</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>4869</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>5426</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>5427</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>4871</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -41884,13 +41964,13 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>5412</v>
+      </c>
+      <c r="B44" t="s">
         <v>5413</v>
       </c>
-      <c r="B44" t="s">
-        <v>5414</v>
-      </c>
       <c r="C44" t="s">
-        <v>5417</v>
+        <v>5416</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -41902,13 +41982,13 @@
         <v>4676</v>
       </c>
       <c r="G44" t="s">
-        <v>5415</v>
+        <v>5414</v>
       </c>
       <c r="H44">
         <v>7798</v>
       </c>
       <c r="I44" t="s">
-        <v>5416</v>
+        <v>5415</v>
       </c>
       <c r="J44" t="s">
         <v>2969</v>
@@ -60246,8 +60326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="K107" sqref="K107"/>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="L107" sqref="L107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -63851,7 +63931,7 @@
         <v>5411</v>
       </c>
       <c r="L106" t="s">
-        <v>5412</v>
+        <v>4915</v>
       </c>
       <c r="M106" s="8">
         <v>1.97</v>
@@ -64479,10 +64559,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -65611,6 +65691,44 @@
       </c>
       <c r="M32" s="8">
         <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>5429</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5430</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5431</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2171</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5432</v>
+      </c>
+      <c r="G33" t="s">
+        <v>5089</v>
+      </c>
+      <c r="H33" t="s">
+        <v>2521</v>
+      </c>
+      <c r="I33" t="s">
+        <v>4604</v>
+      </c>
+      <c r="J33" t="s">
+        <v>5433</v>
+      </c>
+      <c r="K33" t="s">
+        <v>5433</v>
+      </c>
+      <c r="L33" t="s">
+        <v>5361</v>
+      </c>
+      <c r="M33" s="8">
+        <v>19.41</v>
       </c>
     </row>
   </sheetData>
@@ -65822,10 +65940,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -66908,6 +67026,29 @@
       </c>
       <c r="G48" s="8">
         <v>0.45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>5420</v>
+      </c>
+      <c r="B49" t="s">
+        <v>5421</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2431</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5422</v>
+      </c>
+      <c r="E49" t="s">
+        <v>5424</v>
+      </c>
+      <c r="F49" t="s">
+        <v>5423</v>
+      </c>
+      <c r="G49" s="8">
+        <v>1.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add some more components
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14168" uniqueCount="5434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14215" uniqueCount="5460">
   <si>
     <t>Part Number</t>
   </si>
@@ -16338,6 +16338,84 @@
   </si>
   <si>
     <t>VOF-15-12</t>
+  </si>
+  <si>
+    <t>MAG-00105</t>
+  </si>
+  <si>
+    <t>Pulse Xfmr, 7.75mH, 28VuS, 2kV isolation</t>
+  </si>
+  <si>
+    <t>7.75mH</t>
+  </si>
+  <si>
+    <t>DA103JC</t>
+  </si>
+  <si>
+    <t>DA100J</t>
+  </si>
+  <si>
+    <t>xfmr_5</t>
+  </si>
+  <si>
+    <t>CAP-00553</t>
+  </si>
+  <si>
+    <t>Glennan Circuits Lab</t>
+  </si>
+  <si>
+    <t>CAP_RADIAL_0.4</t>
+  </si>
+  <si>
+    <t>1kV</t>
+  </si>
+  <si>
+    <t>CONN-00043</t>
+  </si>
+  <si>
+    <t>MOLEX_387207503</t>
+  </si>
+  <si>
+    <t>Barrier Blk, 3 Pos, 25A, 300V, 0.375" pitch</t>
+  </si>
+  <si>
+    <t>MOLEX_387207502</t>
+  </si>
+  <si>
+    <t>MOLEX_387207504</t>
+  </si>
+  <si>
+    <t>Barrier Blk, 2 Pos, 25A, 300V, 0.375" pitch</t>
+  </si>
+  <si>
+    <t>Barrier Blk, 4 Pos, 25A, 300V, 0.375" pitch</t>
+  </si>
+  <si>
+    <t>CONN-00044</t>
+  </si>
+  <si>
+    <t>CONN-00045</t>
+  </si>
+  <si>
+    <t>XSTR-00031</t>
+  </si>
+  <si>
+    <t>800V</t>
+  </si>
+  <si>
+    <t>10W</t>
+  </si>
+  <si>
+    <t>1.55V</t>
+  </si>
+  <si>
+    <t>T2535-800G-TR</t>
+  </si>
+  <si>
+    <t>triac_1</t>
+  </si>
+  <si>
+    <t>TRIAC, 25A, 800V, Vt 1.55V, D2PAK</t>
   </si>
 </sst>
 </file>
@@ -37511,10 +37589,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38695,6 +38773,44 @@
       </c>
       <c r="L32" s="8">
         <v>0.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>5453</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5459</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5454</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5156</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5455</v>
+      </c>
+      <c r="F33" t="s">
+        <v>5214</v>
+      </c>
+      <c r="G33" t="s">
+        <v>5456</v>
+      </c>
+      <c r="H33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I33" t="s">
+        <v>5457</v>
+      </c>
+      <c r="J33" t="s">
+        <v>5401</v>
+      </c>
+      <c r="K33" t="s">
+        <v>5458</v>
+      </c>
+      <c r="L33" s="8">
+        <v>2.84</v>
       </c>
     </row>
   </sheetData>
@@ -40665,10 +40781,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41997,6 +42113,111 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>5444</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5449</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2388</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>5156</v>
+      </c>
+      <c r="G45" t="s">
+        <v>2389</v>
+      </c>
+      <c r="H45">
+        <v>387207502</v>
+      </c>
+      <c r="I45" t="s">
+        <v>5447</v>
+      </c>
+      <c r="J45" t="s">
+        <v>2391</v>
+      </c>
+      <c r="K45" s="8">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>5451</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5446</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2388</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>5156</v>
+      </c>
+      <c r="G46" t="s">
+        <v>2389</v>
+      </c>
+      <c r="H46">
+        <v>387207503</v>
+      </c>
+      <c r="I46" t="s">
+        <v>5445</v>
+      </c>
+      <c r="J46" t="s">
+        <v>2384</v>
+      </c>
+      <c r="K46" s="8">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>5452</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5450</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2388</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>5156</v>
+      </c>
+      <c r="G47" t="s">
+        <v>2389</v>
+      </c>
+      <c r="H47">
+        <v>387207504</v>
+      </c>
+      <c r="I47" t="s">
+        <v>5448</v>
+      </c>
+      <c r="J47" t="s">
+        <v>2962</v>
+      </c>
+      <c r="K47" s="8">
+        <v>3.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -42005,10 +42226,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K554"/>
+  <dimension ref="A1:K555"/>
   <sheetViews>
     <sheetView topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="B555" sqref="B555"/>
+      <selection activeCell="E558" sqref="E558"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -60316,6 +60537,36 @@
         <v>2.41</v>
       </c>
     </row>
+    <row r="555" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A555" t="s">
+        <v>5440</v>
+      </c>
+      <c r="B555" t="str">
+        <f>CONCATENATE("CAP",", ",C555,", ",D555,", ",E555,", ",F555,", Radial 0.4inch")</f>
+        <v>CAP, 0.1uF, ±10%, 1kV, X7R, Radial 0.4inch</v>
+      </c>
+      <c r="C555" t="s">
+        <v>4679</v>
+      </c>
+      <c r="D555" t="s">
+        <v>4355</v>
+      </c>
+      <c r="E555" t="s">
+        <v>5443</v>
+      </c>
+      <c r="F555" t="s">
+        <v>20</v>
+      </c>
+      <c r="G555" t="s">
+        <v>5441</v>
+      </c>
+      <c r="I555" t="s">
+        <v>5442</v>
+      </c>
+      <c r="J555" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -60324,10 +60575,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M106"/>
+  <dimension ref="A1:M107"/>
   <sheetViews>
     <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="L107" sqref="L107"/>
+      <selection activeCell="H108" sqref="H108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -63935,6 +64186,32 @@
       </c>
       <c r="M106" s="8">
         <v>1.97</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>5434</v>
+      </c>
+      <c r="B107" t="s">
+        <v>5435</v>
+      </c>
+      <c r="C107" t="s">
+        <v>5436</v>
+      </c>
+      <c r="I107" t="s">
+        <v>21</v>
+      </c>
+      <c r="J107" t="s">
+        <v>5437</v>
+      </c>
+      <c r="K107" t="s">
+        <v>5438</v>
+      </c>
+      <c r="L107" t="s">
+        <v>5439</v>
+      </c>
+      <c r="M107" s="8">
+        <v>1.57</v>
       </c>
     </row>
   </sheetData>
@@ -64561,7 +64838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add some new parts, add some Power Supply snippits
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14239" uniqueCount="5475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14258" uniqueCount="5485">
   <si>
     <t>Part Number</t>
   </si>
@@ -16461,6 +16461,36 @@
   </si>
   <si>
     <t>24AA01</t>
+  </si>
+  <si>
+    <t>DIO-00054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dio, Schottky, 15A, 0.85V, 150V, TO-227 </t>
+  </si>
+  <si>
+    <t>0.85V</t>
+  </si>
+  <si>
+    <t>150V</t>
+  </si>
+  <si>
+    <t>15A</t>
+  </si>
+  <si>
+    <t>FSV15150V</t>
+  </si>
+  <si>
+    <t>TO-227-3</t>
+  </si>
+  <si>
+    <t>diode_sch_A12C3</t>
+  </si>
+  <si>
+    <t>CL32B106KMVNNWE</t>
+  </si>
+  <si>
+    <t>CAP-00554</t>
   </si>
 </sst>
 </file>
@@ -37003,7 +37033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -38903,10 +38933,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40852,6 +40882,41 @@
       </c>
       <c r="L55" s="2" t="s">
         <v>4869</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>5475</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>5476</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>5477</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>5478</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>5479</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>2092</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>5480</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>5481</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>5482</v>
+      </c>
+      <c r="M56" s="8">
+        <v>0.82</v>
       </c>
     </row>
   </sheetData>
@@ -42308,10 +42373,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K555"/>
+  <dimension ref="A1:K556"/>
   <sheetViews>
-    <sheetView topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="E558" sqref="E558"/>
+    <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
+      <selection activeCell="M545" sqref="M545"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -60647,6 +60712,42 @@
       </c>
       <c r="J555" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="556" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A556" t="s">
+        <v>5484</v>
+      </c>
+      <c r="B556" t="str">
+        <f>CONCATENATE("CAP",", ",C556,", ",D556,", ",E556,", ",F556,", 1210")</f>
+        <v>CAP, 10uF, ±10%, 63V, X7R, 1210</v>
+      </c>
+      <c r="C556" t="s">
+        <v>1582</v>
+      </c>
+      <c r="D556" t="s">
+        <v>4354</v>
+      </c>
+      <c r="E556" t="s">
+        <v>1842</v>
+      </c>
+      <c r="F556" t="s">
+        <v>20</v>
+      </c>
+      <c r="G556" t="s">
+        <v>5127</v>
+      </c>
+      <c r="H556" t="s">
+        <v>5483</v>
+      </c>
+      <c r="I556" t="s">
+        <v>4333</v>
+      </c>
+      <c r="J556" t="s">
+        <v>23</v>
+      </c>
+      <c r="K556" s="8">
+        <v>0.81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add LM5088 to DB.xlsx
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="8"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14605" uniqueCount="5677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14615" uniqueCount="5682">
   <si>
     <t>Part Number</t>
   </si>
@@ -17062,6 +17062,21 @@
   </si>
   <si>
     <t>Switch, SPDT, 120VAC/28VDC, 5A, Horizontal Slide Switch</t>
+  </si>
+  <si>
+    <t>PWREG-00035</t>
+  </si>
+  <si>
+    <t>REG CNTRL, SW Buck, LM5088</t>
+  </si>
+  <si>
+    <t>4.5-75V</t>
+  </si>
+  <si>
+    <t>50kHz-2.5MHz</t>
+  </si>
+  <si>
+    <t>LM5088</t>
   </si>
 </sst>
 </file>
@@ -66638,10 +66653,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67937,6 +67952,41 @@
       </c>
       <c r="M36" s="8">
         <v>51.11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>5677</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5678</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5679</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5680</v>
+      </c>
+      <c r="G37" t="s">
+        <v>72</v>
+      </c>
+      <c r="H37" t="s">
+        <v>73</v>
+      </c>
+      <c r="I37" t="s">
+        <v>2288</v>
+      </c>
+      <c r="J37" t="s">
+        <v>5681</v>
+      </c>
+      <c r="K37" t="s">
+        <v>5081</v>
+      </c>
+      <c r="L37" t="s">
+        <v>5681</v>
+      </c>
+      <c r="M37" s="8">
+        <v>3.53</v>
       </c>
     </row>
   </sheetData>
@@ -69315,7 +69365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add lorge power resistor
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14615" uniqueCount="5682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14622" uniqueCount="5691">
   <si>
     <t>Part Number</t>
   </si>
@@ -17077,6 +17077,33 @@
   </si>
   <si>
     <t>LM5088</t>
+  </si>
+  <si>
+    <t>CP_RADIAL_D6.3_P2.5_H12.5</t>
+  </si>
+  <si>
+    <t>CP_RADIAL_D10.0_P5.0_H14.0</t>
+  </si>
+  <si>
+    <t>CP_RADIAL_D12.5_P5.0_H22.0</t>
+  </si>
+  <si>
+    <t>CP_RADIAL_D12.5_P5.0_H27.0</t>
+  </si>
+  <si>
+    <t>RES-00700</t>
+  </si>
+  <si>
+    <t>RES SMD 0.003 OHM 1% 7W 2818</t>
+  </si>
+  <si>
+    <t>7W</t>
+  </si>
+  <si>
+    <t>WSHM28183L000FEA</t>
+  </si>
+  <si>
+    <t>CHIP_2818_VISHAY</t>
   </si>
 </sst>
 </file>
@@ -17449,8 +17476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J839"/>
   <sheetViews>
-    <sheetView topLeftCell="A676" workbookViewId="0">
-      <selection activeCell="G702" sqref="G702"/>
+    <sheetView tabSelected="1" topLeftCell="A676" workbookViewId="0">
+      <selection activeCell="H703" sqref="H703"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37373,8 +37400,36 @@
       </c>
     </row>
     <row r="702" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C702"/>
-      <c r="D702"/>
+      <c r="A702" t="s">
+        <v>5686</v>
+      </c>
+      <c r="B702" t="s">
+        <v>5687</v>
+      </c>
+      <c r="C702" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D702" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="E702" s="12" t="s">
+        <v>5688</v>
+      </c>
+      <c r="F702" t="s">
+        <v>2440</v>
+      </c>
+      <c r="G702" t="s">
+        <v>5689</v>
+      </c>
+      <c r="H702" t="s">
+        <v>5690</v>
+      </c>
+      <c r="I702" t="s">
+        <v>12</v>
+      </c>
+      <c r="J702" s="8">
+        <v>1.86</v>
+      </c>
     </row>
     <row r="703" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C703"/>
@@ -43686,8 +43741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K560"/>
   <sheetViews>
-    <sheetView topLeftCell="A533" workbookViewId="0">
-      <selection activeCell="B561" sqref="B561"/>
+    <sheetView topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="C213" sqref="C213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51159,7 +51214,7 @@
         <v>1671</v>
       </c>
       <c r="I226" t="s">
-        <v>2082</v>
+        <v>5682</v>
       </c>
       <c r="J226" t="s">
         <v>2080</v>
@@ -51192,7 +51247,7 @@
         <v>1672</v>
       </c>
       <c r="I227" t="s">
-        <v>2084</v>
+        <v>5683</v>
       </c>
       <c r="J227" t="s">
         <v>2080</v>
@@ -51225,7 +51280,7 @@
         <v>1673</v>
       </c>
       <c r="I228" t="s">
-        <v>2085</v>
+        <v>5684</v>
       </c>
       <c r="J228" t="s">
         <v>2080</v>
@@ -51258,7 +51313,7 @@
         <v>1674</v>
       </c>
       <c r="I229" t="s">
-        <v>2085</v>
+        <v>5685</v>
       </c>
       <c r="J229" t="s">
         <v>2080</v>
@@ -62215,8 +62270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="J98" sqref="J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -66655,8 +66710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add bourns SRP2313AA series footprint and 6.8uH inductor
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14622" uniqueCount="5691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14632" uniqueCount="5697">
   <si>
     <t>Part Number</t>
   </si>
@@ -17104,6 +17104,24 @@
   </si>
   <si>
     <t>CHIP_2818_VISHAY</t>
+  </si>
+  <si>
+    <t>MAG-00109</t>
+  </si>
+  <si>
+    <t>Ind, 6.8uH, 36A (32A sat.), 20%, 0.0031 Ohm</t>
+  </si>
+  <si>
+    <t>36A</t>
+  </si>
+  <si>
+    <t>3.1mOhm</t>
+  </si>
+  <si>
+    <t>SRP2313AA-6R8M</t>
+  </si>
+  <si>
+    <t>BOURNS_SRP2313AA</t>
   </si>
 </sst>
 </file>
@@ -17476,7 +17494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J839"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A676" workbookViewId="0">
+    <sheetView topLeftCell="A676" workbookViewId="0">
       <selection activeCell="H703" sqref="H703"/>
     </sheetView>
   </sheetViews>
@@ -62268,16 +62286,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N110"/>
+  <dimension ref="A1:N111"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="J98" sqref="J98"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="H112" sqref="H112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
@@ -66019,6 +66037,41 @@
       </c>
       <c r="M110" s="8">
         <v>5.35</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>5691</v>
+      </c>
+      <c r="B111" t="s">
+        <v>5692</v>
+      </c>
+      <c r="C111" t="s">
+        <v>1290</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E111" t="s">
+        <v>5693</v>
+      </c>
+      <c r="H111" t="s">
+        <v>5694</v>
+      </c>
+      <c r="I111" t="s">
+        <v>4890</v>
+      </c>
+      <c r="J111" t="s">
+        <v>5695</v>
+      </c>
+      <c r="K111" t="s">
+        <v>5696</v>
+      </c>
+      <c r="L111" t="s">
+        <v>1383</v>
+      </c>
+      <c r="M111" s="8">
+        <v>8.91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add parts for ROV buck converter clamping network
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14632" uniqueCount="5697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14650" uniqueCount="5707">
   <si>
     <t>Part Number</t>
   </si>
@@ -17122,6 +17122,36 @@
   </si>
   <si>
     <t>BOURNS_SRP2313AA</t>
+  </si>
+  <si>
+    <t>XSTR-00035</t>
+  </si>
+  <si>
+    <t>XSTR NPN, 10A, 50V, Vce 0.18V, DPAK</t>
+  </si>
+  <si>
+    <t>950mW</t>
+  </si>
+  <si>
+    <t>0.18V</t>
+  </si>
+  <si>
+    <t>2SC6017-TL-E</t>
+  </si>
+  <si>
+    <t>npn-bjt_BCE</t>
+  </si>
+  <si>
+    <t>RES-00701</t>
+  </si>
+  <si>
+    <t>RES SMD 6.8 OHM 5% 1.5W 2512</t>
+  </si>
+  <si>
+    <t>1.5W</t>
+  </si>
+  <si>
+    <t>RPC2512JT6R80</t>
   </si>
 </sst>
 </file>
@@ -17495,7 +17525,7 @@
   <dimension ref="A1:J839"/>
   <sheetViews>
     <sheetView topLeftCell="A676" workbookViewId="0">
-      <selection activeCell="H703" sqref="H703"/>
+      <selection activeCell="B704" sqref="B704"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37450,8 +37480,36 @@
       </c>
     </row>
     <row r="703" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C703"/>
-      <c r="D703"/>
+      <c r="A703" t="s">
+        <v>5703</v>
+      </c>
+      <c r="B703" t="s">
+        <v>5704</v>
+      </c>
+      <c r="C703" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="D703" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="E703" s="12" t="s">
+        <v>5705</v>
+      </c>
+      <c r="F703" t="s">
+        <v>2301</v>
+      </c>
+      <c r="G703" t="s">
+        <v>5706</v>
+      </c>
+      <c r="H703" t="s">
+        <v>2374</v>
+      </c>
+      <c r="I703" t="s">
+        <v>12</v>
+      </c>
+      <c r="J703" s="8">
+        <v>0.56999999999999995</v>
+      </c>
     </row>
     <row r="704" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C704"/>
@@ -38675,10 +38733,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40010,6 +40068,44 @@
         <v>0.8</v>
       </c>
     </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>5697</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5698</v>
+      </c>
+      <c r="C37" t="s">
+        <v>944</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4904</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5699</v>
+      </c>
+      <c r="F37" t="s">
+        <v>2237</v>
+      </c>
+      <c r="G37" t="s">
+        <v>5700</v>
+      </c>
+      <c r="H37" t="s">
+        <v>2092</v>
+      </c>
+      <c r="I37" t="s">
+        <v>5701</v>
+      </c>
+      <c r="J37" t="s">
+        <v>2414</v>
+      </c>
+      <c r="K37" t="s">
+        <v>5702</v>
+      </c>
+      <c r="L37" s="8">
+        <v>0.73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -40020,8 +40116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43759,8 +43855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K560"/>
   <sheetViews>
-    <sheetView topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="C213" sqref="C213"/>
+    <sheetView topLeftCell="A530" workbookViewId="0">
+      <selection activeCell="H289" sqref="H289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -62288,8 +62384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="H112" sqref="H112"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add 470uF Al Electrolytic cap with higher ripple current rating
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="11"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14650" uniqueCount="5707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14659" uniqueCount="5710">
   <si>
     <t>Part Number</t>
   </si>
@@ -17152,6 +17152,15 @@
   </si>
   <si>
     <t>RPC2512JT6R80</t>
+  </si>
+  <si>
+    <t>CAP-00559</t>
+  </si>
+  <si>
+    <t>UHV1V471MPD</t>
+  </si>
+  <si>
+    <t>CP_RADIAL_D10.0_P5.0_H17.5</t>
   </si>
 </sst>
 </file>
@@ -40116,7 +40125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
@@ -43853,10 +43862,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K560"/>
+  <dimension ref="A1:K561"/>
   <sheetViews>
-    <sheetView topLeftCell="A530" workbookViewId="0">
-      <selection activeCell="H289" sqref="H289"/>
+    <sheetView tabSelected="1" topLeftCell="A532" workbookViewId="0">
+      <selection activeCell="B562" sqref="B562"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -62372,6 +62381,42 @@
       </c>
       <c r="K560" s="8">
         <v>0.7</v>
+      </c>
+    </row>
+    <row r="561" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A561" t="s">
+        <v>5707</v>
+      </c>
+      <c r="B561" t="str">
+        <f>CONCATENATE("CAP",", ",C561,", ",D561,", ",E561,", ",F561,", 6000hrs at 105°C")</f>
+        <v>CAP, 470uF, ±20%, 35V, Al, 6000hrs at 105°C</v>
+      </c>
+      <c r="C561" t="s">
+        <v>1826</v>
+      </c>
+      <c r="D561" t="s">
+        <v>4328</v>
+      </c>
+      <c r="E561" t="s">
+        <v>949</v>
+      </c>
+      <c r="F561" t="s">
+        <v>1843</v>
+      </c>
+      <c r="G561" t="s">
+        <v>1556</v>
+      </c>
+      <c r="H561" t="s">
+        <v>5708</v>
+      </c>
+      <c r="I561" t="s">
+        <v>5709</v>
+      </c>
+      <c r="J561" t="s">
+        <v>2080</v>
+      </c>
+      <c r="K561" s="8">
+        <v>0.76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 4.7 ohm power resistor
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14659" uniqueCount="5710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14666" uniqueCount="5713">
   <si>
     <t>Part Number</t>
   </si>
@@ -17161,6 +17161,15 @@
   </si>
   <si>
     <t>CP_RADIAL_D10.0_P5.0_H17.5</t>
+  </si>
+  <si>
+    <t>RES-00702</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7 OHM 5% 2W 2512</t>
+  </si>
+  <si>
+    <t>CRM2512-JW-4R7ELF</t>
   </si>
 </sst>
 </file>
@@ -17533,8 +17542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J839"/>
   <sheetViews>
-    <sheetView topLeftCell="A676" workbookViewId="0">
-      <selection activeCell="B704" sqref="B704"/>
+    <sheetView tabSelected="1" topLeftCell="A676" workbookViewId="0">
+      <selection activeCell="B705" sqref="B705"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37521,8 +37530,36 @@
       </c>
     </row>
     <row r="704" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C704"/>
-      <c r="D704"/>
+      <c r="A704" t="s">
+        <v>5710</v>
+      </c>
+      <c r="B704" t="s">
+        <v>5711</v>
+      </c>
+      <c r="C704" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="D704" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="E704" s="12" t="s">
+        <v>2375</v>
+      </c>
+      <c r="F704" t="s">
+        <v>4890</v>
+      </c>
+      <c r="G704" t="s">
+        <v>5712</v>
+      </c>
+      <c r="H704" t="s">
+        <v>2374</v>
+      </c>
+      <c r="I704" t="s">
+        <v>12</v>
+      </c>
+      <c r="J704" s="8">
+        <v>0.56999999999999995</v>
+      </c>
     </row>
     <row r="705" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C705"/>
@@ -43864,8 +43901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K561"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A532" workbookViewId="0">
-      <selection activeCell="B562" sqref="B562"/>
+    <sheetView topLeftCell="A532" workbookViewId="0">
+      <selection activeCell="B561" sqref="B561"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add new high-current large gauge screwless terminal block
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="10"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14666" uniqueCount="5713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14673" uniqueCount="5716">
   <si>
     <t>Part Number</t>
   </si>
@@ -17170,6 +17170,15 @@
   </si>
   <si>
     <t>n-mosfet_GxSD</t>
+  </si>
+  <si>
+    <t>CONN-00053</t>
+  </si>
+  <si>
+    <t>Terminal Blk, 2 Pos, 20A, 5.0mm Pitch, Screwless, 12-24AWG</t>
+  </si>
+  <si>
+    <t>PHOENIX_SPT_5.00MM_2x1</t>
   </si>
 </sst>
 </file>
@@ -38781,8 +38790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42188,10 +42197,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="L55" sqref="L55"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43889,6 +43898,41 @@
       </c>
       <c r="K54" s="8">
         <v>0.34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>5713</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5714</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2383</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" t="s">
+        <v>4601</v>
+      </c>
+      <c r="G55" t="s">
+        <v>2381</v>
+      </c>
+      <c r="H55">
+        <v>1991095</v>
+      </c>
+      <c r="I55" t="s">
+        <v>5715</v>
+      </c>
+      <c r="J55" t="s">
+        <v>2391</v>
+      </c>
+      <c r="K55" s="8">
+        <v>1.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Honeywell HMC5983 Compass IC
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14673" uniqueCount="5716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14679" uniqueCount="5721">
   <si>
     <t>Part Number</t>
   </si>
@@ -17179,6 +17179,21 @@
   </si>
   <si>
     <t>PHOENIX_SPT_5.00MM_2x1</t>
+  </si>
+  <si>
+    <t>MISC-00034</t>
+  </si>
+  <si>
+    <t>IC, 3-Axis Digital Compass, I2C and SPI, HMC5983</t>
+  </si>
+  <si>
+    <t>Honeywell</t>
+  </si>
+  <si>
+    <t>HMC5983</t>
+  </si>
+  <si>
+    <t>LCC-16-3x3mm</t>
   </si>
 </sst>
 </file>
@@ -42199,8 +42214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -69693,10 +69708,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -70466,6 +70481,29 @@
         <v>3.93</v>
       </c>
     </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>5716</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5717</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5718</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5719</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5720</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5719</v>
+      </c>
+      <c r="G36" s="8">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add 10-pin IDC connector
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="2" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14679" uniqueCount="5721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14747" uniqueCount="5762">
   <si>
     <t>Part Number</t>
   </si>
@@ -17194,6 +17194,129 @@
   </si>
   <si>
     <t>LCC-16-3x3mm</t>
+  </si>
+  <si>
+    <t>1.05V</t>
+  </si>
+  <si>
+    <t>600V</t>
+  </si>
+  <si>
+    <t>GBJ2506-F</t>
+  </si>
+  <si>
+    <t>PWREG-00036</t>
+  </si>
+  <si>
+    <t>85~305VAC</t>
+  </si>
+  <si>
+    <t>MEANWELL_IRM-15</t>
+  </si>
+  <si>
+    <t>Bridge, 25A, 1.05V, 600V, GBJ</t>
+  </si>
+  <si>
+    <t>SIP-4-GBJ</t>
+  </si>
+  <si>
+    <t>DIO-00055</t>
+  </si>
+  <si>
+    <t>DIO-00056</t>
+  </si>
+  <si>
+    <t>ANLG-00050</t>
+  </si>
+  <si>
+    <t>IC, Current Source, Adjustable, 3%, LM334, SOIC-8</t>
+  </si>
+  <si>
+    <t>LM334MX/NOPB</t>
+  </si>
+  <si>
+    <t>LM334</t>
+  </si>
+  <si>
+    <t>RES-00703</t>
+  </si>
+  <si>
+    <t>CHV2512-FX-1004ELF</t>
+  </si>
+  <si>
+    <t>RES SMD 1M OHM 1% 1W 2512, High Voltage, Thick Film</t>
+  </si>
+  <si>
+    <t>ANLG-00051</t>
+  </si>
+  <si>
+    <t>IC, Voltage Reference, 1.235V, LM285-1.2</t>
+  </si>
+  <si>
+    <t>LM285D-1-2</t>
+  </si>
+  <si>
+    <t>LM285</t>
+  </si>
+  <si>
+    <t>MISC-00035</t>
+  </si>
+  <si>
+    <t>UCC27517DBVR</t>
+  </si>
+  <si>
+    <t>UCC2751x</t>
+  </si>
+  <si>
+    <t>IC, Gate Driver, Single Channel High-Speed, 4A Source and Sink</t>
+  </si>
+  <si>
+    <t>ANLG-00052</t>
+  </si>
+  <si>
+    <t>Comparator, Dual, 40ns, Push-Pull Output, 2.7-5.5V</t>
+  </si>
+  <si>
+    <t>comp-d_0</t>
+  </si>
+  <si>
+    <t>TLV3202AID</t>
+  </si>
+  <si>
+    <t>MISC-00036</t>
+  </si>
+  <si>
+    <t>Fuse Holder, Cartridge, 5x20mm, 500V 10A</t>
+  </si>
+  <si>
+    <t>0031.8211</t>
+  </si>
+  <si>
+    <t>SCHURTER_0031-8211</t>
+  </si>
+  <si>
+    <t>IRM-15-12</t>
+  </si>
+  <si>
+    <t>Module, AC-DC Isolated, 12V 1.25A</t>
+  </si>
+  <si>
+    <t>CONN-00054</t>
+  </si>
+  <si>
+    <t>Header, 10-pin IDC, 2.54mm Pitch</t>
+  </si>
+  <si>
+    <t>CNC Tech</t>
+  </si>
+  <si>
+    <t>3020-10-0100-00</t>
+  </si>
+  <si>
+    <t>CNC_TECH_3020-10-0100-XX</t>
+  </si>
+  <si>
+    <t>conn-5x2_0</t>
   </si>
 </sst>
 </file>
@@ -17566,8 +17689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J839"/>
   <sheetViews>
-    <sheetView topLeftCell="A676" workbookViewId="0">
-      <selection activeCell="B705" sqref="B705"/>
+    <sheetView topLeftCell="A682" workbookViewId="0">
+      <selection activeCell="B706" sqref="B706"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37585,67 +37708,95 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="705" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C705"/>
-      <c r="D705"/>
-    </row>
-    <row r="706" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="705" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A705" t="s">
+        <v>5735</v>
+      </c>
+      <c r="B705" t="s">
+        <v>5737</v>
+      </c>
+      <c r="C705" t="s">
+        <v>791</v>
+      </c>
+      <c r="D705" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="E705" s="12" t="s">
+        <v>2611</v>
+      </c>
+      <c r="F705" t="s">
+        <v>4890</v>
+      </c>
+      <c r="G705" t="s">
+        <v>5736</v>
+      </c>
+      <c r="H705" t="s">
+        <v>2374</v>
+      </c>
+      <c r="I705" t="s">
+        <v>12</v>
+      </c>
+      <c r="J705" s="8">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="706" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C706"/>
       <c r="D706"/>
     </row>
-    <row r="707" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="707" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C707"/>
       <c r="D707"/>
     </row>
-    <row r="708" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="708" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C708"/>
       <c r="D708"/>
     </row>
-    <row r="709" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="709" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C709"/>
       <c r="D709"/>
     </row>
-    <row r="710" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="710" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C710"/>
       <c r="D710"/>
     </row>
-    <row r="711" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="711" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C711"/>
       <c r="D711"/>
     </row>
-    <row r="712" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="712" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C712"/>
       <c r="D712"/>
     </row>
-    <row r="713" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="713" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C713"/>
       <c r="D713"/>
     </row>
-    <row r="714" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="714" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C714"/>
       <c r="D714"/>
     </row>
-    <row r="715" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="715" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C715"/>
       <c r="D715"/>
     </row>
-    <row r="716" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="716" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C716"/>
       <c r="D716"/>
     </row>
-    <row r="717" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="717" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C717"/>
       <c r="D717"/>
     </row>
-    <row r="718" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="718" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C718"/>
       <c r="D718"/>
     </row>
-    <row r="719" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="719" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C719"/>
       <c r="D719"/>
     </row>
-    <row r="720" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="720" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C720"/>
       <c r="D720"/>
     </row>
@@ -38806,7 +38957,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40184,10 +40335,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M57"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42175,6 +42326,9 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>5729</v>
+      </c>
       <c r="B57" s="2" t="s">
         <v>5644</v>
       </c>
@@ -42201,6 +42355,41 @@
       </c>
       <c r="M57" s="8">
         <v>0.43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>5730</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>5727</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>5721</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>5722</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>5139</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>4546</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>5150</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>5723</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>5728</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>4548</v>
+      </c>
+      <c r="M58" s="8">
+        <v>1.33</v>
       </c>
     </row>
   </sheetData>
@@ -42212,10 +42401,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43948,6 +44137,41 @@
       </c>
       <c r="K55" s="8">
         <v>1.23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>5756</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5757</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2397</v>
+      </c>
+      <c r="D56">
+        <v>5</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>70</v>
+      </c>
+      <c r="G56" t="s">
+        <v>5758</v>
+      </c>
+      <c r="H56" t="s">
+        <v>5759</v>
+      </c>
+      <c r="I56" t="s">
+        <v>5760</v>
+      </c>
+      <c r="J56" t="s">
+        <v>5761</v>
+      </c>
+      <c r="K56" s="8">
+        <v>0.57999999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -66998,10 +67222,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68332,6 +68556,44 @@
       </c>
       <c r="M37" s="8">
         <v>3.53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>5724</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5755</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5725</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2171</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5415</v>
+      </c>
+      <c r="G38" t="s">
+        <v>5072</v>
+      </c>
+      <c r="H38" t="s">
+        <v>2520</v>
+      </c>
+      <c r="I38" t="s">
+        <v>4786</v>
+      </c>
+      <c r="J38" t="s">
+        <v>5754</v>
+      </c>
+      <c r="K38" t="s">
+        <v>5726</v>
+      </c>
+      <c r="L38" t="s">
+        <v>5344</v>
+      </c>
+      <c r="M38" s="8">
+        <v>10.85</v>
       </c>
     </row>
   </sheetData>
@@ -68543,10 +68805,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -69700,6 +69962,72 @@
         <v>0.45</v>
       </c>
     </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>5731</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5732</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D52" t="s">
+        <v>5733</v>
+      </c>
+      <c r="E52" t="s">
+        <v>4470</v>
+      </c>
+      <c r="F52" t="s">
+        <v>5734</v>
+      </c>
+      <c r="G52" s="8">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>5738</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5739</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5740</v>
+      </c>
+      <c r="E53" t="s">
+        <v>4470</v>
+      </c>
+      <c r="F53" t="s">
+        <v>5741</v>
+      </c>
+      <c r="G53" s="8">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>5746</v>
+      </c>
+      <c r="B54" t="s">
+        <v>5747</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D54" t="s">
+        <v>5749</v>
+      </c>
+      <c r="E54" t="s">
+        <v>4470</v>
+      </c>
+      <c r="F54" t="s">
+        <v>5748</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -69708,10 +70036,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -70504,6 +70832,52 @@
         <v>35</v>
       </c>
     </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>5742</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5745</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5743</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2522</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5744</v>
+      </c>
+      <c r="G37" s="8">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>5750</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5751</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5374</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>5752</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5753</v>
+      </c>
+      <c r="F38" t="s">
+        <v>3369</v>
+      </c>
+      <c r="G38" s="8">
+        <v>0.91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add 2-pin 0.1in header
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14747" uniqueCount="5762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14770" uniqueCount="5771">
   <si>
     <t>Part Number</t>
   </si>
@@ -17317,6 +17317,33 @@
   </si>
   <si>
     <t>conn-5x2_0</t>
+  </si>
+  <si>
+    <t>CAP-00560</t>
+  </si>
+  <si>
+    <t>CC1206KKX7RZBB102</t>
+  </si>
+  <si>
+    <t>RPC2512JT33R0</t>
+  </si>
+  <si>
+    <t>RES SMD 33 OHM 5% 1.5W 2512</t>
+  </si>
+  <si>
+    <t>RES-00704</t>
+  </si>
+  <si>
+    <t>CONN-00055</t>
+  </si>
+  <si>
+    <t>Header, 2x1, 0.1"</t>
+  </si>
+  <si>
+    <t>TSW-102-07-F-S</t>
+  </si>
+  <si>
+    <t>HDDR_2x1_0</t>
   </si>
 </sst>
 </file>
@@ -17690,7 +17717,7 @@
   <dimension ref="A1:J839"/>
   <sheetViews>
     <sheetView topLeftCell="A682" workbookViewId="0">
-      <selection activeCell="B706" sqref="B706"/>
+      <selection activeCell="C708" sqref="C708"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37741,8 +37768,36 @@
       </c>
     </row>
     <row r="706" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C706"/>
-      <c r="D706"/>
+      <c r="A706" t="s">
+        <v>5766</v>
+      </c>
+      <c r="B706" t="s">
+        <v>5765</v>
+      </c>
+      <c r="C706" s="1">
+        <v>33</v>
+      </c>
+      <c r="D706" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="E706" s="12" t="s">
+        <v>5704</v>
+      </c>
+      <c r="F706" t="s">
+        <v>2301</v>
+      </c>
+      <c r="G706" t="s">
+        <v>5764</v>
+      </c>
+      <c r="H706" t="s">
+        <v>2374</v>
+      </c>
+      <c r="I706" t="s">
+        <v>12</v>
+      </c>
+      <c r="J706" s="8">
+        <v>0.56999999999999995</v>
+      </c>
     </row>
     <row r="707" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C707"/>
@@ -42401,10 +42456,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44174,6 +44229,38 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>5767</v>
+      </c>
+      <c r="B57" t="s">
+        <v>5768</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2397</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="G57" t="s">
+        <v>4738</v>
+      </c>
+      <c r="H57" t="s">
+        <v>5769</v>
+      </c>
+      <c r="I57" t="s">
+        <v>5770</v>
+      </c>
+      <c r="J57" t="s">
+        <v>2391</v>
+      </c>
+      <c r="K57" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -44182,10 +44269,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K561"/>
+  <dimension ref="A1:K562"/>
   <sheetViews>
-    <sheetView topLeftCell="A532" workbookViewId="0">
-      <selection activeCell="B561" sqref="B561"/>
+    <sheetView topLeftCell="A538" workbookViewId="0">
+      <selection activeCell="I563" sqref="I563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -62737,6 +62824,42 @@
       </c>
       <c r="K561" s="8">
         <v>0.76</v>
+      </c>
+    </row>
+    <row r="562" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A562" t="s">
+        <v>5762</v>
+      </c>
+      <c r="B562" t="str">
+        <f>CONCATENATE("CAP",", ",C562,", ",D562,", ",E562,", ",F562,", 1206")</f>
+        <v>CAP, 1000pF, ±10%, 630V, X7R, 1206</v>
+      </c>
+      <c r="C562" t="s">
+        <v>931</v>
+      </c>
+      <c r="D562" t="s">
+        <v>4345</v>
+      </c>
+      <c r="E562" t="s">
+        <v>4805</v>
+      </c>
+      <c r="F562" t="s">
+        <v>20</v>
+      </c>
+      <c r="G562" t="s">
+        <v>2612</v>
+      </c>
+      <c r="H562" t="s">
+        <v>5763</v>
+      </c>
+      <c r="I562" t="s">
+        <v>1472</v>
+      </c>
+      <c r="J562" t="s">
+        <v>23</v>
+      </c>
+      <c r="K562" s="8">
+        <v>0.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Early February update, add many parts for ROV control board
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="2" activeTab="12"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14770" uniqueCount="5771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="5850">
   <si>
     <t>Part Number</t>
   </si>
@@ -17344,6 +17344,243 @@
   </si>
   <si>
     <t>HDDR_2x1_0</t>
+  </si>
+  <si>
+    <t>CONN-00056</t>
+  </si>
+  <si>
+    <t>Card-Edge Connector, 200-pin DDR2 SODIMM, Vertical</t>
+  </si>
+  <si>
+    <t>2040910-1</t>
+  </si>
+  <si>
+    <t>DDR2-SODIMM-V</t>
+  </si>
+  <si>
+    <t>conn-100x2_0</t>
+  </si>
+  <si>
+    <t>ECS-240-8-47-CKM-TR</t>
+  </si>
+  <si>
+    <t>ECS Inc.</t>
+  </si>
+  <si>
+    <t>10ppm</t>
+  </si>
+  <si>
+    <t>24M</t>
+  </si>
+  <si>
+    <t>XTAL, 24MHz, 8pF, 10ppm</t>
+  </si>
+  <si>
+    <t>OSC-00004</t>
+  </si>
+  <si>
+    <t>ECS-240-8-47</t>
+  </si>
+  <si>
+    <t>osc_xtal_4p_1-3</t>
+  </si>
+  <si>
+    <t>NDS9407</t>
+  </si>
+  <si>
+    <t>XSTR-00036</t>
+  </si>
+  <si>
+    <t>XSTR PFET, 3A, 60V, 2.5W, SOIC-8</t>
+  </si>
+  <si>
+    <t>p-mosfet-SSSGDDDD_1</t>
+  </si>
+  <si>
+    <t>PWREG-00037</t>
+  </si>
+  <si>
+    <t>REG, Linear, Fixed 3.3V, 500mA, Low-Noise with Enable Pin</t>
+  </si>
+  <si>
+    <t>LP5912-1.8DRVR</t>
+  </si>
+  <si>
+    <t>LP5912-3.3DRVR</t>
+  </si>
+  <si>
+    <t>WSON-6_0</t>
+  </si>
+  <si>
+    <t>LP5912</t>
+  </si>
+  <si>
+    <t>3.5 - 6.5V</t>
+  </si>
+  <si>
+    <t>PWREG-00038</t>
+  </si>
+  <si>
+    <t>REG, Linear, Fixed 1.8V, 500mA, Low-Noise with Enable Pin</t>
+  </si>
+  <si>
+    <t>2.0 - 6.5V</t>
+  </si>
+  <si>
+    <t>LM3880</t>
+  </si>
+  <si>
+    <t>LM3880MF-1AE/NOPB</t>
+  </si>
+  <si>
+    <t>PWREG-00039</t>
+  </si>
+  <si>
+    <t>IC, Three-Rail Power Supply Sequencer, LM3880</t>
+  </si>
+  <si>
+    <t>2.7 - 5.5V</t>
+  </si>
+  <si>
+    <t>IFACE-00018</t>
+  </si>
+  <si>
+    <t>LAN9514</t>
+  </si>
+  <si>
+    <t>QFN-64-EP</t>
+  </si>
+  <si>
+    <t>LAN9514-JZX</t>
+  </si>
+  <si>
+    <t>IC, USB 2.0 Hub and Ethernet 10/100 Controller, LAN9514</t>
+  </si>
+  <si>
+    <t>CONN-00057</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>RJMG1BD3B8K1ANR</t>
+  </si>
+  <si>
+    <t>AMPHENOL_RJMG1B</t>
+  </si>
+  <si>
+    <t>amphenol-RJMG1B</t>
+  </si>
+  <si>
+    <t>RJ45 Modular Mag-Jack, 8P8C, 10/100 Base-T</t>
+  </si>
+  <si>
+    <t>CONN-00058</t>
+  </si>
+  <si>
+    <t>USB-A Jack, USB 2.0, SMD Right-Angle</t>
+  </si>
+  <si>
+    <t>1932638-3</t>
+  </si>
+  <si>
+    <t>TE_1932638-3</t>
+  </si>
+  <si>
+    <t>usb_a</t>
+  </si>
+  <si>
+    <t>MAG-00110</t>
+  </si>
+  <si>
+    <t>Fe Bead, 120 @ 100MHz, 3A, 0805</t>
+  </si>
+  <si>
+    <t>30mOhm</t>
+  </si>
+  <si>
+    <t>RC0603FR-0749R9L</t>
+  </si>
+  <si>
+    <t>1/10W</t>
+  </si>
+  <si>
+    <t>RES SMD 49.9 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RES-00705</t>
+  </si>
+  <si>
+    <t>PWREG-00040</t>
+  </si>
+  <si>
+    <t>REG, Synchronous Buck, 2A, 4.5-17V Input, SOT-23-6, TPS562201</t>
+  </si>
+  <si>
+    <t>4.5 - 17V</t>
+  </si>
+  <si>
+    <t>0.76 - 7V</t>
+  </si>
+  <si>
+    <t>580kHz</t>
+  </si>
+  <si>
+    <t>TPS562201DDCR</t>
+  </si>
+  <si>
+    <t>TPS56220x</t>
+  </si>
+  <si>
+    <t>MAG-00111</t>
+  </si>
+  <si>
+    <t>Ind, 3.3uH, 3.3A (3.8A sat.), 0.027 Ohm</t>
+  </si>
+  <si>
+    <t>3.3A</t>
+  </si>
+  <si>
+    <t>27mOhm</t>
+  </si>
+  <si>
+    <t>BOURNS_SRN5040</t>
+  </si>
+  <si>
+    <t>SRN5040-3R3M</t>
+  </si>
+  <si>
+    <t>SRN5040-2R2Y</t>
+  </si>
+  <si>
+    <t>21mOhm</t>
+  </si>
+  <si>
+    <t>3.5A</t>
+  </si>
+  <si>
+    <t>30%</t>
+  </si>
+  <si>
+    <t>MAG-00112</t>
+  </si>
+  <si>
+    <t>Ind, 2.2uH, 3.5A (4.6A sat.), 0.027 Ohm</t>
+  </si>
+  <si>
+    <t>DIO-00057</t>
+  </si>
+  <si>
+    <t>DLPT05</t>
+  </si>
+  <si>
+    <t>DLPT05-7-F</t>
+  </si>
+  <si>
+    <t>TVS, Steering (Rail-Rail), 9.8V Clamping, 17A Peak Pulse, SOT-23</t>
+  </si>
+  <si>
+    <t>6.0V</t>
   </si>
 </sst>
 </file>
@@ -17717,7 +17954,7 @@
   <dimension ref="A1:J839"/>
   <sheetViews>
     <sheetView topLeftCell="A682" workbookViewId="0">
-      <selection activeCell="C708" sqref="C708"/>
+      <selection activeCell="B708" sqref="B708"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37800,8 +38037,36 @@
       </c>
     </row>
     <row r="707" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C707"/>
-      <c r="D707"/>
+      <c r="A707" t="s">
+        <v>5825</v>
+      </c>
+      <c r="B707" t="s">
+        <v>5824</v>
+      </c>
+      <c r="C707" s="1">
+        <v>49.9</v>
+      </c>
+      <c r="D707" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="E707" s="12" t="s">
+        <v>5823</v>
+      </c>
+      <c r="F707" t="s">
+        <v>2612</v>
+      </c>
+      <c r="G707" t="s">
+        <v>5822</v>
+      </c>
+      <c r="H707" t="s">
+        <v>35</v>
+      </c>
+      <c r="I707" t="s">
+        <v>12</v>
+      </c>
+      <c r="J707" s="8">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="708" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C708"/>
@@ -39009,10 +39274,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40382,6 +40647,44 @@
         <v>0.73</v>
       </c>
     </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>5785</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5786</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2121</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2120</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5664</v>
+      </c>
+      <c r="F38" t="s">
+        <v>2268</v>
+      </c>
+      <c r="G38" t="s">
+        <v>2254</v>
+      </c>
+      <c r="H38" t="s">
+        <v>2092</v>
+      </c>
+      <c r="I38" t="s">
+        <v>5784</v>
+      </c>
+      <c r="J38" t="s">
+        <v>4470</v>
+      </c>
+      <c r="K38" t="s">
+        <v>5787</v>
+      </c>
+      <c r="L38" s="8">
+        <v>0.78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -40390,10 +40693,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M58"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42447,6 +42750,35 @@
         <v>1.33</v>
       </c>
     </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>5845</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>5848</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>5849</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>2944</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>5150</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>5847</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>2182</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>5846</v>
+      </c>
+      <c r="M59" s="8">
+        <v>0.38</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -42456,10 +42788,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44259,6 +44591,99 @@
       </c>
       <c r="K57" s="8">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>5771</v>
+      </c>
+      <c r="B58" t="s">
+        <v>5772</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5517</v>
+      </c>
+      <c r="D58">
+        <v>100</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="G58" t="s">
+        <v>2979</v>
+      </c>
+      <c r="H58" t="s">
+        <v>5773</v>
+      </c>
+      <c r="I58" t="s">
+        <v>5774</v>
+      </c>
+      <c r="J58" t="s">
+        <v>5775</v>
+      </c>
+      <c r="K58" s="8">
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>5808</v>
+      </c>
+      <c r="B59" t="s">
+        <v>5813</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5809</v>
+      </c>
+      <c r="G59" t="s">
+        <v>2908</v>
+      </c>
+      <c r="H59" t="s">
+        <v>5810</v>
+      </c>
+      <c r="I59" t="s">
+        <v>5811</v>
+      </c>
+      <c r="J59" t="s">
+        <v>5812</v>
+      </c>
+      <c r="K59" s="8">
+        <v>3.92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>5814</v>
+      </c>
+      <c r="B60" t="s">
+        <v>5815</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5809</v>
+      </c>
+      <c r="D60">
+        <v>4</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" t="s">
+        <v>70</v>
+      </c>
+      <c r="G60" t="s">
+        <v>2979</v>
+      </c>
+      <c r="H60" t="s">
+        <v>5816</v>
+      </c>
+      <c r="I60" t="s">
+        <v>5817</v>
+      </c>
+      <c r="J60" t="s">
+        <v>5818</v>
+      </c>
+      <c r="K60" s="8">
+        <v>1.52</v>
       </c>
     </row>
   </sheetData>
@@ -62870,10 +63295,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N111"/>
+  <dimension ref="A1:N114"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -66656,6 +67081,108 @@
       </c>
       <c r="M111" s="8">
         <v>8.91</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>5819</v>
+      </c>
+      <c r="B112" t="s">
+        <v>5820</v>
+      </c>
+      <c r="E112" t="s">
+        <v>2120</v>
+      </c>
+      <c r="F112">
+        <v>120</v>
+      </c>
+      <c r="G112" t="s">
+        <v>37</v>
+      </c>
+      <c r="H112" t="s">
+        <v>5821</v>
+      </c>
+      <c r="I112" t="s">
+        <v>2421</v>
+      </c>
+      <c r="J112">
+        <v>742792023</v>
+      </c>
+      <c r="K112" t="s">
+        <v>11</v>
+      </c>
+      <c r="L112" t="s">
+        <v>36</v>
+      </c>
+      <c r="M112" s="8">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>5833</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5834</v>
+      </c>
+      <c r="C113" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E113" t="s">
+        <v>5835</v>
+      </c>
+      <c r="H113" t="s">
+        <v>5836</v>
+      </c>
+      <c r="I113" t="s">
+        <v>4890</v>
+      </c>
+      <c r="J113" t="s">
+        <v>5838</v>
+      </c>
+      <c r="K113" t="s">
+        <v>5837</v>
+      </c>
+      <c r="L113" t="s">
+        <v>1383</v>
+      </c>
+      <c r="M113" s="8">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>5843</v>
+      </c>
+      <c r="B114" t="s">
+        <v>5844</v>
+      </c>
+      <c r="C114" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>5842</v>
+      </c>
+      <c r="E114" t="s">
+        <v>5841</v>
+      </c>
+      <c r="H114" t="s">
+        <v>5840</v>
+      </c>
+      <c r="I114" t="s">
+        <v>4890</v>
+      </c>
+      <c r="J114" t="s">
+        <v>5839</v>
+      </c>
+      <c r="K114" t="s">
+        <v>5837</v>
+      </c>
+      <c r="L114" t="s">
+        <v>1383</v>
       </c>
     </row>
   </sheetData>
@@ -66898,10 +67425,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67337,6 +67864,29 @@
         <v>0.54</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>5803</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5807</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5806</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5805</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5804</v>
+      </c>
+      <c r="G20" s="8">
+        <v>5.54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -67345,10 +67895,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68719,6 +69269,149 @@
         <v>10.85</v>
       </c>
     </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>5788</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5789</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5794</v>
+      </c>
+      <c r="D39" t="s">
+        <v>4766</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1226</v>
+      </c>
+      <c r="G39" t="s">
+        <v>2561</v>
+      </c>
+      <c r="H39" t="s">
+        <v>2520</v>
+      </c>
+      <c r="I39" t="s">
+        <v>2288</v>
+      </c>
+      <c r="J39" t="s">
+        <v>5791</v>
+      </c>
+      <c r="K39" t="s">
+        <v>5792</v>
+      </c>
+      <c r="L39" t="s">
+        <v>5793</v>
+      </c>
+      <c r="M39" s="8">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>5795</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5796</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5797</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5013</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1226</v>
+      </c>
+      <c r="G40" t="s">
+        <v>2561</v>
+      </c>
+      <c r="H40" t="s">
+        <v>2520</v>
+      </c>
+      <c r="I40" t="s">
+        <v>2288</v>
+      </c>
+      <c r="J40" t="s">
+        <v>5790</v>
+      </c>
+      <c r="K40" t="s">
+        <v>5792</v>
+      </c>
+      <c r="L40" t="s">
+        <v>5793</v>
+      </c>
+      <c r="M40" s="8">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>5800</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5801</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5802</v>
+      </c>
+      <c r="I41" t="s">
+        <v>2288</v>
+      </c>
+      <c r="J41" t="s">
+        <v>5799</v>
+      </c>
+      <c r="K41" t="s">
+        <v>2559</v>
+      </c>
+      <c r="L41" t="s">
+        <v>5798</v>
+      </c>
+      <c r="M41" s="8">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>5826</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5827</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5828</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5829</v>
+      </c>
+      <c r="E42" t="s">
+        <v>2107</v>
+      </c>
+      <c r="F42" t="s">
+        <v>5830</v>
+      </c>
+      <c r="G42" t="s">
+        <v>72</v>
+      </c>
+      <c r="H42" t="s">
+        <v>73</v>
+      </c>
+      <c r="I42" t="s">
+        <v>2288</v>
+      </c>
+      <c r="J42" t="s">
+        <v>5831</v>
+      </c>
+      <c r="K42" t="s">
+        <v>2559</v>
+      </c>
+      <c r="L42" t="s">
+        <v>5832</v>
+      </c>
+      <c r="M42" s="8">
+        <v>0.68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -68727,10 +69420,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68745,10 +69438,11 @@
     <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -68782,8 +69476,11 @@
       <c r="K1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="8" t="s">
+        <v>4495</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -68818,7 +69515,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2922</v>
       </c>
@@ -68853,7 +69550,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4759</v>
       </c>
@@ -68888,7 +69585,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4760</v>
       </c>
@@ -68918,6 +69615,44 @@
       </c>
       <c r="K5" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5781</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5780</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5779</v>
+      </c>
+      <c r="D6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5778</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5778</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5777</v>
+      </c>
+      <c r="I6" t="s">
+        <v>5776</v>
+      </c>
+      <c r="J6" t="s">
+        <v>5782</v>
+      </c>
+      <c r="K6" t="s">
+        <v>5783</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add PCI Express socket and card edge connector
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="11"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="2" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="5850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14918" uniqueCount="5858">
   <si>
     <t>Part Number</t>
   </si>
@@ -17349,9 +17349,6 @@
     <t>CONN-00056</t>
   </si>
   <si>
-    <t>Card-Edge Connector, 200-pin DDR2 SODIMM, Vertical</t>
-  </si>
-  <si>
     <t>2040910-1</t>
   </si>
   <si>
@@ -17581,6 +17578,33 @@
   </si>
   <si>
     <t>6.0V</t>
+  </si>
+  <si>
+    <t>CONN-00059</t>
+  </si>
+  <si>
+    <t>Card-Edge Socket, 200-pin DDR2 SODIMM, Vertical</t>
+  </si>
+  <si>
+    <t>AMPHENOL_10061913-XX0</t>
+  </si>
+  <si>
+    <t>10061913-100PLF</t>
+  </si>
+  <si>
+    <t>Card-Edge Socket, 36-pin PCI Express, Vertical SMD</t>
+  </si>
+  <si>
+    <t>CONN-00060</t>
+  </si>
+  <si>
+    <t>Card Edge</t>
+  </si>
+  <si>
+    <t>Card-Edge Contacts, 36-pin PCI Express, 1.0mm Pitch</t>
+  </si>
+  <si>
+    <t>PCIE_CARD_EDGE_36_1.0MM</t>
   </si>
 </sst>
 </file>
@@ -38038,10 +38062,10 @@
     </row>
     <row r="707" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A707" t="s">
-        <v>5825</v>
+        <v>5824</v>
       </c>
       <c r="B707" t="s">
-        <v>5824</v>
+        <v>5823</v>
       </c>
       <c r="C707" s="1">
         <v>49.9</v>
@@ -38050,13 +38074,13 @@
         <v>0.01</v>
       </c>
       <c r="E707" s="12" t="s">
-        <v>5823</v>
+        <v>5822</v>
       </c>
       <c r="F707" t="s">
         <v>2612</v>
       </c>
       <c r="G707" t="s">
-        <v>5822</v>
+        <v>5821</v>
       </c>
       <c r="H707" t="s">
         <v>35</v>
@@ -40649,10 +40673,10 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>5784</v>
+      </c>
+      <c r="B38" t="s">
         <v>5785</v>
-      </c>
-      <c r="B38" t="s">
-        <v>5786</v>
       </c>
       <c r="C38" t="s">
         <v>2121</v>
@@ -40673,13 +40697,13 @@
         <v>2092</v>
       </c>
       <c r="I38" t="s">
-        <v>5784</v>
+        <v>5783</v>
       </c>
       <c r="J38" t="s">
         <v>4470</v>
       </c>
       <c r="K38" t="s">
-        <v>5787</v>
+        <v>5786</v>
       </c>
       <c r="L38" s="8">
         <v>0.78</v>
@@ -40695,7 +40719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
@@ -42752,13 +42776,13 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>5845</v>
+        <v>5844</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>5847</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>5848</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>5849</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>2944</v>
@@ -42767,13 +42791,13 @@
         <v>5150</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>5847</v>
+        <v>5846</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>2182</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>5846</v>
+        <v>5845</v>
       </c>
       <c r="M59" s="8">
         <v>0.38</v>
@@ -42788,10 +42812,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44598,7 +44622,7 @@
         <v>5771</v>
       </c>
       <c r="B58" t="s">
-        <v>5772</v>
+        <v>5850</v>
       </c>
       <c r="C58" t="s">
         <v>5517</v>
@@ -44613,13 +44637,13 @@
         <v>2979</v>
       </c>
       <c r="H58" t="s">
+        <v>5772</v>
+      </c>
+      <c r="I58" t="s">
         <v>5773</v>
       </c>
-      <c r="I58" t="s">
+      <c r="J58" t="s">
         <v>5774</v>
-      </c>
-      <c r="J58" t="s">
-        <v>5775</v>
       </c>
       <c r="K58" s="8">
         <v>5.43</v>
@@ -44627,25 +44651,25 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>5807</v>
+      </c>
+      <c r="B59" t="s">
+        <v>5812</v>
+      </c>
+      <c r="C59" t="s">
         <v>5808</v>
-      </c>
-      <c r="B59" t="s">
-        <v>5813</v>
-      </c>
-      <c r="C59" t="s">
-        <v>5809</v>
       </c>
       <c r="G59" t="s">
         <v>2908</v>
       </c>
       <c r="H59" t="s">
+        <v>5809</v>
+      </c>
+      <c r="I59" t="s">
         <v>5810</v>
       </c>
-      <c r="I59" t="s">
+      <c r="J59" t="s">
         <v>5811</v>
-      </c>
-      <c r="J59" t="s">
-        <v>5812</v>
       </c>
       <c r="K59" s="8">
         <v>3.92</v>
@@ -44653,13 +44677,13 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>5813</v>
+      </c>
+      <c r="B60" t="s">
         <v>5814</v>
       </c>
-      <c r="B60" t="s">
-        <v>5815</v>
-      </c>
       <c r="C60" t="s">
-        <v>5809</v>
+        <v>5808</v>
       </c>
       <c r="D60">
         <v>4</v>
@@ -44674,16 +44698,80 @@
         <v>2979</v>
       </c>
       <c r="H60" t="s">
+        <v>5815</v>
+      </c>
+      <c r="I60" t="s">
         <v>5816</v>
       </c>
-      <c r="I60" t="s">
+      <c r="J60" t="s">
         <v>5817</v>
-      </c>
-      <c r="J60" t="s">
-        <v>5818</v>
       </c>
       <c r="K60" s="8">
         <v>1.52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>5849</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5853</v>
+      </c>
+      <c r="C61" t="s">
+        <v>5517</v>
+      </c>
+      <c r="D61">
+        <v>18</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61" t="s">
+        <v>70</v>
+      </c>
+      <c r="G61" t="s">
+        <v>2908</v>
+      </c>
+      <c r="H61" t="s">
+        <v>5852</v>
+      </c>
+      <c r="I61" t="s">
+        <v>5851</v>
+      </c>
+      <c r="J61" t="s">
+        <v>2455</v>
+      </c>
+      <c r="K61" s="8">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>5854</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5856</v>
+      </c>
+      <c r="C62" t="s">
+        <v>5855</v>
+      </c>
+      <c r="D62">
+        <v>18</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="F62" t="s">
+        <v>70</v>
+      </c>
+      <c r="I62" t="s">
+        <v>5857</v>
+      </c>
+      <c r="J62" t="s">
+        <v>2455</v>
+      </c>
+      <c r="K62" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -67085,10 +67173,10 @@
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
+        <v>5818</v>
+      </c>
+      <c r="B112" t="s">
         <v>5819</v>
-      </c>
-      <c r="B112" t="s">
-        <v>5820</v>
       </c>
       <c r="E112" t="s">
         <v>2120</v>
@@ -67100,7 +67188,7 @@
         <v>37</v>
       </c>
       <c r="H112" t="s">
-        <v>5821</v>
+        <v>5820</v>
       </c>
       <c r="I112" t="s">
         <v>2421</v>
@@ -67120,10 +67208,10 @@
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
+        <v>5832</v>
+      </c>
+      <c r="B113" t="s">
         <v>5833</v>
-      </c>
-      <c r="B113" t="s">
-        <v>5834</v>
       </c>
       <c r="C113" t="s">
         <v>1288</v>
@@ -67132,19 +67220,19 @@
         <v>1284</v>
       </c>
       <c r="E113" t="s">
+        <v>5834</v>
+      </c>
+      <c r="H113" t="s">
         <v>5835</v>
-      </c>
-      <c r="H113" t="s">
-        <v>5836</v>
       </c>
       <c r="I113" t="s">
         <v>4890</v>
       </c>
       <c r="J113" t="s">
-        <v>5838</v>
+        <v>5837</v>
       </c>
       <c r="K113" t="s">
-        <v>5837</v>
+        <v>5836</v>
       </c>
       <c r="L113" t="s">
         <v>1383</v>
@@ -67155,31 +67243,31 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
+        <v>5842</v>
+      </c>
+      <c r="B114" t="s">
         <v>5843</v>
-      </c>
-      <c r="B114" t="s">
-        <v>5844</v>
       </c>
       <c r="C114" t="s">
         <v>1287</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>5842</v>
+        <v>5841</v>
       </c>
       <c r="E114" t="s">
-        <v>5841</v>
+        <v>5840</v>
       </c>
       <c r="H114" t="s">
-        <v>5840</v>
+        <v>5839</v>
       </c>
       <c r="I114" t="s">
         <v>4890</v>
       </c>
       <c r="J114" t="s">
-        <v>5839</v>
+        <v>5838</v>
       </c>
       <c r="K114" t="s">
-        <v>5837</v>
+        <v>5836</v>
       </c>
       <c r="L114" t="s">
         <v>1383</v>
@@ -67866,22 +67954,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>5803</v>
+        <v>5802</v>
       </c>
       <c r="B20" t="s">
-        <v>5807</v>
+        <v>5806</v>
       </c>
       <c r="C20" t="s">
         <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>5806</v>
+        <v>5805</v>
       </c>
       <c r="E20" t="s">
-        <v>5805</v>
+        <v>5804</v>
       </c>
       <c r="F20" t="s">
-        <v>5804</v>
+        <v>5803</v>
       </c>
       <c r="G20" s="8">
         <v>5.54</v>
@@ -69271,13 +69359,13 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>5787</v>
+      </c>
+      <c r="B39" t="s">
         <v>5788</v>
       </c>
-      <c r="B39" t="s">
-        <v>5789</v>
-      </c>
       <c r="C39" t="s">
-        <v>5794</v>
+        <v>5793</v>
       </c>
       <c r="D39" t="s">
         <v>4766</v>
@@ -69295,13 +69383,13 @@
         <v>2288</v>
       </c>
       <c r="J39" t="s">
+        <v>5790</v>
+      </c>
+      <c r="K39" t="s">
         <v>5791</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>5792</v>
-      </c>
-      <c r="L39" t="s">
-        <v>5793</v>
       </c>
       <c r="M39" s="8">
         <v>1.2</v>
@@ -69309,13 +69397,13 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>5794</v>
+      </c>
+      <c r="B40" t="s">
         <v>5795</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>5796</v>
-      </c>
-      <c r="C40" t="s">
-        <v>5797</v>
       </c>
       <c r="D40" t="s">
         <v>5013</v>
@@ -69333,13 +69421,13 @@
         <v>2288</v>
       </c>
       <c r="J40" t="s">
-        <v>5790</v>
+        <v>5789</v>
       </c>
       <c r="K40" t="s">
+        <v>5791</v>
+      </c>
+      <c r="L40" t="s">
         <v>5792</v>
-      </c>
-      <c r="L40" t="s">
-        <v>5793</v>
       </c>
       <c r="M40" s="8">
         <v>1.2</v>
@@ -69347,25 +69435,25 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>5799</v>
+      </c>
+      <c r="B41" t="s">
         <v>5800</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>5801</v>
-      </c>
-      <c r="C41" t="s">
-        <v>5802</v>
       </c>
       <c r="I41" t="s">
         <v>2288</v>
       </c>
       <c r="J41" t="s">
-        <v>5799</v>
+        <v>5798</v>
       </c>
       <c r="K41" t="s">
         <v>2559</v>
       </c>
       <c r="L41" t="s">
-        <v>5798</v>
+        <v>5797</v>
       </c>
       <c r="M41" s="8">
         <v>1.35</v>
@@ -69373,22 +69461,22 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>5825</v>
+      </c>
+      <c r="B42" t="s">
         <v>5826</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>5827</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>5828</v>
-      </c>
-      <c r="D42" t="s">
-        <v>5829</v>
       </c>
       <c r="E42" t="s">
         <v>2107</v>
       </c>
       <c r="F42" t="s">
-        <v>5830</v>
+        <v>5829</v>
       </c>
       <c r="G42" t="s">
         <v>72</v>
@@ -69400,13 +69488,13 @@
         <v>2288</v>
       </c>
       <c r="J42" t="s">
-        <v>5831</v>
+        <v>5830</v>
       </c>
       <c r="K42" t="s">
         <v>2559</v>
       </c>
       <c r="L42" t="s">
-        <v>5832</v>
+        <v>5831</v>
       </c>
       <c r="M42" s="8">
         <v>0.68</v>
@@ -69619,13 +69707,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5781</v>
+        <v>5780</v>
       </c>
       <c r="B6" t="s">
-        <v>5780</v>
+        <v>5779</v>
       </c>
       <c r="C6" t="s">
-        <v>5779</v>
+        <v>5778</v>
       </c>
       <c r="D6" t="s">
         <v>80</v>
@@ -69634,22 +69722,22 @@
         <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>5778</v>
+        <v>5777</v>
       </c>
       <c r="G6" t="s">
-        <v>5778</v>
+        <v>5777</v>
       </c>
       <c r="H6" t="s">
-        <v>5777</v>
+        <v>5776</v>
       </c>
       <c r="I6" t="s">
-        <v>5776</v>
+        <v>5775</v>
       </c>
       <c r="J6" t="s">
+        <v>5781</v>
+      </c>
+      <c r="K6" t="s">
         <v>5782</v>
-      </c>
-      <c r="K6" t="s">
-        <v>5783</v>
       </c>
       <c r="L6" s="8">
         <v>0.79</v>

</xml_diff>

<commit_message>
DDR1 & DDR2 SODIMM connectors and card-edge contacts
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14918" uniqueCount="5858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14960" uniqueCount="5884">
   <si>
     <t>Part Number</t>
   </si>
@@ -17352,9 +17352,6 @@
     <t>2040910-1</t>
   </si>
   <si>
-    <t>DDR2-SODIMM-V</t>
-  </si>
-  <si>
     <t>conn-100x2_0</t>
   </si>
   <si>
@@ -17583,9 +17580,6 @@
     <t>CONN-00059</t>
   </si>
   <si>
-    <t>Card-Edge Socket, 200-pin DDR2 SODIMM, Vertical</t>
-  </si>
-  <si>
     <t>AMPHENOL_10061913-XX0</t>
   </si>
   <si>
@@ -17605,6 +17599,90 @@
   </si>
   <si>
     <t>PCIE_CARD_EDGE_36_1.0MM</t>
+  </si>
+  <si>
+    <t>OSC-00005</t>
+  </si>
+  <si>
+    <t>XTAL, 25MHz, 20pF, 20ppm</t>
+  </si>
+  <si>
+    <t>25M</t>
+  </si>
+  <si>
+    <t>20pF</t>
+  </si>
+  <si>
+    <t>ECS-250-20-33-JTN-TR</t>
+  </si>
+  <si>
+    <t>ECS-32</t>
+  </si>
+  <si>
+    <t>osc_xtal_4p_1-4</t>
+  </si>
+  <si>
+    <t>CONN-00061</t>
+  </si>
+  <si>
+    <t>Flat-Flex</t>
+  </si>
+  <si>
+    <t>Flat-Flex Cable Connector, Vertical, 15-Pos, 1.0mm Pitch SMD</t>
+  </si>
+  <si>
+    <t>1-1734248-5</t>
+  </si>
+  <si>
+    <t>TE_1-1734248-5</t>
+  </si>
+  <si>
+    <t>PCF8574A</t>
+  </si>
+  <si>
+    <t>PCF8574ADWR</t>
+  </si>
+  <si>
+    <t>IFACE-00019</t>
+  </si>
+  <si>
+    <t>IC, Remote 8-bit IO Expander, I2C 100kHz, PCF8574A</t>
+  </si>
+  <si>
+    <t>DDR1-SODIMM-V</t>
+  </si>
+  <si>
+    <t>CONN-00062</t>
+  </si>
+  <si>
+    <t>CONN-00063</t>
+  </si>
+  <si>
+    <t>DDR1-SODIMM-CARD-EDGE</t>
+  </si>
+  <si>
+    <t>DDR2-SODIMM-CARD-EDGE</t>
+  </si>
+  <si>
+    <t>Card-Edge, DDR1 SODIMM (2.5V), 200-pin</t>
+  </si>
+  <si>
+    <t>Card-Edge, DDR2 SODIMM (1.8V), 200-pin</t>
+  </si>
+  <si>
+    <t>CONN-00064</t>
+  </si>
+  <si>
+    <t>TE_1473005-1</t>
+  </si>
+  <si>
+    <t>1473005-1</t>
+  </si>
+  <si>
+    <t>Card-Edge Socket, DDR2 SODIMM (1.8V) 200-pin , Right-Angle</t>
+  </si>
+  <si>
+    <t>Card-Edge Socket, DDR1 SODIMM (2.5V), 200-pin, Vertical</t>
   </si>
 </sst>
 </file>
@@ -38062,10 +38140,10 @@
     </row>
     <row r="707" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A707" t="s">
-        <v>5824</v>
+        <v>5823</v>
       </c>
       <c r="B707" t="s">
-        <v>5823</v>
+        <v>5822</v>
       </c>
       <c r="C707" s="1">
         <v>49.9</v>
@@ -38074,13 +38152,13 @@
         <v>0.01</v>
       </c>
       <c r="E707" s="12" t="s">
-        <v>5822</v>
+        <v>5821</v>
       </c>
       <c r="F707" t="s">
         <v>2612</v>
       </c>
       <c r="G707" t="s">
-        <v>5821</v>
+        <v>5820</v>
       </c>
       <c r="H707" t="s">
         <v>35</v>
@@ -40673,10 +40751,10 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>5783</v>
+      </c>
+      <c r="B38" t="s">
         <v>5784</v>
-      </c>
-      <c r="B38" t="s">
-        <v>5785</v>
       </c>
       <c r="C38" t="s">
         <v>2121</v>
@@ -40697,13 +40775,13 @@
         <v>2092</v>
       </c>
       <c r="I38" t="s">
-        <v>5783</v>
+        <v>5782</v>
       </c>
       <c r="J38" t="s">
         <v>4470</v>
       </c>
       <c r="K38" t="s">
-        <v>5786</v>
+        <v>5785</v>
       </c>
       <c r="L38" s="8">
         <v>0.78</v>
@@ -42776,13 +42854,13 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>5844</v>
+        <v>5843</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>5846</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>5847</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>5848</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>2944</v>
@@ -42791,13 +42869,13 @@
         <v>5150</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>5846</v>
+        <v>5845</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>2182</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>5845</v>
+        <v>5844</v>
       </c>
       <c r="M59" s="8">
         <v>0.38</v>
@@ -42812,10 +42890,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44622,7 +44700,7 @@
         <v>5771</v>
       </c>
       <c r="B58" t="s">
-        <v>5850</v>
+        <v>5883</v>
       </c>
       <c r="C58" t="s">
         <v>5517</v>
@@ -44640,10 +44718,10 @@
         <v>5772</v>
       </c>
       <c r="I58" t="s">
+        <v>5872</v>
+      </c>
+      <c r="J58" t="s">
         <v>5773</v>
-      </c>
-      <c r="J58" t="s">
-        <v>5774</v>
       </c>
       <c r="K58" s="8">
         <v>5.43</v>
@@ -44651,25 +44729,25 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>5806</v>
+      </c>
+      <c r="B59" t="s">
+        <v>5811</v>
+      </c>
+      <c r="C59" t="s">
         <v>5807</v>
-      </c>
-      <c r="B59" t="s">
-        <v>5812</v>
-      </c>
-      <c r="C59" t="s">
-        <v>5808</v>
       </c>
       <c r="G59" t="s">
         <v>2908</v>
       </c>
       <c r="H59" t="s">
+        <v>5808</v>
+      </c>
+      <c r="I59" t="s">
         <v>5809</v>
       </c>
-      <c r="I59" t="s">
+      <c r="J59" t="s">
         <v>5810</v>
-      </c>
-      <c r="J59" t="s">
-        <v>5811</v>
       </c>
       <c r="K59" s="8">
         <v>3.92</v>
@@ -44677,13 +44755,13 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>5812</v>
+      </c>
+      <c r="B60" t="s">
         <v>5813</v>
       </c>
-      <c r="B60" t="s">
-        <v>5814</v>
-      </c>
       <c r="C60" t="s">
-        <v>5808</v>
+        <v>5807</v>
       </c>
       <c r="D60">
         <v>4</v>
@@ -44698,13 +44776,13 @@
         <v>2979</v>
       </c>
       <c r="H60" t="s">
+        <v>5814</v>
+      </c>
+      <c r="I60" t="s">
         <v>5815</v>
       </c>
-      <c r="I60" t="s">
+      <c r="J60" t="s">
         <v>5816</v>
-      </c>
-      <c r="J60" t="s">
-        <v>5817</v>
       </c>
       <c r="K60" s="8">
         <v>1.52</v>
@@ -44712,10 +44790,10 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>5849</v>
+        <v>5848</v>
       </c>
       <c r="B61" t="s">
-        <v>5853</v>
+        <v>5851</v>
       </c>
       <c r="C61" t="s">
         <v>5517</v>
@@ -44733,10 +44811,10 @@
         <v>2908</v>
       </c>
       <c r="H61" t="s">
-        <v>5852</v>
+        <v>5850</v>
       </c>
       <c r="I61" t="s">
-        <v>5851</v>
+        <v>5849</v>
       </c>
       <c r="J61" t="s">
         <v>2455</v>
@@ -44747,13 +44825,13 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>5852</v>
+      </c>
+      <c r="B62" t="s">
         <v>5854</v>
       </c>
-      <c r="B62" t="s">
-        <v>5856</v>
-      </c>
       <c r="C62" t="s">
-        <v>5855</v>
+        <v>5853</v>
       </c>
       <c r="D62">
         <v>18</v>
@@ -44765,13 +44843,129 @@
         <v>70</v>
       </c>
       <c r="I62" t="s">
-        <v>5857</v>
+        <v>5855</v>
       </c>
       <c r="J62" t="s">
         <v>2455</v>
       </c>
       <c r="K62" s="8">
         <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>5863</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5865</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5864</v>
+      </c>
+      <c r="D63">
+        <v>15</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
+        <v>70</v>
+      </c>
+      <c r="G63" t="s">
+        <v>2979</v>
+      </c>
+      <c r="H63" t="s">
+        <v>5866</v>
+      </c>
+      <c r="I63" t="s">
+        <v>5867</v>
+      </c>
+      <c r="J63" t="s">
+        <v>5169</v>
+      </c>
+      <c r="K63" s="8">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>5873</v>
+      </c>
+      <c r="B64" t="s">
+        <v>5882</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5517</v>
+      </c>
+      <c r="D64">
+        <v>100</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64" t="s">
+        <v>70</v>
+      </c>
+      <c r="G64" t="s">
+        <v>2979</v>
+      </c>
+      <c r="H64" t="s">
+        <v>5881</v>
+      </c>
+      <c r="I64" t="s">
+        <v>5880</v>
+      </c>
+      <c r="J64" t="s">
+        <v>5773</v>
+      </c>
+      <c r="K64" s="8">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>5874</v>
+      </c>
+      <c r="B65" t="s">
+        <v>5877</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5853</v>
+      </c>
+      <c r="D65">
+        <v>100</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="I65" t="s">
+        <v>5875</v>
+      </c>
+      <c r="J65" t="s">
+        <v>5773</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>5879</v>
+      </c>
+      <c r="B66" t="s">
+        <v>5878</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5853</v>
+      </c>
+      <c r="D66">
+        <v>100</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="I66" t="s">
+        <v>5876</v>
+      </c>
+      <c r="J66" t="s">
+        <v>5773</v>
       </c>
     </row>
   </sheetData>
@@ -67173,10 +67367,10 @@
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
+        <v>5817</v>
+      </c>
+      <c r="B112" t="s">
         <v>5818</v>
-      </c>
-      <c r="B112" t="s">
-        <v>5819</v>
       </c>
       <c r="E112" t="s">
         <v>2120</v>
@@ -67188,7 +67382,7 @@
         <v>37</v>
       </c>
       <c r="H112" t="s">
-        <v>5820</v>
+        <v>5819</v>
       </c>
       <c r="I112" t="s">
         <v>2421</v>
@@ -67208,10 +67402,10 @@
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
+        <v>5831</v>
+      </c>
+      <c r="B113" t="s">
         <v>5832</v>
-      </c>
-      <c r="B113" t="s">
-        <v>5833</v>
       </c>
       <c r="C113" t="s">
         <v>1288</v>
@@ -67220,19 +67414,19 @@
         <v>1284</v>
       </c>
       <c r="E113" t="s">
+        <v>5833</v>
+      </c>
+      <c r="H113" t="s">
         <v>5834</v>
-      </c>
-      <c r="H113" t="s">
-        <v>5835</v>
       </c>
       <c r="I113" t="s">
         <v>4890</v>
       </c>
       <c r="J113" t="s">
-        <v>5837</v>
+        <v>5836</v>
       </c>
       <c r="K113" t="s">
-        <v>5836</v>
+        <v>5835</v>
       </c>
       <c r="L113" t="s">
         <v>1383</v>
@@ -67243,31 +67437,31 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
+        <v>5841</v>
+      </c>
+      <c r="B114" t="s">
         <v>5842</v>
-      </c>
-      <c r="B114" t="s">
-        <v>5843</v>
       </c>
       <c r="C114" t="s">
         <v>1287</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>5841</v>
+        <v>5840</v>
       </c>
       <c r="E114" t="s">
-        <v>5840</v>
+        <v>5839</v>
       </c>
       <c r="H114" t="s">
-        <v>5839</v>
+        <v>5838</v>
       </c>
       <c r="I114" t="s">
         <v>4890</v>
       </c>
       <c r="J114" t="s">
-        <v>5838</v>
+        <v>5837</v>
       </c>
       <c r="K114" t="s">
-        <v>5836</v>
+        <v>5835</v>
       </c>
       <c r="L114" t="s">
         <v>1383</v>
@@ -67513,10 +67707,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67954,25 +68148,48 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>5802</v>
+        <v>5801</v>
       </c>
       <c r="B20" t="s">
-        <v>5806</v>
+        <v>5805</v>
       </c>
       <c r="C20" t="s">
         <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>5805</v>
+        <v>5804</v>
       </c>
       <c r="E20" t="s">
-        <v>5804</v>
+        <v>5803</v>
       </c>
       <c r="F20" t="s">
-        <v>5803</v>
+        <v>5802</v>
       </c>
       <c r="G20" s="8">
         <v>5.54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>5870</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5871</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5869</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4777</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5868</v>
+      </c>
+      <c r="G21" s="8">
+        <v>1.32</v>
       </c>
     </row>
   </sheetData>
@@ -69359,13 +69576,13 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>5786</v>
+      </c>
+      <c r="B39" t="s">
         <v>5787</v>
       </c>
-      <c r="B39" t="s">
-        <v>5788</v>
-      </c>
       <c r="C39" t="s">
-        <v>5793</v>
+        <v>5792</v>
       </c>
       <c r="D39" t="s">
         <v>4766</v>
@@ -69383,13 +69600,13 @@
         <v>2288</v>
       </c>
       <c r="J39" t="s">
+        <v>5789</v>
+      </c>
+      <c r="K39" t="s">
         <v>5790</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>5791</v>
-      </c>
-      <c r="L39" t="s">
-        <v>5792</v>
       </c>
       <c r="M39" s="8">
         <v>1.2</v>
@@ -69397,13 +69614,13 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>5793</v>
+      </c>
+      <c r="B40" t="s">
         <v>5794</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>5795</v>
-      </c>
-      <c r="C40" t="s">
-        <v>5796</v>
       </c>
       <c r="D40" t="s">
         <v>5013</v>
@@ -69421,13 +69638,13 @@
         <v>2288</v>
       </c>
       <c r="J40" t="s">
-        <v>5789</v>
+        <v>5788</v>
       </c>
       <c r="K40" t="s">
+        <v>5790</v>
+      </c>
+      <c r="L40" t="s">
         <v>5791</v>
-      </c>
-      <c r="L40" t="s">
-        <v>5792</v>
       </c>
       <c r="M40" s="8">
         <v>1.2</v>
@@ -69435,25 +69652,25 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>5798</v>
+      </c>
+      <c r="B41" t="s">
         <v>5799</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>5800</v>
-      </c>
-      <c r="C41" t="s">
-        <v>5801</v>
       </c>
       <c r="I41" t="s">
         <v>2288</v>
       </c>
       <c r="J41" t="s">
-        <v>5798</v>
+        <v>5797</v>
       </c>
       <c r="K41" t="s">
         <v>2559</v>
       </c>
       <c r="L41" t="s">
-        <v>5797</v>
+        <v>5796</v>
       </c>
       <c r="M41" s="8">
         <v>1.35</v>
@@ -69461,22 +69678,22 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>5824</v>
+      </c>
+      <c r="B42" t="s">
         <v>5825</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>5826</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>5827</v>
-      </c>
-      <c r="D42" t="s">
-        <v>5828</v>
       </c>
       <c r="E42" t="s">
         <v>2107</v>
       </c>
       <c r="F42" t="s">
-        <v>5829</v>
+        <v>5828</v>
       </c>
       <c r="G42" t="s">
         <v>72</v>
@@ -69488,13 +69705,13 @@
         <v>2288</v>
       </c>
       <c r="J42" t="s">
-        <v>5830</v>
+        <v>5829</v>
       </c>
       <c r="K42" t="s">
         <v>2559</v>
       </c>
       <c r="L42" t="s">
-        <v>5831</v>
+        <v>5830</v>
       </c>
       <c r="M42" s="8">
         <v>0.68</v>
@@ -69508,10 +69725,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -69707,13 +69924,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5780</v>
+        <v>5779</v>
       </c>
       <c r="B6" t="s">
-        <v>5779</v>
+        <v>5778</v>
       </c>
       <c r="C6" t="s">
-        <v>5778</v>
+        <v>5777</v>
       </c>
       <c r="D6" t="s">
         <v>80</v>
@@ -69722,25 +69939,63 @@
         <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>5777</v>
+        <v>5776</v>
       </c>
       <c r="G6" t="s">
-        <v>5777</v>
+        <v>5776</v>
       </c>
       <c r="H6" t="s">
-        <v>5776</v>
+        <v>5775</v>
       </c>
       <c r="I6" t="s">
-        <v>5775</v>
+        <v>5774</v>
       </c>
       <c r="J6" t="s">
+        <v>5780</v>
+      </c>
+      <c r="K6" t="s">
         <v>5781</v>
-      </c>
-      <c r="K6" t="s">
-        <v>5782</v>
       </c>
       <c r="L6" s="8">
         <v>0.79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5856</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5857</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5858</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5859</v>
+      </c>
+      <c r="E7">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5775</v>
+      </c>
+      <c r="I7" t="s">
+        <v>5860</v>
+      </c>
+      <c r="J7" t="s">
+        <v>5861</v>
+      </c>
+      <c r="K7" t="s">
+        <v>5862</v>
+      </c>
+      <c r="L7" s="8">
+        <v>0.56000000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -70985,7 +71240,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add 5A schottky diode
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="6"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15035" uniqueCount="5919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15045" uniqueCount="5923">
   <si>
     <t>Part Number</t>
   </si>
@@ -17788,6 +17788,18 @@
   </si>
   <si>
     <t>ECX-1247</t>
+  </si>
+  <si>
+    <t>SD2114S040S5R0</t>
+  </si>
+  <si>
+    <t>0.52V</t>
+  </si>
+  <si>
+    <t>Dio, Schottky, 5A, 520mV, 40V, DO-214AB</t>
+  </si>
+  <si>
+    <t>DIO-00058</t>
   </si>
 </sst>
 </file>
@@ -41056,10 +41068,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43142,6 +43154,41 @@
         <v>0.38</v>
       </c>
     </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>5922</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>5921</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>5920</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>2101</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>2112</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>4972</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>5919</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>2116</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>2098</v>
+      </c>
+      <c r="M60" s="8">
+        <v>0.74</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43154,7 +43201,7 @@
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -70090,8 +70137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add inductors for ROV power design
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15045" uniqueCount="5923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15063" uniqueCount="5935">
   <si>
     <t>Part Number</t>
   </si>
@@ -17800,6 +17800,42 @@
   </si>
   <si>
     <t>DIO-00058</t>
+  </si>
+  <si>
+    <t>MAG-00114</t>
+  </si>
+  <si>
+    <t>Ind, 33uH, 2.68A (3A sat.), 0.057 Ohm</t>
+  </si>
+  <si>
+    <t>2.68A</t>
+  </si>
+  <si>
+    <t>57mOhm</t>
+  </si>
+  <si>
+    <t>WURTH_74477110</t>
+  </si>
+  <si>
+    <t>Ind, 18uH, 3.9A, 0.0392 Ohm, SMD</t>
+  </si>
+  <si>
+    <t>18uH</t>
+  </si>
+  <si>
+    <t>3.9A</t>
+  </si>
+  <si>
+    <t>39.2mOhm</t>
+  </si>
+  <si>
+    <t>Sumida</t>
+  </si>
+  <si>
+    <t>CDRH127NP-180MC</t>
+  </si>
+  <si>
+    <t>SUMIDA_CDRH127</t>
   </si>
 </sst>
 </file>
@@ -41070,8 +41106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -63917,10 +63953,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N115"/>
+  <dimension ref="A1:N117"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="M115" sqref="M115"/>
+    <sheetView tabSelected="1" topLeftCell="B94" workbookViewId="0">
+      <selection activeCell="M118" sqref="M118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67837,6 +67873,73 @@
       </c>
       <c r="L115" t="s">
         <v>1383</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>5923</v>
+      </c>
+      <c r="B116" t="s">
+        <v>5924</v>
+      </c>
+      <c r="C116" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E116" t="s">
+        <v>5925</v>
+      </c>
+      <c r="H116" t="s">
+        <v>5926</v>
+      </c>
+      <c r="I116" t="s">
+        <v>2421</v>
+      </c>
+      <c r="J116">
+        <v>744771133</v>
+      </c>
+      <c r="K116" t="s">
+        <v>5927</v>
+      </c>
+      <c r="L116" t="s">
+        <v>1383</v>
+      </c>
+      <c r="M116" s="8">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
+        <v>5928</v>
+      </c>
+      <c r="C117" t="s">
+        <v>5929</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E117" t="s">
+        <v>5930</v>
+      </c>
+      <c r="H117" t="s">
+        <v>5931</v>
+      </c>
+      <c r="I117" t="s">
+        <v>5932</v>
+      </c>
+      <c r="J117" t="s">
+        <v>5933</v>
+      </c>
+      <c r="K117" t="s">
+        <v>5934</v>
+      </c>
+      <c r="L117" t="s">
+        <v>1383</v>
+      </c>
+      <c r="M117" s="8">
+        <v>2.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add FRAM chip and other stuff
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15063" uniqueCount="5935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15076" uniqueCount="5943">
   <si>
     <t>Part Number</t>
   </si>
@@ -17836,6 +17836,30 @@
   </si>
   <si>
     <t>SUMIDA_CDRH127</t>
+  </si>
+  <si>
+    <t>PHOENIX_MKDS_6.35MM_2x1</t>
+  </si>
+  <si>
+    <t>CONN-00066</t>
+  </si>
+  <si>
+    <t>Terminal Block, 2 Pos, 30A, 300V, 6.35mm Pitch, Rising Cage 10-30 AWG wire</t>
+  </si>
+  <si>
+    <t>MISC-00037</t>
+  </si>
+  <si>
+    <t>IC, FRAM 128K SPI 40MHZ 8-SOIC</t>
+  </si>
+  <si>
+    <t>Cypress Semiconductor Corp.</t>
+  </si>
+  <si>
+    <t>FM25V01A-G</t>
+  </si>
+  <si>
+    <t>FM25V01A</t>
   </si>
 </sst>
 </file>
@@ -43234,10 +43258,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45266,7 +45290,7 @@
         <v>3.49</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>5868</v>
       </c>
@@ -45289,7 +45313,7 @@
         <v>5770</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>5873</v>
       </c>
@@ -45312,7 +45336,7 @@
         <v>5770</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>5879</v>
       </c>
@@ -45342,6 +45366,41 @@
       </c>
       <c r="J67" t="s">
         <v>2391</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>5936</v>
+      </c>
+      <c r="B68" t="s">
+        <v>5937</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2383</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68" t="s">
+        <v>4661</v>
+      </c>
+      <c r="G68" t="s">
+        <v>2381</v>
+      </c>
+      <c r="H68">
+        <v>1714955</v>
+      </c>
+      <c r="I68" t="s">
+        <v>5935</v>
+      </c>
+      <c r="J68" t="s">
+        <v>2391</v>
+      </c>
+      <c r="K68" s="8">
+        <v>1.71</v>
       </c>
     </row>
   </sheetData>
@@ -63955,7 +64014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B94" workbookViewId="0">
+    <sheetView topLeftCell="B94" workbookViewId="0">
       <selection activeCell="M118" sqref="M118"/>
     </sheetView>
   </sheetViews>
@@ -71773,10 +71832,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -72615,6 +72674,29 @@
         <v>0.91</v>
       </c>
     </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>5938</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5939</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5940</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5941</v>
+      </c>
+      <c r="E39" t="s">
+        <v>4470</v>
+      </c>
+      <c r="F39" t="s">
+        <v>5942</v>
+      </c>
+      <c r="G39" s="8">
+        <v>5.65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add tri state buffer for Junhyung
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15076" uniqueCount="5943">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15082" uniqueCount="5947">
   <si>
     <t>Part Number</t>
   </si>
@@ -17860,6 +17860,18 @@
   </si>
   <si>
     <t>FM25V01A</t>
+  </si>
+  <si>
+    <t>SN74LVC2G240</t>
+  </si>
+  <si>
+    <t>SN74LVC2G240DCUR</t>
+  </si>
+  <si>
+    <t>LOGIC-00034</t>
+  </si>
+  <si>
+    <t>IC, Dual Tri-State Inverter, 1.65-5.5V, 8-VSSOP</t>
   </si>
 </sst>
 </file>
@@ -38939,10 +38951,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39699,6 +39711,26 @@
       </c>
       <c r="F35">
         <v>4001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>5945</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5946</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5944</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4486</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5943</v>
       </c>
     </row>
   </sheetData>
@@ -70580,8 +70612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -71834,8 +71866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update leaded capacitor footprints, add PTC fuse
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,8 @@
     <sheet name="Power Reg" sheetId="6" r:id="rId6"/>
     <sheet name="Oscillators" sheetId="7" r:id="rId7"/>
     <sheet name="Analog" sheetId="8" r:id="rId8"/>
-    <sheet name="Misc" sheetId="9" r:id="rId9"/>
-    <sheet name="Logic" sheetId="10" r:id="rId10"/>
+    <sheet name="Logic" sheetId="10" r:id="rId9"/>
+    <sheet name="Misc" sheetId="9" r:id="rId10"/>
     <sheet name="Transistors" sheetId="11" r:id="rId11"/>
     <sheet name="Diodes" sheetId="12" r:id="rId12"/>
     <sheet name="Connectors" sheetId="13" r:id="rId13"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15082" uniqueCount="5947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15088" uniqueCount="5952">
   <si>
     <t>Part Number</t>
   </si>
@@ -17872,6 +17872,21 @@
   </si>
   <si>
     <t>IC, Dual Tri-State Inverter, 1.65-5.5V, 8-VSSOP</t>
+  </si>
+  <si>
+    <t>LOGIC-00035</t>
+  </si>
+  <si>
+    <t>0ZCG0075FF2C</t>
+  </si>
+  <si>
+    <t>chip_1812</t>
+  </si>
+  <si>
+    <t>Bel Fuse Inc.</t>
+  </si>
+  <si>
+    <t>PTC Fuse (Polyfuse), 16V 750mA Hold, 1.5A Trip, 200ms</t>
   </si>
 </sst>
 </file>
@@ -18244,8 +18259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J839"/>
   <sheetViews>
-    <sheetView topLeftCell="A691" workbookViewId="0">
-      <selection activeCell="B710" sqref="B710"/>
+    <sheetView topLeftCell="A698" workbookViewId="0">
+      <selection activeCell="H710" sqref="H710"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38951,24 +38966,23 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.109375" customWidth="1"/>
+    <col min="2" max="2" width="47.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="8"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -38987,750 +39001,857 @@
       <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" t="s">
         <v>4495</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>5486</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2566</v>
+        <v>2370</v>
       </c>
       <c r="B2" t="s">
-        <v>2565</v>
+        <v>2369</v>
       </c>
       <c r="C2" t="s">
-        <v>2288</v>
+        <v>2368</v>
       </c>
       <c r="D2" t="s">
-        <v>2564</v>
+        <v>2367</v>
       </c>
       <c r="E2" t="s">
-        <v>2559</v>
+        <v>2371</v>
       </c>
       <c r="F2" t="s">
-        <v>2564</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2372</v>
+      </c>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2569</v>
+        <v>2464</v>
       </c>
       <c r="B3" t="s">
-        <v>2568</v>
+        <v>2465</v>
       </c>
       <c r="C3" t="s">
-        <v>2288</v>
+        <v>2466</v>
       </c>
       <c r="D3" t="s">
-        <v>2567</v>
+        <v>2467</v>
       </c>
       <c r="E3" t="s">
-        <v>2559</v>
+        <v>2469</v>
       </c>
       <c r="F3" t="s">
-        <v>2567</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2468</v>
+      </c>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2572</v>
+        <v>2710</v>
       </c>
       <c r="B4" t="s">
-        <v>2571</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2288</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2570</v>
+        <v>2711</v>
       </c>
       <c r="E4" t="s">
-        <v>2337</v>
+        <v>2712</v>
       </c>
       <c r="F4" t="s">
-        <v>2570</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2712</v>
+      </c>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2578</v>
+        <v>2902</v>
       </c>
       <c r="B5" t="s">
-        <v>2577</v>
+        <v>2903</v>
       </c>
       <c r="C5" t="s">
-        <v>2288</v>
+        <v>2904</v>
       </c>
       <c r="D5" t="s">
-        <v>2579</v>
+        <v>2903</v>
       </c>
       <c r="E5" t="s">
-        <v>2559</v>
+        <v>2903</v>
       </c>
       <c r="F5" t="s">
-        <v>2579</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2903</v>
+      </c>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2968</v>
+        <v>2927</v>
       </c>
       <c r="B6" t="s">
-        <v>2970</v>
+        <v>2926</v>
       </c>
       <c r="C6" t="s">
-        <v>2288</v>
+        <v>2928</v>
       </c>
       <c r="D6" t="s">
-        <v>2969</v>
+        <v>2925</v>
       </c>
       <c r="E6" t="s">
-        <v>2967</v>
+        <v>2925</v>
       </c>
       <c r="F6" t="s">
-        <v>4318</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2925</v>
+      </c>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4294</v>
+        <v>2977</v>
       </c>
       <c r="B7" t="s">
-        <v>4299</v>
+        <v>2978</v>
       </c>
       <c r="C7" t="s">
-        <v>2288</v>
+        <v>2979</v>
       </c>
       <c r="D7" t="s">
-        <v>4295</v>
+        <v>2980</v>
       </c>
       <c r="E7" t="s">
-        <v>3365</v>
+        <v>2981</v>
       </c>
       <c r="F7" t="s">
-        <v>4305</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2982</v>
+      </c>
+      <c r="G7" s="8">
+        <v>3.12</v>
+      </c>
+      <c r="H7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4297</v>
+        <v>4234</v>
       </c>
       <c r="B8" t="s">
-        <v>4298</v>
+        <v>4235</v>
       </c>
       <c r="C8" t="s">
-        <v>2288</v>
+        <v>4236</v>
       </c>
       <c r="D8" t="s">
-        <v>4296</v>
+        <v>4237</v>
       </c>
       <c r="E8" t="s">
-        <v>4300</v>
+        <v>4238</v>
       </c>
       <c r="F8" t="s">
-        <v>4305</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4237</v>
+      </c>
+      <c r="G8" s="8">
+        <v>26.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4301</v>
+        <v>4261</v>
       </c>
       <c r="B9" t="s">
-        <v>4302</v>
+        <v>4262</v>
       </c>
       <c r="C9" t="s">
-        <v>2288</v>
+        <v>4264</v>
       </c>
       <c r="D9" t="s">
-        <v>4303</v>
+        <v>4263</v>
       </c>
       <c r="E9" t="s">
-        <v>3365</v>
+        <v>4263</v>
       </c>
       <c r="F9" t="s">
-        <v>4304</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4263</v>
+      </c>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4306</v>
+        <v>4265</v>
       </c>
       <c r="B10" t="s">
-        <v>4307</v>
+        <v>4266</v>
       </c>
       <c r="C10" t="s">
-        <v>2288</v>
+        <v>2277</v>
       </c>
       <c r="D10" t="s">
-        <v>4308</v>
+        <v>4267</v>
       </c>
       <c r="E10" t="s">
-        <v>4300</v>
+        <v>1472</v>
       </c>
       <c r="F10" t="s">
-        <v>4304</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4268</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4336</v>
+        <v>4475</v>
       </c>
       <c r="B11" t="s">
-        <v>4342</v>
+        <v>4476</v>
       </c>
       <c r="C11" t="s">
-        <v>2288</v>
+        <v>4477</v>
       </c>
       <c r="D11" t="s">
-        <v>4337</v>
+        <v>4478</v>
       </c>
       <c r="E11" t="s">
-        <v>3365</v>
+        <v>4478</v>
       </c>
       <c r="F11" t="s">
-        <v>4338</v>
+        <v>4479</v>
       </c>
       <c r="G11" s="8">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4339</v>
+        <v>4555</v>
       </c>
       <c r="B12" t="s">
-        <v>4341</v>
+        <v>4552</v>
       </c>
       <c r="C12" t="s">
-        <v>2288</v>
+        <v>4553</v>
       </c>
       <c r="D12" t="s">
-        <v>4340</v>
+        <v>4556</v>
       </c>
       <c r="E12" t="s">
-        <v>4300</v>
+        <v>4554</v>
       </c>
       <c r="F12" t="s">
-        <v>4338</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2964</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4507</v>
+        <v>4583</v>
       </c>
       <c r="B13" t="s">
-        <v>4508</v>
+        <v>4584</v>
       </c>
       <c r="C13" t="s">
         <v>2288</v>
       </c>
       <c r="D13" t="s">
-        <v>4509</v>
+        <v>4585</v>
       </c>
       <c r="E13" t="s">
-        <v>4510</v>
+        <v>2318</v>
       </c>
       <c r="F13" t="s">
-        <v>4511</v>
+        <v>4586</v>
       </c>
       <c r="G13" s="8">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4575</v>
+        <v>4593</v>
       </c>
       <c r="B14" t="s">
-        <v>4576</v>
+        <v>4594</v>
       </c>
       <c r="C14" t="s">
-        <v>2288</v>
+        <v>4595</v>
       </c>
       <c r="D14" t="s">
-        <v>4577</v>
+        <v>4596</v>
       </c>
       <c r="E14" t="s">
-        <v>3365</v>
+        <v>4597</v>
       </c>
       <c r="F14" t="s">
-        <v>4578</v>
+        <v>4598</v>
       </c>
       <c r="G14" s="8">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4708</v>
+        <v>4621</v>
       </c>
       <c r="B15" t="s">
-        <v>4709</v>
+        <v>4622</v>
       </c>
       <c r="C15" t="s">
-        <v>2288</v>
+        <v>4623</v>
       </c>
       <c r="D15" t="s">
-        <v>4710</v>
+        <v>4624</v>
       </c>
       <c r="E15" t="s">
-        <v>4711</v>
+        <v>4625</v>
       </c>
       <c r="F15" t="s">
-        <v>4712</v>
+        <v>4626</v>
       </c>
       <c r="G15" s="8">
-        <v>2.87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4829</v>
+        <v>4639</v>
       </c>
       <c r="B16" t="s">
-        <v>4832</v>
+        <v>4640</v>
       </c>
       <c r="C16" t="s">
-        <v>2288</v>
+        <v>4641</v>
       </c>
       <c r="D16" t="s">
-        <v>4830</v>
+        <v>4642</v>
       </c>
       <c r="E16" t="s">
-        <v>4300</v>
+        <v>4643</v>
       </c>
       <c r="F16" t="s">
-        <v>4831</v>
-      </c>
-      <c r="G16" s="8">
-        <v>0.41</v>
+        <v>4644</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>4877</v>
+        <v>4790</v>
       </c>
       <c r="B17" t="s">
-        <v>4878</v>
+        <v>4794</v>
       </c>
       <c r="C17" t="s">
-        <v>2288</v>
+        <v>4314</v>
       </c>
       <c r="D17" t="s">
-        <v>4879</v>
+        <v>4791</v>
       </c>
       <c r="E17" t="s">
-        <v>4300</v>
+        <v>4792</v>
       </c>
       <c r="F17" t="s">
-        <v>4880</v>
+        <v>4793</v>
+      </c>
+      <c r="G17" s="8">
+        <v>5.03</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>4946</v>
+        <v>4838</v>
       </c>
       <c r="B18" t="s">
-        <v>4947</v>
-      </c>
-      <c r="C18" t="s">
-        <v>2288</v>
-      </c>
-      <c r="D18" t="s">
-        <v>4948</v>
+        <v>4839</v>
       </c>
       <c r="E18" t="s">
-        <v>4300</v>
+        <v>4840</v>
       </c>
       <c r="F18" t="s">
-        <v>4949</v>
-      </c>
-      <c r="G18" s="8">
-        <v>0.42</v>
+        <v>4840</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>4950</v>
+        <v>4864</v>
       </c>
       <c r="B19" t="s">
-        <v>4951</v>
+        <v>4865</v>
       </c>
       <c r="C19" t="s">
-        <v>2288</v>
+        <v>4866</v>
       </c>
       <c r="D19" t="s">
-        <v>4952</v>
+        <v>4867</v>
       </c>
       <c r="E19" t="s">
-        <v>4300</v>
+        <v>4868</v>
       </c>
       <c r="F19" t="s">
-        <v>4953</v>
-      </c>
-      <c r="G19" s="8">
-        <v>0.48</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>5076</v>
+        <v>4931</v>
       </c>
       <c r="B20" t="s">
-        <v>5079</v>
+        <v>4929</v>
       </c>
       <c r="C20" t="s">
-        <v>2288</v>
+        <v>4623</v>
       </c>
       <c r="D20" t="s">
-        <v>5077</v>
+        <v>4932</v>
       </c>
       <c r="E20" t="s">
-        <v>4510</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>5078</v>
+        <v>4930</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2372</v>
       </c>
       <c r="G20" s="8">
-        <v>0.42</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>5134</v>
+        <v>4933</v>
       </c>
       <c r="B21" t="s">
-        <v>5135</v>
+        <v>4936</v>
       </c>
       <c r="C21" t="s">
-        <v>2288</v>
+        <v>4890</v>
       </c>
       <c r="D21" t="s">
-        <v>5136</v>
+        <v>4934</v>
       </c>
       <c r="E21" t="s">
-        <v>4300</v>
-      </c>
-      <c r="F21">
-        <v>4093</v>
+        <v>4935</v>
+      </c>
+      <c r="F21" t="s">
+        <v>4937</v>
       </c>
       <c r="G21" s="8">
-        <v>0.42</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>5211</v>
+        <v>4960</v>
       </c>
       <c r="B22" t="s">
-        <v>5212</v>
-      </c>
-      <c r="C22" t="s">
-        <v>2288</v>
+        <v>4961</v>
       </c>
       <c r="D22" t="s">
-        <v>5213</v>
+        <v>4962</v>
       </c>
       <c r="E22" t="s">
-        <v>5210</v>
-      </c>
-      <c r="F22">
-        <v>4093</v>
-      </c>
-      <c r="G22" s="8">
-        <v>0.49</v>
+        <v>4962</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4963</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>5329</v>
+        <v>4996</v>
       </c>
       <c r="B23" t="s">
-        <v>5362</v>
-      </c>
-      <c r="C23" t="s">
-        <v>2288</v>
-      </c>
-      <c r="D23" t="s">
-        <v>5363</v>
+        <v>4999</v>
       </c>
       <c r="E23" t="s">
-        <v>5210</v>
-      </c>
-      <c r="F23">
-        <v>4066</v>
-      </c>
-      <c r="G23" s="8">
-        <v>0.49</v>
+        <v>4997</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4998</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>5334</v>
+        <v>5083</v>
       </c>
       <c r="B24" t="s">
-        <v>5335</v>
+        <v>5084</v>
       </c>
       <c r="C24" t="s">
         <v>2288</v>
       </c>
       <c r="D24" t="s">
-        <v>5336</v>
+        <v>5080</v>
       </c>
       <c r="E24" t="s">
-        <v>5210</v>
-      </c>
-      <c r="F24">
-        <v>40106</v>
+        <v>5081</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5082</v>
       </c>
       <c r="G24" s="8">
-        <v>0.51</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>5356</v>
+        <v>5143</v>
       </c>
       <c r="B25" t="s">
-        <v>5894</v>
+        <v>5144</v>
       </c>
       <c r="C25" t="s">
-        <v>2288</v>
+        <v>4972</v>
       </c>
       <c r="D25" t="s">
-        <v>5357</v>
+        <v>5145</v>
       </c>
       <c r="E25" t="s">
-        <v>5358</v>
-      </c>
-      <c r="F25">
-        <v>4518</v>
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4937</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0.48</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>5359</v>
+        <v>5179</v>
       </c>
       <c r="B26" t="s">
-        <v>5893</v>
+        <v>5180</v>
       </c>
       <c r="C26" t="s">
-        <v>2288</v>
+        <v>5181</v>
       </c>
       <c r="D26" t="s">
-        <v>5360</v>
+        <v>5183</v>
       </c>
       <c r="E26" t="s">
-        <v>5358</v>
-      </c>
-      <c r="F26">
-        <v>4018</v>
+        <v>5182</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2468</v>
+      </c>
+      <c r="G26" s="8">
+        <v>0.33</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>5361</v>
+        <v>5386</v>
       </c>
       <c r="B27" t="s">
-        <v>5364</v>
+        <v>5383</v>
       </c>
       <c r="C27" t="s">
-        <v>2288</v>
+        <v>4890</v>
       </c>
       <c r="D27" t="s">
-        <v>5365</v>
+        <v>5384</v>
       </c>
       <c r="E27" t="s">
-        <v>5210</v>
+        <v>5385</v>
       </c>
       <c r="F27" t="s">
-        <v>4949</v>
+        <v>4937</v>
+      </c>
+      <c r="G27" s="8">
+        <v>0.49</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>5366</v>
+        <v>5450</v>
       </c>
       <c r="B28" t="s">
-        <v>5367</v>
+        <v>5451</v>
       </c>
       <c r="C28" t="s">
-        <v>2288</v>
+        <v>4623</v>
       </c>
       <c r="D28" t="s">
-        <v>5368</v>
+        <v>5452</v>
       </c>
       <c r="E28" t="s">
-        <v>5210</v>
-      </c>
-      <c r="F28">
-        <v>4001</v>
+        <v>5452</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5453</v>
+      </c>
+      <c r="G28" s="8">
+        <v>1.51</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>5446</v>
+        <v>5477</v>
       </c>
       <c r="B29" t="s">
-        <v>5447</v>
-      </c>
-      <c r="C29" t="s">
-        <v>2288</v>
-      </c>
-      <c r="D29" t="s">
-        <v>5448</v>
+        <v>5478</v>
       </c>
       <c r="E29" t="s">
-        <v>2522</v>
+        <v>5479</v>
       </c>
       <c r="F29" t="s">
-        <v>5045</v>
-      </c>
-      <c r="G29" s="8">
-        <v>0.33</v>
+        <v>4998</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>5454</v>
+        <v>5487</v>
       </c>
       <c r="B30" t="s">
-        <v>5455</v>
+        <v>5488</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>5456</v>
+        <v>5490</v>
       </c>
       <c r="E30" t="s">
-        <v>4470</v>
+        <v>5489</v>
       </c>
       <c r="F30" t="s">
-        <v>5457</v>
+        <v>5489</v>
       </c>
       <c r="G30" s="8">
-        <v>0.2</v>
+        <v>5.36</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>5887</v>
+        <v>5503</v>
       </c>
       <c r="B31" t="s">
-        <v>5886</v>
+        <v>5504</v>
       </c>
       <c r="C31" t="s">
-        <v>2288</v>
+        <v>4477</v>
       </c>
       <c r="D31" t="s">
-        <v>5882</v>
+        <v>5505</v>
       </c>
       <c r="E31" t="s">
-        <v>4300</v>
-      </c>
-      <c r="F31">
-        <v>4066</v>
+        <v>5506</v>
+      </c>
+      <c r="F31" t="s">
+        <v>4479</v>
+      </c>
+      <c r="G31" s="8">
+        <v>2.85</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>5888</v>
+        <v>5518</v>
       </c>
       <c r="B32" t="s">
-        <v>5892</v>
+        <v>5519</v>
       </c>
       <c r="C32" t="s">
+        <v>2092</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5520</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5521</v>
+      </c>
+      <c r="F32" t="s">
+        <v>5522</v>
+      </c>
+      <c r="G32" s="8">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>5539</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5540</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5541</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5542</v>
+      </c>
+      <c r="E33" t="s">
+        <v>2897</v>
+      </c>
+      <c r="F33" t="s">
+        <v>5542</v>
+      </c>
+      <c r="G33" s="8">
+        <v>12.44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>5543</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5544</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5545</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5546</v>
+      </c>
+      <c r="E34" t="s">
+        <v>5548</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5547</v>
+      </c>
+      <c r="G34" s="8">
+        <v>12.48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>5669</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5672</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2466</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5670</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5671</v>
+      </c>
+      <c r="F35" t="s">
+        <v>4479</v>
+      </c>
+      <c r="G35" s="8">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>5713</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5714</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5715</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5716</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5717</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5716</v>
+      </c>
+      <c r="G36" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>5739</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5742</v>
+      </c>
+      <c r="C37" t="s">
         <v>2288</v>
       </c>
-      <c r="D32" t="s">
-        <v>5881</v>
-      </c>
-      <c r="E32" t="s">
-        <v>4300</v>
-      </c>
-      <c r="F32">
-        <v>40106</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>5889</v>
-      </c>
-      <c r="B33" t="s">
-        <v>5895</v>
-      </c>
-      <c r="C33" t="s">
-        <v>2288</v>
-      </c>
-      <c r="D33" t="s">
-        <v>5883</v>
-      </c>
-      <c r="E33" t="s">
-        <v>5507</v>
-      </c>
-      <c r="F33">
-        <v>4518</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>5890</v>
-      </c>
-      <c r="B34" t="s">
-        <v>5896</v>
-      </c>
-      <c r="C34" t="s">
-        <v>2288</v>
-      </c>
-      <c r="D34" t="s">
-        <v>5884</v>
-      </c>
-      <c r="E34" t="s">
-        <v>5507</v>
-      </c>
-      <c r="F34">
-        <v>4018</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>5891</v>
-      </c>
-      <c r="B35" t="s">
-        <v>5897</v>
-      </c>
-      <c r="C35" t="s">
-        <v>2288</v>
-      </c>
-      <c r="D35" t="s">
-        <v>5885</v>
-      </c>
-      <c r="E35" t="s">
-        <v>4300</v>
-      </c>
-      <c r="F35">
-        <v>4001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>5945</v>
-      </c>
-      <c r="B36" t="s">
-        <v>5946</v>
-      </c>
-      <c r="C36" t="s">
-        <v>2288</v>
-      </c>
-      <c r="D36" t="s">
-        <v>5944</v>
-      </c>
-      <c r="E36" t="s">
-        <v>4486</v>
-      </c>
-      <c r="F36" t="s">
-        <v>5943</v>
+      <c r="D37" t="s">
+        <v>5740</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2522</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5741</v>
+      </c>
+      <c r="G37" s="8">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>5747</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5748</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5372</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>5749</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5750</v>
+      </c>
+      <c r="F38" t="s">
+        <v>3369</v>
+      </c>
+      <c r="G38" s="8">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>5938</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5939</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5940</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5941</v>
+      </c>
+      <c r="E39" t="s">
+        <v>4470</v>
+      </c>
+      <c r="F39" t="s">
+        <v>5942</v>
+      </c>
+      <c r="G39" s="8">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>5947</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5951</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5950</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5948</v>
+      </c>
+      <c r="E40" t="s">
+        <v>5949</v>
+      </c>
+      <c r="F40" t="s">
+        <v>4268</v>
+      </c>
+      <c r="G40" s="8">
+        <v>0.13</v>
       </c>
     </row>
   </sheetData>
@@ -45445,8 +45566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K562"/>
   <sheetViews>
-    <sheetView topLeftCell="A538" workbookViewId="0">
-      <selection activeCell="I563" sqref="I563"/>
+    <sheetView topLeftCell="A533" workbookViewId="0">
+      <selection activeCell="I249" sqref="I249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45459,7 +45580,7 @@
     <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.88671875" style="8"/>
   </cols>
@@ -71864,23 +71985,24 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.109375" customWidth="1"/>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -71899,834 +72021,750 @@
       <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="8" t="s">
         <v>4495</v>
       </c>
-      <c r="H1" t="s">
-        <v>5486</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2370</v>
+        <v>2566</v>
       </c>
       <c r="B2" t="s">
-        <v>2369</v>
+        <v>2565</v>
       </c>
       <c r="C2" t="s">
-        <v>2368</v>
+        <v>2288</v>
       </c>
       <c r="D2" t="s">
-        <v>2367</v>
+        <v>2564</v>
       </c>
       <c r="E2" t="s">
-        <v>2371</v>
+        <v>2559</v>
       </c>
       <c r="F2" t="s">
-        <v>2372</v>
-      </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2564</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2464</v>
+        <v>2569</v>
       </c>
       <c r="B3" t="s">
-        <v>2465</v>
+        <v>2568</v>
       </c>
       <c r="C3" t="s">
-        <v>2466</v>
+        <v>2288</v>
       </c>
       <c r="D3" t="s">
-        <v>2467</v>
+        <v>2567</v>
       </c>
       <c r="E3" t="s">
-        <v>2469</v>
+        <v>2559</v>
       </c>
       <c r="F3" t="s">
-        <v>2468</v>
-      </c>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2567</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2710</v>
+        <v>2572</v>
       </c>
       <c r="B4" t="s">
-        <v>2711</v>
+        <v>2571</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2570</v>
       </c>
       <c r="E4" t="s">
-        <v>2712</v>
+        <v>2337</v>
       </c>
       <c r="F4" t="s">
-        <v>2712</v>
-      </c>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2570</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2902</v>
+        <v>2578</v>
       </c>
       <c r="B5" t="s">
-        <v>2903</v>
+        <v>2577</v>
       </c>
       <c r="C5" t="s">
-        <v>2904</v>
+        <v>2288</v>
       </c>
       <c r="D5" t="s">
-        <v>2903</v>
+        <v>2579</v>
       </c>
       <c r="E5" t="s">
-        <v>2903</v>
+        <v>2559</v>
       </c>
       <c r="F5" t="s">
-        <v>2903</v>
-      </c>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2579</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2927</v>
+        <v>2968</v>
       </c>
       <c r="B6" t="s">
-        <v>2926</v>
+        <v>2970</v>
       </c>
       <c r="C6" t="s">
-        <v>2928</v>
+        <v>2288</v>
       </c>
       <c r="D6" t="s">
-        <v>2925</v>
+        <v>2969</v>
       </c>
       <c r="E6" t="s">
-        <v>2925</v>
+        <v>2967</v>
       </c>
       <c r="F6" t="s">
-        <v>2925</v>
-      </c>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>4318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>2977</v>
+        <v>4294</v>
       </c>
       <c r="B7" t="s">
-        <v>2978</v>
+        <v>4299</v>
       </c>
       <c r="C7" t="s">
-        <v>2979</v>
+        <v>2288</v>
       </c>
       <c r="D7" t="s">
-        <v>2980</v>
+        <v>4295</v>
       </c>
       <c r="E7" t="s">
-        <v>2981</v>
+        <v>3365</v>
       </c>
       <c r="F7" t="s">
-        <v>2982</v>
-      </c>
-      <c r="G7" s="8">
-        <v>3.12</v>
-      </c>
-      <c r="H7">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>4305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4234</v>
+        <v>4297</v>
       </c>
       <c r="B8" t="s">
-        <v>4235</v>
+        <v>4298</v>
       </c>
       <c r="C8" t="s">
-        <v>4236</v>
+        <v>2288</v>
       </c>
       <c r="D8" t="s">
-        <v>4237</v>
+        <v>4296</v>
       </c>
       <c r="E8" t="s">
-        <v>4238</v>
+        <v>4300</v>
       </c>
       <c r="F8" t="s">
-        <v>4237</v>
-      </c>
-      <c r="G8" s="8">
-        <v>26.62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>4305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4261</v>
+        <v>4301</v>
       </c>
       <c r="B9" t="s">
-        <v>4262</v>
+        <v>4302</v>
       </c>
       <c r="C9" t="s">
-        <v>4264</v>
+        <v>2288</v>
       </c>
       <c r="D9" t="s">
-        <v>4263</v>
+        <v>4303</v>
       </c>
       <c r="E9" t="s">
-        <v>4263</v>
+        <v>3365</v>
       </c>
       <c r="F9" t="s">
-        <v>4263</v>
-      </c>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>4304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4265</v>
+        <v>4306</v>
       </c>
       <c r="B10" t="s">
-        <v>4266</v>
+        <v>4307</v>
       </c>
       <c r="C10" t="s">
-        <v>2277</v>
+        <v>2288</v>
       </c>
       <c r="D10" t="s">
-        <v>4267</v>
+        <v>4308</v>
       </c>
       <c r="E10" t="s">
-        <v>1472</v>
+        <v>4300</v>
       </c>
       <c r="F10" t="s">
-        <v>4268</v>
-      </c>
-      <c r="G10" s="8">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>4304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4475</v>
+        <v>4336</v>
       </c>
       <c r="B11" t="s">
-        <v>4476</v>
+        <v>4342</v>
       </c>
       <c r="C11" t="s">
-        <v>4477</v>
+        <v>2288</v>
       </c>
       <c r="D11" t="s">
-        <v>4478</v>
+        <v>4337</v>
       </c>
       <c r="E11" t="s">
-        <v>4478</v>
+        <v>3365</v>
       </c>
       <c r="F11" t="s">
-        <v>4479</v>
+        <v>4338</v>
       </c>
       <c r="G11" s="8">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="H11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4555</v>
+        <v>4339</v>
       </c>
       <c r="B12" t="s">
-        <v>4552</v>
+        <v>4341</v>
       </c>
       <c r="C12" t="s">
-        <v>4553</v>
+        <v>2288</v>
       </c>
       <c r="D12" t="s">
-        <v>4556</v>
+        <v>4340</v>
       </c>
       <c r="E12" t="s">
-        <v>4554</v>
+        <v>4300</v>
       </c>
       <c r="F12" t="s">
-        <v>2964</v>
-      </c>
-      <c r="G12" s="8">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>4338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4583</v>
+        <v>4507</v>
       </c>
       <c r="B13" t="s">
-        <v>4584</v>
+        <v>4508</v>
       </c>
       <c r="C13" t="s">
         <v>2288</v>
       </c>
       <c r="D13" t="s">
-        <v>4585</v>
+        <v>4509</v>
       </c>
       <c r="E13" t="s">
-        <v>2318</v>
+        <v>4510</v>
       </c>
       <c r="F13" t="s">
-        <v>4586</v>
+        <v>4511</v>
       </c>
       <c r="G13" s="8">
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4593</v>
+        <v>4575</v>
       </c>
       <c r="B14" t="s">
-        <v>4594</v>
+        <v>4576</v>
       </c>
       <c r="C14" t="s">
-        <v>4595</v>
+        <v>2288</v>
       </c>
       <c r="D14" t="s">
-        <v>4596</v>
+        <v>4577</v>
       </c>
       <c r="E14" t="s">
-        <v>4597</v>
+        <v>3365</v>
       </c>
       <c r="F14" t="s">
-        <v>4598</v>
+        <v>4578</v>
       </c>
       <c r="G14" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4621</v>
+        <v>4708</v>
       </c>
       <c r="B15" t="s">
-        <v>4622</v>
+        <v>4709</v>
       </c>
       <c r="C15" t="s">
-        <v>4623</v>
+        <v>2288</v>
       </c>
       <c r="D15" t="s">
-        <v>4624</v>
+        <v>4710</v>
       </c>
       <c r="E15" t="s">
-        <v>4625</v>
+        <v>4711</v>
       </c>
       <c r="F15" t="s">
-        <v>4626</v>
+        <v>4712</v>
       </c>
       <c r="G15" s="8">
-        <v>3.09</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4639</v>
+        <v>4829</v>
       </c>
       <c r="B16" t="s">
-        <v>4640</v>
+        <v>4832</v>
       </c>
       <c r="C16" t="s">
-        <v>4641</v>
+        <v>2288</v>
       </c>
       <c r="D16" t="s">
-        <v>4642</v>
+        <v>4830</v>
       </c>
       <c r="E16" t="s">
-        <v>4643</v>
+        <v>4300</v>
       </c>
       <c r="F16" t="s">
-        <v>4644</v>
+        <v>4831</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0.41</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>4790</v>
+        <v>4877</v>
       </c>
       <c r="B17" t="s">
-        <v>4794</v>
+        <v>4878</v>
       </c>
       <c r="C17" t="s">
-        <v>4314</v>
+        <v>2288</v>
       </c>
       <c r="D17" t="s">
-        <v>4791</v>
+        <v>4879</v>
       </c>
       <c r="E17" t="s">
-        <v>4792</v>
+        <v>4300</v>
       </c>
       <c r="F17" t="s">
-        <v>4793</v>
-      </c>
-      <c r="G17" s="8">
-        <v>5.03</v>
+        <v>4880</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>4838</v>
+        <v>4946</v>
       </c>
       <c r="B18" t="s">
-        <v>4839</v>
+        <v>4947</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4948</v>
       </c>
       <c r="E18" t="s">
-        <v>4840</v>
+        <v>4300</v>
       </c>
       <c r="F18" t="s">
-        <v>4840</v>
+        <v>4949</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0.42</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>4864</v>
+        <v>4950</v>
       </c>
       <c r="B19" t="s">
-        <v>4865</v>
+        <v>4951</v>
       </c>
       <c r="C19" t="s">
-        <v>4866</v>
+        <v>2288</v>
       </c>
       <c r="D19" t="s">
-        <v>4867</v>
+        <v>4952</v>
       </c>
       <c r="E19" t="s">
-        <v>4868</v>
+        <v>4300</v>
       </c>
       <c r="F19" t="s">
-        <v>2344</v>
+        <v>4953</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.48</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>4931</v>
+        <v>5076</v>
       </c>
       <c r="B20" t="s">
-        <v>4929</v>
+        <v>5079</v>
       </c>
       <c r="C20" t="s">
-        <v>4623</v>
+        <v>2288</v>
       </c>
       <c r="D20" t="s">
-        <v>4932</v>
+        <v>5077</v>
       </c>
       <c r="E20" t="s">
-        <v>4930</v>
-      </c>
-      <c r="F20" t="s">
-        <v>2372</v>
+        <v>4510</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>5078</v>
       </c>
       <c r="G20" s="8">
-        <v>1.33</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>4933</v>
+        <v>5134</v>
       </c>
       <c r="B21" t="s">
-        <v>4936</v>
+        <v>5135</v>
       </c>
       <c r="C21" t="s">
-        <v>4890</v>
+        <v>2288</v>
       </c>
       <c r="D21" t="s">
-        <v>4934</v>
+        <v>5136</v>
       </c>
       <c r="E21" t="s">
-        <v>4935</v>
-      </c>
-      <c r="F21" t="s">
-        <v>4937</v>
+        <v>4300</v>
+      </c>
+      <c r="F21">
+        <v>4093</v>
       </c>
       <c r="G21" s="8">
-        <v>0.54</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>4960</v>
+        <v>5211</v>
       </c>
       <c r="B22" t="s">
-        <v>4961</v>
+        <v>5212</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2288</v>
       </c>
       <c r="D22" t="s">
-        <v>4962</v>
+        <v>5213</v>
       </c>
       <c r="E22" t="s">
-        <v>4962</v>
-      </c>
-      <c r="F22" t="s">
-        <v>4963</v>
+        <v>5210</v>
+      </c>
+      <c r="F22">
+        <v>4093</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.49</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>4996</v>
+        <v>5329</v>
       </c>
       <c r="B23" t="s">
-        <v>4999</v>
+        <v>5362</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5363</v>
       </c>
       <c r="E23" t="s">
-        <v>4997</v>
-      </c>
-      <c r="F23" t="s">
-        <v>4998</v>
+        <v>5210</v>
+      </c>
+      <c r="F23">
+        <v>4066</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.49</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>5083</v>
+        <v>5334</v>
       </c>
       <c r="B24" t="s">
-        <v>5084</v>
+        <v>5335</v>
       </c>
       <c r="C24" t="s">
         <v>2288</v>
       </c>
       <c r="D24" t="s">
-        <v>5080</v>
+        <v>5336</v>
       </c>
       <c r="E24" t="s">
-        <v>5081</v>
-      </c>
-      <c r="F24" t="s">
-        <v>5082</v>
+        <v>5210</v>
+      </c>
+      <c r="F24">
+        <v>40106</v>
       </c>
       <c r="G24" s="8">
-        <v>1.53</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>5143</v>
+        <v>5356</v>
       </c>
       <c r="B25" t="s">
-        <v>5144</v>
+        <v>5894</v>
       </c>
       <c r="C25" t="s">
-        <v>4972</v>
+        <v>2288</v>
       </c>
       <c r="D25" t="s">
-        <v>5145</v>
+        <v>5357</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" t="s">
-        <v>4937</v>
-      </c>
-      <c r="G25" s="8">
-        <v>0.48</v>
+        <v>5358</v>
+      </c>
+      <c r="F25">
+        <v>4518</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>5179</v>
+        <v>5359</v>
       </c>
       <c r="B26" t="s">
-        <v>5180</v>
+        <v>5893</v>
       </c>
       <c r="C26" t="s">
-        <v>5181</v>
+        <v>2288</v>
       </c>
       <c r="D26" t="s">
-        <v>5183</v>
+        <v>5360</v>
       </c>
       <c r="E26" t="s">
-        <v>5182</v>
-      </c>
-      <c r="F26" t="s">
-        <v>2468</v>
-      </c>
-      <c r="G26" s="8">
-        <v>0.33</v>
+        <v>5358</v>
+      </c>
+      <c r="F26">
+        <v>4018</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>5386</v>
+        <v>5361</v>
       </c>
       <c r="B27" t="s">
-        <v>5383</v>
+        <v>5364</v>
       </c>
       <c r="C27" t="s">
-        <v>4890</v>
+        <v>2288</v>
       </c>
       <c r="D27" t="s">
-        <v>5384</v>
+        <v>5365</v>
       </c>
       <c r="E27" t="s">
-        <v>5385</v>
+        <v>5210</v>
       </c>
       <c r="F27" t="s">
-        <v>4937</v>
-      </c>
-      <c r="G27" s="8">
-        <v>0.49</v>
+        <v>4949</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>5450</v>
+        <v>5366</v>
       </c>
       <c r="B28" t="s">
-        <v>5451</v>
+        <v>5367</v>
       </c>
       <c r="C28" t="s">
-        <v>4623</v>
+        <v>2288</v>
       </c>
       <c r="D28" t="s">
-        <v>5452</v>
+        <v>5368</v>
       </c>
       <c r="E28" t="s">
-        <v>5452</v>
-      </c>
-      <c r="F28" t="s">
-        <v>5453</v>
-      </c>
-      <c r="G28" s="8">
-        <v>1.51</v>
+        <v>5210</v>
+      </c>
+      <c r="F28">
+        <v>4001</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>5477</v>
+        <v>5446</v>
       </c>
       <c r="B29" t="s">
-        <v>5478</v>
+        <v>5447</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5448</v>
       </c>
       <c r="E29" t="s">
-        <v>5479</v>
+        <v>2522</v>
       </c>
       <c r="F29" t="s">
-        <v>4998</v>
+        <v>5045</v>
+      </c>
+      <c r="G29" s="8">
+        <v>0.33</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>5487</v>
+        <v>5454</v>
       </c>
       <c r="B30" t="s">
-        <v>5488</v>
+        <v>5455</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D30" t="s">
-        <v>5490</v>
+        <v>5456</v>
       </c>
       <c r="E30" t="s">
-        <v>5489</v>
+        <v>4470</v>
       </c>
       <c r="F30" t="s">
-        <v>5489</v>
+        <v>5457</v>
       </c>
       <c r="G30" s="8">
-        <v>5.36</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>5503</v>
+        <v>5887</v>
       </c>
       <c r="B31" t="s">
-        <v>5504</v>
+        <v>5886</v>
       </c>
       <c r="C31" t="s">
-        <v>4477</v>
+        <v>2288</v>
       </c>
       <c r="D31" t="s">
-        <v>5505</v>
+        <v>5882</v>
       </c>
       <c r="E31" t="s">
-        <v>5506</v>
-      </c>
-      <c r="F31" t="s">
-        <v>4479</v>
-      </c>
-      <c r="G31" s="8">
-        <v>2.85</v>
+        <v>4300</v>
+      </c>
+      <c r="F31">
+        <v>4066</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>5518</v>
+        <v>5888</v>
       </c>
       <c r="B32" t="s">
-        <v>5519</v>
+        <v>5892</v>
       </c>
       <c r="C32" t="s">
-        <v>2092</v>
+        <v>2288</v>
       </c>
       <c r="D32" t="s">
-        <v>5520</v>
+        <v>5881</v>
       </c>
       <c r="E32" t="s">
-        <v>5521</v>
-      </c>
-      <c r="F32" t="s">
-        <v>5522</v>
-      </c>
-      <c r="G32" s="8">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4300</v>
+      </c>
+      <c r="F32">
+        <v>40106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>5539</v>
+        <v>5889</v>
       </c>
       <c r="B33" t="s">
-        <v>5540</v>
+        <v>5895</v>
       </c>
       <c r="C33" t="s">
-        <v>5541</v>
+        <v>2288</v>
       </c>
       <c r="D33" t="s">
-        <v>5542</v>
+        <v>5883</v>
       </c>
       <c r="E33" t="s">
-        <v>2897</v>
-      </c>
-      <c r="F33" t="s">
-        <v>5542</v>
-      </c>
-      <c r="G33" s="8">
-        <v>12.44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5507</v>
+      </c>
+      <c r="F33">
+        <v>4518</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>5543</v>
+        <v>5890</v>
       </c>
       <c r="B34" t="s">
-        <v>5544</v>
+        <v>5896</v>
       </c>
       <c r="C34" t="s">
-        <v>5545</v>
+        <v>2288</v>
       </c>
       <c r="D34" t="s">
-        <v>5546</v>
+        <v>5884</v>
       </c>
       <c r="E34" t="s">
-        <v>5548</v>
-      </c>
-      <c r="F34" t="s">
-        <v>5547</v>
-      </c>
-      <c r="G34" s="8">
-        <v>12.48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5507</v>
+      </c>
+      <c r="F34">
+        <v>4018</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>5669</v>
+        <v>5891</v>
       </c>
       <c r="B35" t="s">
-        <v>5672</v>
+        <v>5897</v>
       </c>
       <c r="C35" t="s">
-        <v>2466</v>
+        <v>2288</v>
       </c>
       <c r="D35" t="s">
-        <v>5670</v>
+        <v>5885</v>
       </c>
       <c r="E35" t="s">
-        <v>5671</v>
-      </c>
-      <c r="F35" t="s">
-        <v>4479</v>
-      </c>
-      <c r="G35" s="8">
-        <v>3.93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4300</v>
+      </c>
+      <c r="F35">
+        <v>4001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>5713</v>
+        <v>5945</v>
       </c>
       <c r="B36" t="s">
-        <v>5714</v>
+        <v>5946</v>
       </c>
       <c r="C36" t="s">
-        <v>5715</v>
+        <v>2288</v>
       </c>
       <c r="D36" t="s">
-        <v>5716</v>
+        <v>5944</v>
       </c>
       <c r="E36" t="s">
-        <v>5717</v>
+        <v>4486</v>
       </c>
       <c r="F36" t="s">
-        <v>5716</v>
-      </c>
-      <c r="G36" s="8">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>5739</v>
-      </c>
-      <c r="B37" t="s">
-        <v>5742</v>
-      </c>
-      <c r="C37" t="s">
-        <v>2288</v>
-      </c>
-      <c r="D37" t="s">
-        <v>5740</v>
-      </c>
-      <c r="E37" t="s">
-        <v>2522</v>
-      </c>
-      <c r="F37" t="s">
-        <v>5741</v>
-      </c>
-      <c r="G37" s="8">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>5747</v>
-      </c>
-      <c r="B38" t="s">
-        <v>5748</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5372</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>5749</v>
-      </c>
-      <c r="E38" t="s">
-        <v>5750</v>
-      </c>
-      <c r="F38" t="s">
-        <v>3369</v>
-      </c>
-      <c r="G38" s="8">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>5938</v>
-      </c>
-      <c r="B39" t="s">
-        <v>5939</v>
-      </c>
-      <c r="C39" t="s">
-        <v>5940</v>
-      </c>
-      <c r="D39" t="s">
-        <v>5941</v>
-      </c>
-      <c r="E39" t="s">
-        <v>4470</v>
-      </c>
-      <c r="F39" t="s">
-        <v>5942</v>
-      </c>
-      <c r="G39" s="8">
-        <v>5.65</v>
+        <v>5943</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add LM1117-1.8V, add a few other parts too
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="9"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15088" uniqueCount="5952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15148" uniqueCount="5985">
   <si>
     <t>Part Number</t>
   </si>
@@ -17887,6 +17887,105 @@
   </si>
   <si>
     <t>PTC Fuse (Polyfuse), 16V 750mA Hold, 1.5A Trip, 200ms</t>
+  </si>
+  <si>
+    <t>ANLG-00054</t>
+  </si>
+  <si>
+    <t>Diff Amp, +/-250V Common Mode Range, LT1990</t>
+  </si>
+  <si>
+    <t>LT1990</t>
+  </si>
+  <si>
+    <t>LT1990CS8</t>
+  </si>
+  <si>
+    <t>IC, 3:8 Decoder/Demux, SOIC-16, 2V-6V</t>
+  </si>
+  <si>
+    <t>SN74HC138DR</t>
+  </si>
+  <si>
+    <t>74HC138</t>
+  </si>
+  <si>
+    <t>CAP-00561</t>
+  </si>
+  <si>
+    <t>C1206C105K1RACTU</t>
+  </si>
+  <si>
+    <t>MAG-00115</t>
+  </si>
+  <si>
+    <t>MAG-00116</t>
+  </si>
+  <si>
+    <t>Ind, 39uH, 15.1A (32.3A sat.), 0.012 Ohm, THT</t>
+  </si>
+  <si>
+    <t>39uH</t>
+  </si>
+  <si>
+    <t>15.1A</t>
+  </si>
+  <si>
+    <t>12mOhm</t>
+  </si>
+  <si>
+    <t>1140-390K-RC</t>
+  </si>
+  <si>
+    <t>BOURNS_1140-390K-RC</t>
+  </si>
+  <si>
+    <t>RES-00708</t>
+  </si>
+  <si>
+    <t>RES SMD 0.005 OHM 1% 3W 2512, Current Sense, 50ppm/°C</t>
+  </si>
+  <si>
+    <t>3W</t>
+  </si>
+  <si>
+    <t>CRE2512-FZ-R005E-3</t>
+  </si>
+  <si>
+    <t>MISC-00039</t>
+  </si>
+  <si>
+    <t>Net Tie</t>
+  </si>
+  <si>
+    <t>net_tie_0</t>
+  </si>
+  <si>
+    <t>ANLG-00055</t>
+  </si>
+  <si>
+    <t>IC, Voltage Reference, 2.5V, 3ppm/°C, REF5020</t>
+  </si>
+  <si>
+    <t>REF5025AIDR</t>
+  </si>
+  <si>
+    <t>REF50xx</t>
+  </si>
+  <si>
+    <t>PWREG-00042</t>
+  </si>
+  <si>
+    <t>REG, Linear, Fixed 1.8V, 800mA, LM1117-1.8, SOT-223</t>
+  </si>
+  <si>
+    <t>LInear</t>
+  </si>
+  <si>
+    <t>LM1117MPX-1.8/NOPB</t>
+  </si>
+  <si>
+    <t>3 - 15V</t>
   </si>
 </sst>
 </file>
@@ -18260,7 +18359,7 @@
   <dimension ref="A1:J839"/>
   <sheetViews>
     <sheetView topLeftCell="A698" workbookViewId="0">
-      <selection activeCell="H710" sqref="H710"/>
+      <selection activeCell="B711" sqref="B711"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38439,8 +38538,36 @@
       </c>
     </row>
     <row r="710" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C710"/>
-      <c r="D710"/>
+      <c r="A710" t="s">
+        <v>5969</v>
+      </c>
+      <c r="B710" t="s">
+        <v>5970</v>
+      </c>
+      <c r="C710">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D710" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="E710" s="12" t="s">
+        <v>5971</v>
+      </c>
+      <c r="F710" t="s">
+        <v>4890</v>
+      </c>
+      <c r="G710" t="s">
+        <v>5972</v>
+      </c>
+      <c r="H710" t="s">
+        <v>2374</v>
+      </c>
+      <c r="I710" t="s">
+        <v>12</v>
+      </c>
+      <c r="J710" s="8">
+        <v>0.81</v>
+      </c>
     </row>
     <row r="711" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C711"/>
@@ -38966,10 +39093,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39852,6 +39979,20 @@
       </c>
       <c r="G40" s="8">
         <v>0.13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>5973</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5974</v>
+      </c>
+      <c r="E41" t="s">
+        <v>5975</v>
+      </c>
+      <c r="F41" t="s">
+        <v>5975</v>
       </c>
     </row>
   </sheetData>
@@ -45564,10 +45705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K562"/>
+  <dimension ref="A1:K563"/>
   <sheetViews>
-    <sheetView topLeftCell="A533" workbookViewId="0">
-      <selection activeCell="I249" sqref="I249"/>
+    <sheetView topLeftCell="A548" workbookViewId="0">
+      <selection activeCell="B564" sqref="B564"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -64157,6 +64298,42 @@
         <v>0.23</v>
       </c>
     </row>
+    <row r="563" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A563" t="s">
+        <v>5959</v>
+      </c>
+      <c r="B563" t="str">
+        <f>CONCATENATE("CAP",", ",C563,", ",D563,", ",E563,", ",F563,", 1206")</f>
+        <v>CAP, 1uF, ±10%, 100V, X7R, 1206</v>
+      </c>
+      <c r="C563" t="s">
+        <v>1577</v>
+      </c>
+      <c r="D563" t="s">
+        <v>4345</v>
+      </c>
+      <c r="E563" t="s">
+        <v>945</v>
+      </c>
+      <c r="F563" t="s">
+        <v>20</v>
+      </c>
+      <c r="G563" t="s">
+        <v>4806</v>
+      </c>
+      <c r="H563" t="s">
+        <v>5960</v>
+      </c>
+      <c r="I563" t="s">
+        <v>1472</v>
+      </c>
+      <c r="J563" t="s">
+        <v>23</v>
+      </c>
+      <c r="K563" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -64165,10 +64342,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N117"/>
+  <dimension ref="A1:N118"/>
   <sheetViews>
-    <sheetView topLeftCell="B94" workbookViewId="0">
-      <selection activeCell="M118" sqref="M118"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68123,6 +68300,9 @@
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>5961</v>
+      </c>
       <c r="B117" t="s">
         <v>5928</v>
       </c>
@@ -68152,6 +68332,41 @@
       </c>
       <c r="M117" s="8">
         <v>2.02</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>5962</v>
+      </c>
+      <c r="B118" t="s">
+        <v>5963</v>
+      </c>
+      <c r="C118" t="s">
+        <v>5964</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>951</v>
+      </c>
+      <c r="E118" t="s">
+        <v>5965</v>
+      </c>
+      <c r="H118" t="s">
+        <v>5966</v>
+      </c>
+      <c r="I118" t="s">
+        <v>4890</v>
+      </c>
+      <c r="J118" t="s">
+        <v>5967</v>
+      </c>
+      <c r="K118" t="s">
+        <v>5968</v>
+      </c>
+      <c r="L118" t="s">
+        <v>1383</v>
+      </c>
+      <c r="M118" s="8">
+        <v>9.56</v>
       </c>
     </row>
   </sheetData>
@@ -68887,10 +69102,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -70440,6 +70655,44 @@
       </c>
       <c r="M43" s="8">
         <v>6.91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>5980</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5981</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5984</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5013</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G44" t="s">
+        <v>5982</v>
+      </c>
+      <c r="H44" t="s">
+        <v>2520</v>
+      </c>
+      <c r="I44" t="s">
+        <v>2288</v>
+      </c>
+      <c r="J44" t="s">
+        <v>5983</v>
+      </c>
+      <c r="K44" t="s">
+        <v>4280</v>
+      </c>
+      <c r="L44" t="s">
+        <v>4767</v>
+      </c>
+      <c r="M44" s="8">
+        <v>1.1399999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -70731,10 +70984,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -71977,6 +72230,52 @@
         <v>1.04</v>
       </c>
     </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>5952</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5953</v>
+      </c>
+      <c r="C56" t="s">
+        <v>4314</v>
+      </c>
+      <c r="D56" t="s">
+        <v>5955</v>
+      </c>
+      <c r="E56" t="s">
+        <v>4470</v>
+      </c>
+      <c r="F56" t="s">
+        <v>5954</v>
+      </c>
+      <c r="G56" s="8">
+        <v>3.26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>5976</v>
+      </c>
+      <c r="B57" t="s">
+        <v>5977</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D57" t="s">
+        <v>5978</v>
+      </c>
+      <c r="E57" t="s">
+        <v>4470</v>
+      </c>
+      <c r="F57" t="s">
+        <v>5979</v>
+      </c>
+      <c r="G57" s="8">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -71985,10 +72284,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:E37"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -72687,7 +72986,7 @@
         <v>40106</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>5889</v>
       </c>
@@ -72707,7 +73006,7 @@
         <v>4518</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5890</v>
       </c>
@@ -72727,7 +73026,7 @@
         <v>4018</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>5891</v>
       </c>
@@ -72747,7 +73046,7 @@
         <v>4001</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>5945</v>
       </c>
@@ -72765,6 +73064,29 @@
       </c>
       <c r="F36" t="s">
         <v>5943</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>5947</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5956</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5957</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5507</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5958</v>
+      </c>
+      <c r="G37" s="8">
+        <v>0.37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add DF13 connector and update 16x1 male header model
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15148" uniqueCount="5985">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15171" uniqueCount="6000">
   <si>
     <t>Part Number</t>
   </si>
@@ -17986,6 +17986,51 @@
   </si>
   <si>
     <t>3 - 15V</t>
+  </si>
+  <si>
+    <t>PWREG-00043</t>
+  </si>
+  <si>
+    <t>8 - 17V</t>
+  </si>
+  <si>
+    <t>4A</t>
+  </si>
+  <si>
+    <t>UCC2721x</t>
+  </si>
+  <si>
+    <t>UCC27211DDAR</t>
+  </si>
+  <si>
+    <t>Gate Driver, 4A, Half-Bridge, 7.2ns Rise, 120V DC Max Bootstrap</t>
+  </si>
+  <si>
+    <t>MISC-00040</t>
+  </si>
+  <si>
+    <t>WURTH_696103201002</t>
+  </si>
+  <si>
+    <t>Fuse Holder, Cartridge, 5x20mm, 250V 20A</t>
+  </si>
+  <si>
+    <t>696103201002</t>
+  </si>
+  <si>
+    <t>DF13-40-1.25mm</t>
+  </si>
+  <si>
+    <t>DF13-4P-1.25DSA</t>
+  </si>
+  <si>
+    <t>Hirose Electric Co Ltd</t>
+  </si>
+  <si>
+    <t>CONN-00067</t>
+  </si>
+  <si>
+    <t>Header, DF13 4-pos 1.25mm Pitch</t>
   </si>
 </sst>
 </file>
@@ -39093,10 +39138,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39993,6 +40038,29 @@
       </c>
       <c r="F41" t="s">
         <v>5975</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>5991</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5993</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2421</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>5994</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5992</v>
+      </c>
+      <c r="F42" t="s">
+        <v>3369</v>
+      </c>
+      <c r="G42" s="8">
+        <v>1.18</v>
       </c>
     </row>
   </sheetData>
@@ -43552,9 +43620,9 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
@@ -45695,6 +45763,41 @@
       </c>
       <c r="K68" s="8">
         <v>1.71</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>5998</v>
+      </c>
+      <c r="B69" t="s">
+        <v>5999</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2397</v>
+      </c>
+      <c r="D69">
+        <v>4</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
+        <v>70</v>
+      </c>
+      <c r="G69" t="s">
+        <v>5997</v>
+      </c>
+      <c r="H69" t="s">
+        <v>5996</v>
+      </c>
+      <c r="I69" t="s">
+        <v>5995</v>
+      </c>
+      <c r="J69" t="s">
+        <v>2957</v>
+      </c>
+      <c r="K69">
+        <v>0.43</v>
       </c>
     </row>
   </sheetData>
@@ -69102,10 +69205,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -70693,6 +70796,38 @@
       </c>
       <c r="M44" s="8">
         <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>5985</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5990</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5986</v>
+      </c>
+      <c r="E45" t="s">
+        <v>5987</v>
+      </c>
+      <c r="G45" t="s">
+        <v>2428</v>
+      </c>
+      <c r="I45" t="s">
+        <v>2288</v>
+      </c>
+      <c r="J45" t="s">
+        <v>5989</v>
+      </c>
+      <c r="K45" t="s">
+        <v>4699</v>
+      </c>
+      <c r="L45" t="s">
+        <v>5988</v>
+      </c>
+      <c r="M45" s="8">
+        <v>3.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify DDR1 SODIMM connector to be less tall, add a few other components
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15171" uniqueCount="6000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15199" uniqueCount="6020">
   <si>
     <t>Part Number</t>
   </si>
@@ -18031,6 +18031,66 @@
   </si>
   <si>
     <t>Header, DF13 4-pos 1.25mm Pitch</t>
+  </si>
+  <si>
+    <t>DIO-00059</t>
+  </si>
+  <si>
+    <t>56.7V</t>
+  </si>
+  <si>
+    <t>4.9A</t>
+  </si>
+  <si>
+    <t>SMAJ51A</t>
+  </si>
+  <si>
+    <t>TVS, 51V, 4.9A 400W, Unidirectional, DO-214AC</t>
+  </si>
+  <si>
+    <t>MISC-00041</t>
+  </si>
+  <si>
+    <t>LCD_DISPLAY_0</t>
+  </si>
+  <si>
+    <t>NHD-0216XZ-FSW-GBW</t>
+  </si>
+  <si>
+    <t>Newhaven Display</t>
+  </si>
+  <si>
+    <t>LCD Display, 16-pin interface, 80x36mm, Hitachi standard driver</t>
+  </si>
+  <si>
+    <t>MISC-00042</t>
+  </si>
+  <si>
+    <t>B3FS-1012P</t>
+  </si>
+  <si>
+    <t>B3FS-1000</t>
+  </si>
+  <si>
+    <t>SW_1P1T_2</t>
+  </si>
+  <si>
+    <t>Switch, SPST-NO, Tactile, 6.3x6.0mm, SMD, 50mA 24VDC</t>
+  </si>
+  <si>
+    <t>PEC11R-4020F-S0024</t>
+  </si>
+  <si>
+    <t>BOURNS_PEC11R</t>
+  </si>
+  <si>
+    <t>rotary_encoder_0</t>
+  </si>
+  <si>
+    <t>Rotary Encoder, Mechanical, 24PPR, THT</t>
+  </si>
+  <si>
+    <t>MISC-00043</t>
   </si>
 </sst>
 </file>
@@ -39138,10 +39198,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40061,6 +40121,75 @@
       </c>
       <c r="G42" s="8">
         <v>1.18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>6005</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6009</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6008</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6007</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6006</v>
+      </c>
+      <c r="F43" t="s">
+        <v>6006</v>
+      </c>
+      <c r="G43" s="8">
+        <v>11.63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>6010</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6014</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4623</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6011</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6012</v>
+      </c>
+      <c r="F44" t="s">
+        <v>6013</v>
+      </c>
+      <c r="G44" s="8">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>6019</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6018</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4890</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6015</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6016</v>
+      </c>
+      <c r="F45" t="s">
+        <v>6017</v>
+      </c>
+      <c r="G45" s="8">
+        <v>1.68</v>
       </c>
     </row>
   </sheetData>
@@ -41490,16 +41619,16 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M60"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="2" customWidth="1"/>
@@ -43611,6 +43740,41 @@
         <v>0.74</v>
       </c>
     </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>6000</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>6004</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>6001</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>2947</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>6002</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>2944</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>4553</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>6003</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>2127</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>2130</v>
+      </c>
+      <c r="M61" s="8">
+        <v>0.4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43622,8 +43786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add double decker USB A
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="2" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15199" uniqueCount="6020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15207" uniqueCount="6025">
   <si>
     <t>Part Number</t>
   </si>
@@ -18091,6 +18091,21 @@
   </si>
   <si>
     <t>MISC-00043</t>
+  </si>
+  <si>
+    <t>CONN-00068</t>
+  </si>
+  <si>
+    <t>USB-A Jack x2, USB 2.0, Right-Angle, Thru-Hole</t>
+  </si>
+  <si>
+    <t>UJ2-ADH-1-TH</t>
+  </si>
+  <si>
+    <t>CUI_UJ2-ADH-1-TH</t>
+  </si>
+  <si>
+    <t>usb_a_x2</t>
   </si>
 </sst>
 </file>
@@ -39200,8 +39215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43784,10 +43799,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45960,8 +45975,43 @@
       <c r="J69" t="s">
         <v>2957</v>
       </c>
-      <c r="K69">
+      <c r="K69" s="8">
         <v>0.43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>6020</v>
+      </c>
+      <c r="B70" t="s">
+        <v>6021</v>
+      </c>
+      <c r="C70" t="s">
+        <v>5803</v>
+      </c>
+      <c r="D70">
+        <v>4</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70" t="s">
+        <v>70</v>
+      </c>
+      <c r="G70" t="s">
+        <v>4589</v>
+      </c>
+      <c r="H70" t="s">
+        <v>6022</v>
+      </c>
+      <c r="I70" t="s">
+        <v>6023</v>
+      </c>
+      <c r="J70" t="s">
+        <v>6024</v>
+      </c>
+      <c r="K70" s="8">
+        <v>0.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add vertical USB A and Ethernet Mag-jack
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="2" activeTab="12"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15207" uniqueCount="6025">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15234" uniqueCount="6043">
   <si>
     <t>Part Number</t>
   </si>
@@ -18106,6 +18106,60 @@
   </si>
   <si>
     <t>usb_a_x2</t>
+  </si>
+  <si>
+    <t>ANLG-00056</t>
+  </si>
+  <si>
+    <t>ADC, 24-bit, 4-channel, Sigma-Delta, 31.25k SPS, TSSOP-24</t>
+  </si>
+  <si>
+    <t>TSSOP-24_0</t>
+  </si>
+  <si>
+    <t>AD7172</t>
+  </si>
+  <si>
+    <t>AD7172-2BRUZ-RL7</t>
+  </si>
+  <si>
+    <t>UCTRL-00010</t>
+  </si>
+  <si>
+    <t>STM32F334R8</t>
+  </si>
+  <si>
+    <t>STM32F334R8T7</t>
+  </si>
+  <si>
+    <t>STM32F334 ARM Cortex-M4, LQFP-64</t>
+  </si>
+  <si>
+    <t>CONN-00069</t>
+  </si>
+  <si>
+    <t>USB-A Jack, USB 2.0, Vertical, THT</t>
+  </si>
+  <si>
+    <t>1050570001</t>
+  </si>
+  <si>
+    <t>MOLEX_1050570001</t>
+  </si>
+  <si>
+    <t>ABRACON_ARJ11G-MB</t>
+  </si>
+  <si>
+    <t>CONN-00070</t>
+  </si>
+  <si>
+    <t>RJ45 Modular Mag-Jack, 8P8C, 10/100 Base-T, Vertical</t>
+  </si>
+  <si>
+    <t>ARJ11G-MBSE-MU2</t>
+  </si>
+  <si>
+    <t>abracon-ARJ11G-MBSE</t>
   </si>
 </sst>
 </file>
@@ -43799,10 +43853,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+      <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -46012,6 +46066,73 @@
       </c>
       <c r="K70" s="8">
         <v>0.95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>6034</v>
+      </c>
+      <c r="B71" t="s">
+        <v>6035</v>
+      </c>
+      <c r="C71" t="s">
+        <v>5803</v>
+      </c>
+      <c r="D71">
+        <v>4</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>2333</v>
+      </c>
+      <c r="G71" t="s">
+        <v>2389</v>
+      </c>
+      <c r="H71" s="11" t="s">
+        <v>6036</v>
+      </c>
+      <c r="I71" t="s">
+        <v>6037</v>
+      </c>
+      <c r="J71" t="s">
+        <v>5812</v>
+      </c>
+      <c r="K71" s="8">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>6039</v>
+      </c>
+      <c r="B72" t="s">
+        <v>6040</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5803</v>
+      </c>
+      <c r="D72">
+        <v>8</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="G72" t="s">
+        <v>2918</v>
+      </c>
+      <c r="H72" t="s">
+        <v>6041</v>
+      </c>
+      <c r="I72" t="s">
+        <v>6038</v>
+      </c>
+      <c r="J72" t="s">
+        <v>6042</v>
+      </c>
+      <c r="K72" s="8">
+        <v>5.26</v>
       </c>
     </row>
   </sheetData>
@@ -68694,10 +68815,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68916,6 +69037,26 @@
       </c>
       <c r="F11" t="s">
         <v>5510</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>6030</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6033</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6032</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6031</v>
       </c>
     </row>
   </sheetData>
@@ -71333,10 +71474,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -72623,6 +72764,29 @@
       </c>
       <c r="G57" s="8">
         <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>6025</v>
+      </c>
+      <c r="B58" t="s">
+        <v>6026</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4314</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6029</v>
+      </c>
+      <c r="E58" t="s">
+        <v>6027</v>
+      </c>
+      <c r="F58" t="s">
+        <v>6028</v>
+      </c>
+      <c r="G58" s="8">
+        <v>14.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add samtec SMD 5x2 header and other stuff
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15234" uniqueCount="6043">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15277" uniqueCount="6064">
   <si>
     <t>Part Number</t>
   </si>
@@ -18160,6 +18160,69 @@
   </si>
   <si>
     <t>abracon-ARJ11G-MBSE</t>
+  </si>
+  <si>
+    <t>PWREG-00044</t>
+  </si>
+  <si>
+    <t>Gate Driver, Isolated, Dual-Channel, 4A/6A Source/Sink, 5ns Rise-Time</t>
+  </si>
+  <si>
+    <t>UCC21540ADWK</t>
+  </si>
+  <si>
+    <t>SOW-14-DWK</t>
+  </si>
+  <si>
+    <t>UCC21540</t>
+  </si>
+  <si>
+    <t>DIO-00060</t>
+  </si>
+  <si>
+    <t>Dio, Silicon, 200mA, 1V, 100V, SOD-123</t>
+  </si>
+  <si>
+    <t>1.0V</t>
+  </si>
+  <si>
+    <t>SMMSD4148T3G</t>
+  </si>
+  <si>
+    <t>DIO-00061</t>
+  </si>
+  <si>
+    <t>1.65V</t>
+  </si>
+  <si>
+    <t>STTH112A</t>
+  </si>
+  <si>
+    <t>Dio, Silicon, 1A, 1.65V, 1.2kV, High Voltage, 75ns RR-time, DO-214AC</t>
+  </si>
+  <si>
+    <t>RES-00709</t>
+  </si>
+  <si>
+    <t>VARRES, 10K, 20% 250mW, SMD</t>
+  </si>
+  <si>
+    <t>PVG3A103C01R00</t>
+  </si>
+  <si>
+    <t>BOURNS_PVG3A103C01R00</t>
+  </si>
+  <si>
+    <t>CONN-00071</t>
+  </si>
+  <si>
+    <t>TSM-105-01-L-DV-P</t>
+  </si>
+  <si>
+    <t>SAMTEC_SMD_HDDR_5x2</t>
+  </si>
+  <si>
+    <t>Header, 5x2, 0.1", SMD</t>
   </si>
 </sst>
 </file>
@@ -18532,8 +18595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J839"/>
   <sheetViews>
-    <sheetView topLeftCell="A698" workbookViewId="0">
-      <selection activeCell="B711" sqref="B711"/>
+    <sheetView topLeftCell="A696" workbookViewId="0">
+      <selection activeCell="A712" sqref="A712"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38744,8 +38807,36 @@
       </c>
     </row>
     <row r="711" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C711"/>
-      <c r="D711"/>
+      <c r="A711" t="s">
+        <v>6056</v>
+      </c>
+      <c r="B711" t="s">
+        <v>6057</v>
+      </c>
+      <c r="C711" t="s">
+        <v>901</v>
+      </c>
+      <c r="D711" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="E711" s="12" t="s">
+        <v>5252</v>
+      </c>
+      <c r="F711" t="s">
+        <v>4890</v>
+      </c>
+      <c r="G711" t="s">
+        <v>6058</v>
+      </c>
+      <c r="H711" t="s">
+        <v>6059</v>
+      </c>
+      <c r="I711" t="s">
+        <v>2344</v>
+      </c>
+      <c r="J711" s="8">
+        <v>1.57</v>
+      </c>
     </row>
     <row r="712" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C712"/>
@@ -41688,10 +41779,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43844,6 +43935,76 @@
         <v>0.4</v>
       </c>
     </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>6049</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>6050</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>945</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>2954</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>4854</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>2092</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>6051</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>2105</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>4856</v>
+      </c>
+      <c r="M62" s="8">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>6052</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>6055</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>6053</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>5012</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>4854</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>6054</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>2127</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>4856</v>
+      </c>
+      <c r="M63" s="8">
+        <v>0.42</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43853,10 +44014,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -46133,6 +46294,38 @@
       </c>
       <c r="K72" s="8">
         <v>5.26</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>6060</v>
+      </c>
+      <c r="B73" t="s">
+        <v>6063</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2397</v>
+      </c>
+      <c r="D73">
+        <v>5</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+      <c r="G73" t="s">
+        <v>4738</v>
+      </c>
+      <c r="H73" t="s">
+        <v>6061</v>
+      </c>
+      <c r="I73" t="s">
+        <v>6062</v>
+      </c>
+      <c r="J73" t="s">
+        <v>5758</v>
+      </c>
+      <c r="K73" s="8">
+        <v>1.17</v>
       </c>
     </row>
   </sheetData>
@@ -69560,10 +69753,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -71183,6 +71376,35 @@
       </c>
       <c r="M45" s="8">
         <v>3.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>6043</v>
+      </c>
+      <c r="B46" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E46" t="s">
+        <v>4312</v>
+      </c>
+      <c r="G46" t="s">
+        <v>2428</v>
+      </c>
+      <c r="I46" t="s">
+        <v>2288</v>
+      </c>
+      <c r="J46" t="s">
+        <v>6045</v>
+      </c>
+      <c r="K46" t="s">
+        <v>6046</v>
+      </c>
+      <c r="L46" t="s">
+        <v>6047</v>
+      </c>
+      <c r="M46" s="8">
+        <v>6.37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More early April updates
</commit_message>
<xml_diff>
--- a/Library/Components/DB.xlsx
+++ b/Library/Components/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15555" uniqueCount="6204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15561" uniqueCount="6209">
   <si>
     <t>Part Number</t>
   </si>
@@ -18643,6 +18643,21 @@
   </si>
   <si>
     <t>Module, AC-DC Isolated, 5V 3A, MEAN WELL</t>
+  </si>
+  <si>
+    <t>ANLG-00059</t>
+  </si>
+  <si>
+    <t>ADC, 24-bit, 8-channel MUX-PGA, Sigma-Delta, 30k SPS, SSOP-28</t>
+  </si>
+  <si>
+    <t>ADS1256IDBR</t>
+  </si>
+  <si>
+    <t>SSOP-28_0</t>
+  </si>
+  <si>
+    <t>ADS1256</t>
   </si>
 </sst>
 </file>
@@ -70980,7 +70995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
@@ -73064,10 +73079,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -74423,6 +74438,29 @@
       </c>
       <c r="G60" s="8">
         <v>0.64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>6204</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6205</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6206</v>
+      </c>
+      <c r="E61" t="s">
+        <v>6207</v>
+      </c>
+      <c r="F61" t="s">
+        <v>6208</v>
+      </c>
+      <c r="G61" s="8">
+        <v>14.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>